<commit_message>
Rw Usage Updates S.1.0.0.9 _4:00PM
Rw Usage Updates S.1.0.0.9 _4:00PM
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.9.xlsx
+++ b/Usage_S_1.0.9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD2728B-5706-424E-9F16-74C52085627C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45124EE5-64D5-40D4-ABF1-4FC7FC5D17FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2264" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2291" uniqueCount="262">
   <si>
     <t>UnSettled</t>
   </si>
@@ -792,6 +792,36 @@
   </si>
   <si>
     <t>Vendor Tdy</t>
+  </si>
+  <si>
+    <t>X-FuelW(20)  - X</t>
+  </si>
+  <si>
+    <t>X-VillageW(Kudiary) - X</t>
+  </si>
+  <si>
+    <t>X-VillageW(HarirajPur) - X</t>
+  </si>
+  <si>
+    <t>X-FishMP(2)-X</t>
+  </si>
+  <si>
+    <t>X-MarketW(2) - X</t>
+  </si>
+  <si>
+    <t>X-Kudiary  X</t>
+  </si>
+  <si>
+    <t>X-Harirajpur  X</t>
+  </si>
+  <si>
+    <t>HAF</t>
+  </si>
+  <si>
+    <t>zError-Blockade</t>
+  </si>
+  <si>
+    <t>RPF</t>
   </si>
 </sst>
 </file>
@@ -990,7 +1020,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1096,6 +1126,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1722,7 +1758,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="307">
+  <cellXfs count="314">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2397,6 +2433,45 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2421,61 +2496,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2489,14 +2522,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2788,7 +2839,7 @@
   <dimension ref="A1:AI20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH15" sqref="AH15"/>
+      <selection activeCell="AI12" sqref="AI12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2818,7 +2869,8 @@
     <col min="25" max="25" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="3.85546875" customWidth="1"/>
-    <col min="29" max="30" width="5.28515625" customWidth="1"/>
+    <col min="29" max="29" width="5.28515625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="5.28515625" customWidth="1"/>
     <col min="31" max="31" width="1" customWidth="1"/>
     <col min="32" max="32" width="9.5703125" customWidth="1"/>
   </cols>
@@ -2920,9 +2972,9 @@
         <f>SUM(AB3:AB17)</f>
         <v>20</v>
       </c>
-      <c r="AC2" s="8">
+      <c r="AC2" s="34">
         <f>SUM(AC3:AC17)</f>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="AD2" s="8">
         <f>SUM(AD3:AD17)</f>
@@ -2960,7 +3012,7 @@
         <v>1</v>
       </c>
       <c r="AB3" s="251"/>
-      <c r="AC3" s="43">
+      <c r="AC3" s="59">
         <v>4</v>
       </c>
       <c r="AD3" s="44"/>
@@ -3015,7 +3067,7 @@
       <c r="S4" s="154">
         <v>0.4861111111111111</v>
       </c>
-      <c r="T4" s="240">
+      <c r="T4" s="313">
         <v>1</v>
       </c>
       <c r="U4" s="245">
@@ -3027,8 +3079,9 @@
       <c r="Z4" s="169" t="s">
         <v>220</v>
       </c>
-      <c r="AB4" s="25"/>
-      <c r="AC4">
+      <c r="AA4" s="307"/>
+      <c r="AB4" s="308"/>
+      <c r="AC4" s="311">
         <v>4</v>
       </c>
       <c r="AD4" s="240">
@@ -3041,7 +3094,7 @@
       <c r="AG4" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="AH4" s="1" t="s">
+      <c r="AH4" s="24" t="s">
         <v>249</v>
       </c>
     </row>
@@ -3093,8 +3146,9 @@
       <c r="Z5" s="215" t="s">
         <v>219</v>
       </c>
-      <c r="AB5" s="25"/>
-      <c r="AC5">
+      <c r="AA5" s="307"/>
+      <c r="AB5" s="308"/>
+      <c r="AC5" s="311">
         <v>4</v>
       </c>
       <c r="AD5" s="240">
@@ -3107,16 +3161,16 @@
       <c r="AG5" s="25" t="s">
         <v>247</v>
       </c>
-      <c r="AH5" s="1" t="s">
+      <c r="AH5" s="24" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
-        <v>2932</v>
+        <v>3192</v>
       </c>
       <c r="C6">
-        <v>6033</v>
+        <v>5773</v>
       </c>
       <c r="E6" s="218"/>
       <c r="F6" s="207"/>
@@ -3167,10 +3221,11 @@
       <c r="AB6" s="26">
         <v>1</v>
       </c>
+      <c r="AC6" s="311"/>
       <c r="AD6" s="49"/>
       <c r="AE6" s="268"/>
       <c r="AF6" s="25"/>
-      <c r="AH6" s="1"/>
+      <c r="AH6" s="24"/>
     </row>
     <row r="7" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
@@ -3180,8 +3235,12 @@
         <v>0</v>
       </c>
       <c r="E7" s="165"/>
-      <c r="F7" s="242"/>
-      <c r="G7" s="177"/>
+      <c r="F7" s="242">
+        <v>15</v>
+      </c>
+      <c r="G7" s="177">
+        <v>15</v>
+      </c>
       <c r="H7" s="9" t="s">
         <v>188</v>
       </c>
@@ -3191,7 +3250,9 @@
       <c r="J7" s="83" t="s">
         <v>105</v>
       </c>
-      <c r="K7" s="215"/>
+      <c r="K7" s="169" t="s">
+        <v>254</v>
+      </c>
       <c r="L7" s="83" t="s">
         <v>139</v>
       </c>
@@ -3208,10 +3269,13 @@
         <v>95</v>
       </c>
       <c r="Q7" s="154">
-        <v>0.88611111111111107</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="S7" s="154">
-        <v>0.88611111111111107</v>
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="T7" s="310">
+        <v>1</v>
       </c>
       <c r="U7" s="245">
         <v>45292</v>
@@ -3228,7 +3292,7 @@
       <c r="AB7" s="26">
         <v>6</v>
       </c>
-      <c r="AC7">
+      <c r="AC7" s="311">
         <v>4</v>
       </c>
       <c r="AD7" s="49"/>
@@ -3237,7 +3301,7 @@
       <c r="AG7" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AH7" s="1" t="s">
+      <c r="AH7" s="24" t="s">
         <v>249</v>
       </c>
     </row>
@@ -3290,17 +3354,20 @@
       <c r="Z8" s="169" t="s">
         <v>228</v>
       </c>
-      <c r="AA8" s="25"/>
+      <c r="AA8" s="308"/>
       <c r="AB8" s="26">
         <v>4</v>
       </c>
-      <c r="AC8">
+      <c r="AC8" s="311">
         <v>4</v>
       </c>
       <c r="AD8" s="49"/>
       <c r="AE8" s="268"/>
       <c r="AF8" s="25"/>
-      <c r="AH8" s="24"/>
+      <c r="AG8" s="25"/>
+      <c r="AH8" s="24" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="9" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
@@ -3308,10 +3375,12 @@
       </c>
       <c r="B9" s="8">
         <f>7000+B6+B5-C2</f>
-        <v>9932</v>
+        <v>10192</v>
       </c>
       <c r="E9" s="163"/>
-      <c r="F9" s="165"/>
+      <c r="F9" s="165">
+        <v>14</v>
+      </c>
       <c r="G9" s="177"/>
       <c r="H9" s="9" t="s">
         <v>71</v>
@@ -3323,7 +3392,7 @@
         <v>165</v>
       </c>
       <c r="K9" s="169" t="s">
-        <v>215</v>
+        <v>252</v>
       </c>
       <c r="L9" s="223" t="s">
         <v>163</v>
@@ -3341,25 +3410,32 @@
         <v>30</v>
       </c>
       <c r="Q9" s="154">
-        <v>0.57638888888888895</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="S9" s="154">
-        <v>0.57638888888888895</v>
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="T9" s="238">
+        <v>3</v>
       </c>
       <c r="U9" s="245">
-        <v>45292</v>
+        <v>45293</v>
+      </c>
+      <c r="Y9" s="25" t="s">
+        <v>260</v>
       </c>
       <c r="Z9" s="169" t="s">
         <v>229</v>
       </c>
-      <c r="AA9" s="25"/>
+      <c r="AA9" s="308"/>
       <c r="AB9" s="26">
         <v>1</v>
       </c>
+      <c r="AC9" s="311"/>
       <c r="AD9" s="49"/>
       <c r="AE9" s="268"/>
       <c r="AF9" s="25"/>
-      <c r="AH9" s="1"/>
+      <c r="AH9" s="24"/>
     </row>
     <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="220"/>
@@ -3399,12 +3475,17 @@
       <c r="U10" s="245">
         <v>45292</v>
       </c>
+      <c r="Y10" s="25" t="s">
+        <v>259</v>
+      </c>
       <c r="Z10" s="169" t="s">
         <v>232</v>
       </c>
+      <c r="AA10" s="307"/>
       <c r="AB10" s="26">
         <v>1</v>
       </c>
+      <c r="AC10" s="311"/>
       <c r="AD10" s="49">
         <v>1</v>
       </c>
@@ -3415,7 +3496,7 @@
       <c r="AG10" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="AH10" s="1">
+      <c r="AH10" s="24">
         <v>1</v>
       </c>
     </row>
@@ -3430,7 +3511,9 @@
       <c r="E11" s="221">
         <v>10</v>
       </c>
-      <c r="F11" s="242"/>
+      <c r="F11" s="242">
+        <v>5</v>
+      </c>
       <c r="G11" s="37"/>
       <c r="H11" s="9" t="s">
         <v>102</v>
@@ -3474,28 +3557,36 @@
       <c r="U11" s="245">
         <v>45293</v>
       </c>
+      <c r="Y11" s="25" t="s">
+        <v>259</v>
+      </c>
       <c r="Z11" s="169" t="s">
         <v>233</v>
       </c>
+      <c r="AA11" s="307"/>
       <c r="AB11" s="26">
         <v>2</v>
       </c>
-      <c r="AC11">
+      <c r="AC11" s="311">
         <v>5</v>
       </c>
       <c r="AD11" s="49"/>
       <c r="AE11" s="268"/>
-      <c r="AF11" s="25"/>
+      <c r="AF11" s="25" t="s">
+        <v>261</v>
+      </c>
       <c r="AG11" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="AH11" s="1">
-        <v>1</v>
+      <c r="AH11" s="24" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E12" s="165"/>
-      <c r="F12" s="205"/>
+      <c r="F12" s="205">
+        <v>200</v>
+      </c>
       <c r="G12" s="164"/>
       <c r="H12" s="28" t="s">
         <v>128</v>
@@ -3504,7 +3595,9 @@
         <v>17</v>
       </c>
       <c r="J12" s="213"/>
-      <c r="K12" s="169"/>
+      <c r="K12" s="169" t="s">
+        <v>253</v>
+      </c>
       <c r="L12" s="224" t="s">
         <v>123</v>
       </c>
@@ -3521,32 +3614,42 @@
         <v>181</v>
       </c>
       <c r="Q12" s="154">
-        <v>0.88611111111111107</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="R12" s="24"/>
       <c r="S12" s="154">
-        <v>0.88611111111111107</v>
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="T12" s="238">
+        <v>3</v>
       </c>
       <c r="U12" s="245">
         <v>45292</v>
       </c>
+      <c r="Y12" s="25" t="s">
+        <v>245</v>
+      </c>
       <c r="Z12" s="169" t="s">
         <v>234</v>
       </c>
+      <c r="AA12" s="307"/>
       <c r="AB12" s="26">
         <v>1</v>
       </c>
+      <c r="AC12" s="312">
+        <v>1</v>
+      </c>
       <c r="AD12" s="49">
         <v>1</v>
       </c>
       <c r="AE12" s="268"/>
       <c r="AF12" s="25" t="s">
-        <v>243</v>
+        <v>65</v>
       </c>
       <c r="AG12" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="AH12" s="1">
+      <c r="AH12" s="24">
         <v>1</v>
       </c>
     </row>
@@ -3556,10 +3659,12 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>9932</v>
+        <v>10192</v>
       </c>
       <c r="E13" s="36"/>
-      <c r="F13" s="206"/>
+      <c r="F13" s="206">
+        <v>1</v>
+      </c>
       <c r="G13" s="246"/>
       <c r="H13" s="9" t="s">
         <v>189</v>
@@ -3570,7 +3675,9 @@
       <c r="J13" s="228" t="s">
         <v>186</v>
       </c>
-      <c r="K13" s="194"/>
+      <c r="K13" s="194" t="s">
+        <v>255</v>
+      </c>
       <c r="L13" s="183" t="s">
         <v>155</v>
       </c>
@@ -3587,14 +3694,14 @@
         <v>90</v>
       </c>
       <c r="Q13" s="154">
-        <v>0.88611111111111107</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="R13"/>
       <c r="S13" s="154">
         <v>0.88611111111111107</v>
       </c>
       <c r="U13" s="245">
-        <v>45292</v>
+        <v>45293</v>
       </c>
       <c r="Y13" s="25" t="s">
         <v>245</v>
@@ -3602,20 +3709,24 @@
       <c r="Z13" s="169" t="s">
         <v>235</v>
       </c>
+      <c r="AA13" s="307"/>
       <c r="AB13" s="26">
         <v>2</v>
       </c>
+      <c r="AC13" s="311"/>
       <c r="AD13" s="49"/>
       <c r="AE13" s="268"/>
       <c r="AF13" s="25"/>
       <c r="AG13" s="25"/>
-      <c r="AH13" s="1"/>
+      <c r="AH13" s="24"/>
     </row>
     <row r="14" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
       <c r="E14" s="165"/>
-      <c r="F14" s="205"/>
+      <c r="F14" s="205">
+        <v>10</v>
+      </c>
       <c r="G14" s="184"/>
       <c r="H14" s="9" t="s">
         <v>9</v>
@@ -3624,32 +3735,48 @@
         <v>17</v>
       </c>
       <c r="J14" s="213"/>
-      <c r="K14" s="169"/>
+      <c r="K14" s="169" t="s">
+        <v>256</v>
+      </c>
       <c r="L14" s="83" t="s">
         <v>124</v>
       </c>
-      <c r="M14" s="224"/>
+      <c r="M14" s="224" t="s">
+        <v>62</v>
+      </c>
       <c r="N14" s="143" t="s">
         <v>200</v>
       </c>
-      <c r="O14" s="169"/>
+      <c r="O14" s="169" t="s">
+        <v>47</v>
+      </c>
       <c r="P14" s="37" t="s">
         <v>29</v>
       </c>
       <c r="Q14" s="154">
-        <v>0.57638888888888895</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="R14"/>
       <c r="S14" s="154">
         <v>0.91666666666666663</v>
       </c>
+      <c r="T14" s="313">
+        <v>2</v>
+      </c>
       <c r="U14" s="245">
-        <v>45292</v>
+        <v>45293</v>
+      </c>
+      <c r="Y14" s="25" t="s">
+        <v>259</v>
       </c>
       <c r="Z14" s="169" t="s">
         <v>237</v>
       </c>
       <c r="AA14" s="239">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="307"/>
+      <c r="AC14" s="241">
         <v>1</v>
       </c>
       <c r="AD14" s="49">
@@ -3662,7 +3789,7 @@
       <c r="AG14" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="AH14" s="1" t="s">
+      <c r="AH14" s="24" t="s">
         <v>249</v>
       </c>
     </row>
@@ -3704,17 +3831,26 @@
       <c r="U15" s="245">
         <v>45292</v>
       </c>
+      <c r="Y15" s="25" t="s">
+        <v>259</v>
+      </c>
       <c r="Z15" s="169" t="s">
         <v>238</v>
       </c>
-      <c r="AB15" s="25"/>
-      <c r="AC15">
+      <c r="AA15" s="307"/>
+      <c r="AB15" s="308"/>
+      <c r="AC15" s="311">
         <v>1</v>
       </c>
       <c r="AD15" s="49"/>
       <c r="AE15" s="268"/>
       <c r="AF15" s="25"/>
-      <c r="AH15" s="1"/>
+      <c r="AG15" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH15" s="24" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="16" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="25"/>
@@ -3729,13 +3865,15 @@
       <c r="Z16" s="169" t="s">
         <v>239</v>
       </c>
-      <c r="AC16">
+      <c r="AA16" s="307"/>
+      <c r="AB16" s="307"/>
+      <c r="AC16" s="311">
         <v>4</v>
       </c>
       <c r="AD16" s="49"/>
       <c r="AE16" s="268"/>
       <c r="AF16" s="25"/>
-      <c r="AH16" s="1"/>
+      <c r="AH16" s="24"/>
     </row>
     <row r="17" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="25"/>
@@ -3747,7 +3885,7 @@
       <c r="G17" s="189"/>
       <c r="H17" s="9">
         <f>SUM(E4:G15)</f>
-        <v>45</v>
+        <v>305</v>
       </c>
       <c r="I17" s="26"/>
       <c r="J17" s="119"/>
@@ -3765,16 +3903,16 @@
       <c r="AB17" s="26">
         <v>2</v>
       </c>
-      <c r="AC17" s="50"/>
+      <c r="AC17" s="65"/>
       <c r="AD17" s="51"/>
-      <c r="AE17" s="269"/>
+      <c r="AE17" s="268"/>
       <c r="AF17" s="25" t="s">
         <v>65</v>
       </c>
       <c r="AG17" s="25" t="s">
         <v>248</v>
       </c>
-      <c r="AH17" s="1" t="s">
+      <c r="AH17" s="24" t="s">
         <v>249</v>
       </c>
     </row>
@@ -3796,11 +3934,59 @@
       <c r="M18" s="255"/>
       <c r="Q18" s="256"/>
       <c r="R18" s="257"/>
+      <c r="Y18" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="Z18" s="169" t="s">
+        <v>257</v>
+      </c>
+      <c r="AA18" s="307"/>
+      <c r="AB18" s="307"/>
+      <c r="AC18" s="311">
+        <v>4</v>
+      </c>
+      <c r="AD18" s="49">
+        <v>2</v>
+      </c>
+      <c r="AE18" s="268"/>
+      <c r="AF18" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG18" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH18" s="24" t="s">
+        <v>249</v>
+      </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I19" s="226"/>
       <c r="L19" s="119"/>
       <c r="M19" s="255"/>
+      <c r="Y19" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="Z19" s="169" t="s">
+        <v>258</v>
+      </c>
+      <c r="AA19" s="50"/>
+      <c r="AB19" s="50"/>
+      <c r="AC19" s="65">
+        <v>4</v>
+      </c>
+      <c r="AD19" s="51">
+        <v>2</v>
+      </c>
+      <c r="AE19" s="269"/>
+      <c r="AF19" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="AG19" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH19" s="24" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="20" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I20" s="227"/>
@@ -3816,8 +4002,8 @@
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="AE3:AE17"/>
     <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AE3:AE19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3826,10 +4012,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:T57"/>
+  <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3842,7 +4028,7 @@
     <col min="10" max="10" width="4.140625" customWidth="1"/>
     <col min="11" max="11" width="7.140625" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3853,18 +4039,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="272" t="s">
+      <c r="E1" s="285" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="274"/>
+      <c r="F1" s="287"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="272" t="s">
+      <c r="H1" s="285" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="273"/>
-      <c r="J1" s="274"/>
+      <c r="I1" s="286"/>
+      <c r="J1" s="287"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -3882,7 +4068,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="275">
+      <c r="B2" s="288">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -3909,26 +4095,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="278">
+      <c r="K2" s="291">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="293">
+      <c r="L2" s="283">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="283">
+      <c r="M2" s="273">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J57)</f>
-        <v>9892</v>
+        <f>SUM(E2:J58)</f>
+        <v>10152</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="276"/>
+      <c r="B3" s="289"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -3943,13 +4129,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="279"/>
-      <c r="L3" s="294"/>
-      <c r="M3" s="284"/>
+      <c r="K3" s="292"/>
+      <c r="L3" s="284"/>
+      <c r="M3" s="274"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="277"/>
+      <c r="B4" s="290"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -3964,9 +4150,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="279"/>
-      <c r="L4" s="294"/>
-      <c r="M4" s="284"/>
+      <c r="K4" s="292"/>
+      <c r="L4" s="284"/>
+      <c r="M4" s="274"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -4048,7 +4234,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="285">
+      <c r="B7" s="275">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -4065,22 +4251,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="287">
+      <c r="K7" s="277">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="289">
+      <c r="L7" s="279">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="291">
+      <c r="M7" s="281">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="286"/>
+      <c r="B8" s="276"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -4101,9 +4287,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="288"/>
-      <c r="L8" s="290"/>
-      <c r="M8" s="292"/>
+      <c r="K8" s="278"/>
+      <c r="L8" s="280"/>
+      <c r="M8" s="282"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -4183,7 +4369,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="285">
+      <c r="B11" s="275">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -4210,7 +4396,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="286"/>
+      <c r="B12" s="276"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -4267,7 +4453,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="285">
+      <c r="B14" s="275">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -4290,7 +4476,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="286"/>
+      <c r="B15" s="276"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -4314,7 +4500,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="275">
+      <c r="B16" s="288">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -4345,7 +4531,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="276"/>
+      <c r="B17" s="289"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -4363,7 +4549,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="275">
+      <c r="B18" s="288">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -4392,7 +4578,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="277"/>
+      <c r="B19" s="290"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -4452,7 +4638,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="281">
+      <c r="B21" s="293">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -4480,7 +4666,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="282"/>
+      <c r="B22" s="294"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -4620,7 +4806,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="280"/>
+      <c r="B27" s="272"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -4951,7 +5137,7 @@
       <c r="A40" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="280"/>
+      <c r="B40" s="272"/>
       <c r="C40" s="96"/>
       <c r="D40" s="82">
         <v>210</v>
@@ -5006,7 +5192,7 @@
       <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="280"/>
+      <c r="B42" s="272"/>
       <c r="C42" s="142"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -5126,7 +5312,7 @@
       <c r="M46" s="18"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="280"/>
+      <c r="B47" s="272"/>
       <c r="C47" s="211"/>
       <c r="D47" s="132"/>
       <c r="E47" s="132"/>
@@ -5167,7 +5353,7 @@
       <c r="M48" s="18"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="280"/>
+      <c r="B49" s="272"/>
       <c r="C49" s="142"/>
       <c r="D49" s="18">
         <v>175</v>
@@ -5193,7 +5379,7 @@
       <c r="M49" s="18"/>
     </row>
     <row r="50" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="280"/>
+      <c r="B50" s="272"/>
       <c r="C50" s="96"/>
       <c r="D50" s="82"/>
       <c r="E50" s="82"/>
@@ -5305,7 +5491,7 @@
       <c r="T53" s="49"/>
     </row>
     <row r="54" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="280"/>
+      <c r="B54" s="272"/>
       <c r="C54" s="96"/>
       <c r="D54" s="82"/>
       <c r="E54" s="82"/>
@@ -5359,8 +5545,8 @@
       <c r="L55" s="82"/>
       <c r="M55" s="82"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B56" s="280"/>
+    <row r="56" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="261"/>
       <c r="C56" s="96"/>
       <c r="D56" s="82"/>
       <c r="E56" s="82">
@@ -5386,10 +5572,10 @@
       <c r="M56" s="82"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B57" s="17">
+      <c r="B57" s="260">
         <v>1</v>
       </c>
-      <c r="C57" s="18"/>
+      <c r="C57" s="142"/>
       <c r="D57" s="18"/>
       <c r="E57" s="18"/>
       <c r="F57" s="18"/>
@@ -5405,8 +5591,46 @@
       <c r="L57" s="18"/>
       <c r="M57" s="18"/>
     </row>
+    <row r="58" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="261"/>
+      <c r="C58" s="142"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="309">
+        <v>200</v>
+      </c>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="309">
+        <v>20</v>
+      </c>
+      <c r="I58" s="18">
+        <v>10</v>
+      </c>
+      <c r="J58" s="18">
+        <v>30</v>
+      </c>
+      <c r="K58" s="18"/>
+      <c r="L58" s="18"/>
+      <c r="M58" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="31">
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B35:B36"/>
     <mergeCell ref="B55:B56"/>
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="B51:B52"/>
@@ -5422,21 +5646,6 @@
     <mergeCell ref="B46:B47"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="B53:B54"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B35:B36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9872,7 +10081,7 @@
       <c r="AW32" s="163">
         <v>25</v>
       </c>
-      <c r="AX32" s="304">
+      <c r="AX32" s="295">
         <v>70</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -9910,7 +10119,7 @@
       <c r="BM32" s="163">
         <v>50</v>
       </c>
-      <c r="BN32" s="304">
+      <c r="BN32" s="295">
         <v>20</v>
       </c>
       <c r="BO32" s="9" t="s">
@@ -10059,7 +10268,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="163"/>
-      <c r="AX33" s="305"/>
+      <c r="AX33" s="296"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -10095,7 +10304,7 @@
       <c r="BM33" s="140">
         <v>10</v>
       </c>
-      <c r="BN33" s="305"/>
+      <c r="BN33" s="296"/>
       <c r="BO33" s="9" t="s">
         <v>71</v>
       </c>
@@ -10246,7 +10455,7 @@
         <v>148</v>
       </c>
       <c r="AW34" s="140"/>
-      <c r="AX34" s="306"/>
+      <c r="AX34" s="297"/>
       <c r="AY34" s="9" t="s">
         <v>81</v>
       </c>
@@ -10284,7 +10493,7 @@
       <c r="BM34" s="165">
         <v>70</v>
       </c>
-      <c r="BN34" s="306"/>
+      <c r="BN34" s="297"/>
       <c r="BO34" s="9" t="s">
         <v>81</v>
       </c>
@@ -11757,7 +11966,7 @@
     </row>
     <row r="44" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="163"/>
-      <c r="C44" s="304">
+      <c r="C44" s="295">
         <v>55</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -11795,10 +12004,10 @@
       <c r="P44" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S44" s="297">
+      <c r="S44" s="304">
         <v>25</v>
       </c>
-      <c r="T44" s="304">
+      <c r="T44" s="295">
         <v>55</v>
       </c>
       <c r="U44" s="9" t="s">
@@ -11807,7 +12016,7 @@
       <c r="V44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="W44" s="299" t="s">
+      <c r="W44" s="298" t="s">
         <v>105</v>
       </c>
       <c r="X44" s="83" t="s">
@@ -11836,10 +12045,10 @@
       <c r="AG44" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="AJ44" s="297">
+      <c r="AJ44" s="304">
         <v>50</v>
       </c>
-      <c r="AK44" s="304">
+      <c r="AK44" s="295">
         <v>10</v>
       </c>
       <c r="AL44" s="190"/>
@@ -11849,7 +12058,7 @@
       <c r="AN44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO44" s="299" t="s">
+      <c r="AO44" s="298" t="s">
         <v>105</v>
       </c>
       <c r="AP44" s="83" t="s">
@@ -11879,7 +12088,7 @@
         <v>168</v>
       </c>
       <c r="AZ44" s="49"/>
-      <c r="BD44" s="297">
+      <c r="BD44" s="304">
         <v>50</v>
       </c>
       <c r="BE44" s="208"/>
@@ -11890,7 +12099,7 @@
       <c r="BH44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI44" s="299" t="s">
+      <c r="BI44" s="298" t="s">
         <v>105</v>
       </c>
       <c r="BJ44" s="83" t="s">
@@ -11919,7 +12128,7 @@
       <c r="BS44" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW44" s="297">
+      <c r="BW44" s="304">
         <v>25</v>
       </c>
       <c r="BX44" s="208"/>
@@ -11930,7 +12139,7 @@
       <c r="CA44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB44" s="299" t="s">
+      <c r="CB44" s="298" t="s">
         <v>105</v>
       </c>
       <c r="CC44" s="83" t="s">
@@ -11962,7 +12171,7 @@
     </row>
     <row r="45" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="140"/>
-      <c r="C45" s="305"/>
+      <c r="C45" s="296"/>
       <c r="D45" s="9" t="s">
         <v>71</v>
       </c>
@@ -11996,15 +12205,15 @@
       <c r="P45" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S45" s="298"/>
-      <c r="T45" s="306"/>
+      <c r="S45" s="305"/>
+      <c r="T45" s="297"/>
       <c r="U45" s="9" t="s">
         <v>71</v>
       </c>
       <c r="V45" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="W45" s="300"/>
+      <c r="W45" s="299"/>
       <c r="X45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12031,8 +12240,8 @@
       <c r="AG45" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="AJ45" s="298"/>
-      <c r="AK45" s="306"/>
+      <c r="AJ45" s="305"/>
+      <c r="AK45" s="297"/>
       <c r="AL45" s="191"/>
       <c r="AM45" s="9" t="s">
         <v>71</v>
@@ -12040,7 +12249,7 @@
       <c r="AN45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO45" s="300"/>
+      <c r="AO45" s="299"/>
       <c r="AP45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12068,7 +12277,7 @@
         <v>168</v>
       </c>
       <c r="AZ45" s="49"/>
-      <c r="BD45" s="298"/>
+      <c r="BD45" s="305"/>
       <c r="BE45" s="165">
         <v>20</v>
       </c>
@@ -12079,7 +12288,7 @@
       <c r="BH45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI45" s="300"/>
+      <c r="BI45" s="299"/>
       <c r="BJ45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12106,7 +12315,7 @@
       <c r="BS45" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW45" s="298"/>
+      <c r="BW45" s="305"/>
       <c r="BX45" s="165"/>
       <c r="BY45" s="191"/>
       <c r="BZ45" s="9" t="s">
@@ -12115,7 +12324,7 @@
       <c r="CA45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB45" s="300"/>
+      <c r="CB45" s="299"/>
       <c r="CC45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12145,7 +12354,7 @@
     </row>
     <row r="46" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="165"/>
-      <c r="C46" s="306"/>
+      <c r="C46" s="297"/>
       <c r="D46" s="9" t="s">
         <v>81</v>
       </c>
@@ -12750,7 +12959,7 @@
       <c r="AN49" s="25"/>
       <c r="AO49" s="119"/>
       <c r="AP49" s="119"/>
-      <c r="AQ49" s="301"/>
+      <c r="AQ49" s="300"/>
       <c r="AS49" s="192"/>
       <c r="AT49" s="2"/>
       <c r="AU49" s="256"/>
@@ -12766,7 +12975,7 @@
       <c r="BH49" s="25"/>
       <c r="BI49" s="119"/>
       <c r="BJ49" s="119"/>
-      <c r="BK49" s="301"/>
+      <c r="BK49" s="300"/>
       <c r="BM49" s="192"/>
       <c r="BN49" s="2"/>
       <c r="BO49" s="256"/>
@@ -12781,7 +12990,7 @@
       <c r="CA49" s="25"/>
       <c r="CB49" s="119"/>
       <c r="CC49" s="119"/>
-      <c r="CD49" s="301"/>
+      <c r="CD49" s="300"/>
       <c r="CF49" s="192"/>
       <c r="CG49" s="2"/>
       <c r="CH49" s="256"/>
@@ -12805,7 +13014,7 @@
       <c r="AN50" s="25"/>
       <c r="AO50" s="119"/>
       <c r="AP50" s="119"/>
-      <c r="AQ50" s="301"/>
+      <c r="AQ50" s="300"/>
       <c r="AS50" s="192"/>
       <c r="AT50" s="2"/>
       <c r="AU50" s="256"/>
@@ -12826,7 +13035,7 @@
       <c r="BH50" s="25"/>
       <c r="BI50" s="119"/>
       <c r="BJ50" s="119"/>
-      <c r="BK50" s="301"/>
+      <c r="BK50" s="300"/>
       <c r="BM50" s="192"/>
       <c r="BN50" s="2"/>
       <c r="BO50" s="256"/>
@@ -12846,7 +13055,7 @@
       <c r="CA50" s="25"/>
       <c r="CB50" s="119"/>
       <c r="CC50" s="119"/>
-      <c r="CD50" s="301"/>
+      <c r="CD50" s="300"/>
       <c r="CF50" s="192"/>
       <c r="CG50" s="2"/>
       <c r="CH50" s="256"/>
@@ -12910,14 +13119,14 @@
       <c r="AN51" s="114"/>
       <c r="AO51" s="201"/>
       <c r="AP51" s="202"/>
-      <c r="AQ51" s="302"/>
+      <c r="AQ51" s="301"/>
       <c r="AR51" s="201"/>
       <c r="AS51" s="203"/>
       <c r="AT51" s="116" t="s">
         <v>160</v>
       </c>
-      <c r="AU51" s="303"/>
-      <c r="AV51" s="296"/>
+      <c r="AU51" s="302"/>
+      <c r="AV51" s="303"/>
       <c r="AW51" s="65"/>
       <c r="AX51" s="65"/>
       <c r="AY51" s="115"/>
@@ -12929,14 +13138,14 @@
       <c r="BH51" s="114"/>
       <c r="BI51" s="201"/>
       <c r="BJ51" s="202"/>
-      <c r="BK51" s="302"/>
+      <c r="BK51" s="301"/>
       <c r="BL51" s="201"/>
       <c r="BM51" s="203"/>
       <c r="BN51" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="BO51" s="303"/>
-      <c r="BP51" s="296"/>
+      <c r="BO51" s="302"/>
+      <c r="BP51" s="303"/>
       <c r="BQ51" s="65"/>
       <c r="BR51" s="65"/>
       <c r="BS51" s="168"/>
@@ -12947,14 +13156,14 @@
       <c r="CA51" s="114"/>
       <c r="CB51" s="201"/>
       <c r="CC51" s="202"/>
-      <c r="CD51" s="302"/>
+      <c r="CD51" s="301"/>
       <c r="CE51" s="201"/>
       <c r="CF51" s="203" t="s">
         <v>180</v>
       </c>
       <c r="CG51" s="79"/>
-      <c r="CH51" s="303"/>
-      <c r="CI51" s="296"/>
+      <c r="CH51" s="302"/>
+      <c r="CI51" s="303"/>
       <c r="CJ51" s="65"/>
       <c r="CK51" s="65"/>
       <c r="CL51" s="168"/>
@@ -15351,7 +15560,7 @@
       <c r="G68" s="137"/>
       <c r="H68" s="203"/>
       <c r="I68" s="137"/>
-      <c r="J68" s="295"/>
+      <c r="J68" s="306"/>
       <c r="K68" s="50"/>
       <c r="L68" s="79"/>
       <c r="M68" s="79"/>
@@ -15426,7 +15635,7 @@
       <c r="AC69" s="137" t="s">
         <v>184</v>
       </c>
-      <c r="AD69" s="295"/>
+      <c r="AD69" s="306"/>
       <c r="AE69" s="50"/>
       <c r="AF69" s="50"/>
       <c r="AG69" s="79"/>
@@ -15534,22 +15743,40 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="AO44:AO45"/>
-    <mergeCell ref="AQ49:AQ51"/>
-    <mergeCell ref="AU49:AU51"/>
-    <mergeCell ref="AV49:AV51"/>
-    <mergeCell ref="AJ50:AK50"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="S44:S45"/>
-    <mergeCell ref="T44:T45"/>
-    <mergeCell ref="W44:W45"/>
-    <mergeCell ref="AJ38:AL38"/>
-    <mergeCell ref="AJ44:AJ45"/>
-    <mergeCell ref="AK44:AK45"/>
+    <mergeCell ref="BJ53:BL53"/>
+    <mergeCell ref="BJ68:BK68"/>
+    <mergeCell ref="BV68:BV69"/>
+    <mergeCell ref="BW68:BW69"/>
+    <mergeCell ref="BR69:BR70"/>
+    <mergeCell ref="AO53:AQ53"/>
+    <mergeCell ref="AO68:AP68"/>
+    <mergeCell ref="BA68:BA69"/>
+    <mergeCell ref="BB68:BB69"/>
+    <mergeCell ref="AW69:AW70"/>
+    <mergeCell ref="V52:X52"/>
+    <mergeCell ref="V67:W67"/>
+    <mergeCell ref="AH67:AH68"/>
+    <mergeCell ref="AI67:AI68"/>
+    <mergeCell ref="AD68:AD69"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="N66:N67"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="J67:J68"/>
+    <mergeCell ref="CI49:CI51"/>
+    <mergeCell ref="BW50:BX50"/>
+    <mergeCell ref="BW38:BY38"/>
+    <mergeCell ref="BW44:BW45"/>
+    <mergeCell ref="CB44:CB45"/>
+    <mergeCell ref="CD49:CD51"/>
+    <mergeCell ref="CH49:CH51"/>
+    <mergeCell ref="BP49:BP51"/>
+    <mergeCell ref="BD50:BE50"/>
+    <mergeCell ref="BD38:BF38"/>
+    <mergeCell ref="BD44:BD45"/>
+    <mergeCell ref="BI44:BI45"/>
+    <mergeCell ref="BK49:BK51"/>
+    <mergeCell ref="BO49:BO51"/>
     <mergeCell ref="BR24:BS24"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B36:C36"/>
@@ -15565,40 +15792,22 @@
     <mergeCell ref="BM36:BN36"/>
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="BP49:BP51"/>
-    <mergeCell ref="BD50:BE50"/>
-    <mergeCell ref="BD38:BF38"/>
-    <mergeCell ref="BD44:BD45"/>
-    <mergeCell ref="BI44:BI45"/>
-    <mergeCell ref="BK49:BK51"/>
-    <mergeCell ref="BO49:BO51"/>
-    <mergeCell ref="CI49:CI51"/>
-    <mergeCell ref="BW50:BX50"/>
-    <mergeCell ref="BW38:BY38"/>
-    <mergeCell ref="BW44:BW45"/>
-    <mergeCell ref="CB44:CB45"/>
-    <mergeCell ref="CD49:CD51"/>
-    <mergeCell ref="CH49:CH51"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="N66:N67"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="V52:X52"/>
-    <mergeCell ref="V67:W67"/>
-    <mergeCell ref="AH67:AH68"/>
-    <mergeCell ref="AI67:AI68"/>
-    <mergeCell ref="AD68:AD69"/>
-    <mergeCell ref="AO53:AQ53"/>
-    <mergeCell ref="AO68:AP68"/>
-    <mergeCell ref="BA68:BA69"/>
-    <mergeCell ref="BB68:BB69"/>
-    <mergeCell ref="AW69:AW70"/>
-    <mergeCell ref="BJ53:BL53"/>
-    <mergeCell ref="BJ68:BK68"/>
-    <mergeCell ref="BV68:BV69"/>
-    <mergeCell ref="BW68:BW69"/>
-    <mergeCell ref="BR69:BR70"/>
+    <mergeCell ref="AQ49:AQ51"/>
+    <mergeCell ref="AU49:AU51"/>
+    <mergeCell ref="AV49:AV51"/>
+    <mergeCell ref="AJ50:AK50"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="S44:S45"/>
+    <mergeCell ref="T44:T45"/>
+    <mergeCell ref="W44:W45"/>
+    <mergeCell ref="AJ38:AL38"/>
+    <mergeCell ref="AJ44:AJ45"/>
+    <mergeCell ref="AK44:AK45"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="AO44:AO45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.1.0 _9:30PM
Boat Enabled -
InCapacity - [0] , NodeW - [-3] , BirdW - [6] , FuelW - [20] , OnHost - [8+1]
VillageW=[3] , [X-MarketShieldMatrix-X] = [6,20,40,13]
Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.9.xlsx
+++ b/Usage_S_1.0.9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45124EE5-64D5-40D4-ABF1-4FC7FC5D17FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7C6DB4-0965-423E-AEC4-87BED4D729D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2291" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2294" uniqueCount="264">
   <si>
     <t>UnSettled</t>
   </si>
@@ -822,6 +822,12 @@
   </si>
   <si>
     <t>RPF</t>
+  </si>
+  <si>
+    <t>X-Local_BX(2)- X</t>
+  </si>
+  <si>
+    <t>X-Professional - (6)-X</t>
   </si>
 </sst>
 </file>
@@ -1758,7 +1764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="314">
+  <cellXfs count="313">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2372,7 +2378,12 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2418,6 +2429,12 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2427,15 +2444,39 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2472,43 +2513,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2522,32 +2536,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2838,8 +2847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI12" sqref="AI12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2868,7 +2877,8 @@
     <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="3.85546875" customWidth="1"/>
+    <col min="27" max="27" width="3.85546875" customWidth="1"/>
+    <col min="28" max="28" width="3.85546875" style="2" customWidth="1"/>
     <col min="29" max="29" width="5.28515625" style="1" customWidth="1"/>
     <col min="30" max="30" width="5.28515625" customWidth="1"/>
     <col min="31" max="31" width="1" customWidth="1"/>
@@ -2876,13 +2886,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z1" s="270" t="s">
+      <c r="Z1" s="268" t="s">
         <v>250</v>
       </c>
       <c r="AA1" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="AB1" s="36" t="s">
+      <c r="AB1" s="15" t="s">
         <v>231</v>
       </c>
       <c r="AC1" s="250" t="s">
@@ -2891,12 +2901,12 @@
       <c r="AD1" s="249" t="s">
         <v>224</v>
       </c>
-      <c r="AF1" s="252" t="s">
+      <c r="AF1" s="253" t="s">
         <v>241</v>
       </c>
-      <c r="AG1" s="253"/>
-      <c r="AH1" s="253"/>
-      <c r="AI1" s="254"/>
+      <c r="AG1" s="254"/>
+      <c r="AH1" s="254"/>
+      <c r="AI1" s="255"/>
     </row>
     <row r="2" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -2905,15 +2915,15 @@
       <c r="B2" s="34">
         <v>40.380000000000003</v>
       </c>
-      <c r="C2" s="260">
+      <c r="C2" s="261">
         <f>B3+B4</f>
         <v>0</v>
       </c>
-      <c r="E2" s="264" t="s">
+      <c r="E2" s="265" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="265"/>
-      <c r="G2" s="266"/>
+      <c r="F2" s="266"/>
+      <c r="G2" s="267"/>
       <c r="H2" s="26" t="s">
         <v>43</v>
       </c>
@@ -2963,22 +2973,22 @@
       <c r="Y2" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="Z2" s="271"/>
-      <c r="AA2" s="26">
-        <f>SUM(AA3:AA17)</f>
+      <c r="Z2" s="269"/>
+      <c r="AA2" s="36">
+        <f>SUM(AA3:AA19)</f>
         <v>6</v>
       </c>
-      <c r="AB2" s="26">
-        <f>SUM(AB3:AB17)</f>
+      <c r="AB2" s="15">
+        <f>SUM(AB3:AB19)</f>
         <v>20</v>
       </c>
-      <c r="AC2" s="34">
-        <f>SUM(AC3:AC17)</f>
-        <v>32</v>
-      </c>
-      <c r="AD2" s="8">
-        <f>SUM(AD3:AD17)</f>
-        <v>9</v>
+      <c r="AC2" s="36">
+        <f>SUM(AC3:AC19)</f>
+        <v>40</v>
+      </c>
+      <c r="AD2" s="36">
+        <f>SUM(AD3:AD19)</f>
+        <v>13</v>
       </c>
       <c r="AF2" s="9" t="s">
         <v>92</v>
@@ -2992,13 +3002,13 @@
       <c r="AI2" s="8"/>
     </row>
     <row r="3" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="258" t="s">
+      <c r="A3" s="259" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="34">
         <v>0</v>
       </c>
-      <c r="C3" s="261"/>
+      <c r="C3" s="262"/>
       <c r="D3" s="162" t="s">
         <v>36</v>
       </c>
@@ -3011,15 +3021,15 @@
       <c r="AA3" s="238">
         <v>1</v>
       </c>
-      <c r="AB3" s="251"/>
+      <c r="AB3" s="312"/>
       <c r="AC3" s="59">
         <v>4</v>
       </c>
       <c r="AD3" s="44"/>
-      <c r="AE3" s="267"/>
+      <c r="AE3" s="270"/>
     </row>
     <row r="4" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="259"/>
+      <c r="A4" s="260"/>
       <c r="B4" s="34">
         <v>0</v>
       </c>
@@ -3030,7 +3040,9 @@
         <v>10</v>
       </c>
       <c r="F4" s="205"/>
-      <c r="G4" s="247"/>
+      <c r="G4" s="247">
+        <v>15</v>
+      </c>
       <c r="H4" s="9" t="s">
         <v>199</v>
       </c>
@@ -3067,7 +3079,7 @@
       <c r="S4" s="154">
         <v>0.4861111111111111</v>
       </c>
-      <c r="T4" s="313">
+      <c r="T4" s="252">
         <v>1</v>
       </c>
       <c r="U4" s="245">
@@ -3079,15 +3091,14 @@
       <c r="Z4" s="169" t="s">
         <v>220</v>
       </c>
-      <c r="AA4" s="307"/>
-      <c r="AB4" s="308"/>
-      <c r="AC4" s="311">
+      <c r="AB4" s="20"/>
+      <c r="AC4" s="1">
         <v>4</v>
       </c>
       <c r="AD4" s="240">
         <v>3</v>
       </c>
-      <c r="AE4" s="268"/>
+      <c r="AE4" s="271"/>
       <c r="AF4" s="25" t="s">
         <v>181</v>
       </c>
@@ -3105,7 +3116,9 @@
       </c>
       <c r="E5" s="218"/>
       <c r="F5" s="206"/>
-      <c r="G5" s="37"/>
+      <c r="G5" s="127">
+        <v>40</v>
+      </c>
       <c r="H5" s="9" t="s">
         <v>1</v>
       </c>
@@ -3115,7 +3128,9 @@
       <c r="J5" s="213" t="s">
         <v>165</v>
       </c>
-      <c r="K5" s="215"/>
+      <c r="K5" s="194" t="s">
+        <v>242</v>
+      </c>
       <c r="L5" s="167" t="s">
         <v>142</v>
       </c>
@@ -3137,8 +3152,11 @@
       <c r="S5" s="154">
         <v>0.88611111111111107</v>
       </c>
+      <c r="T5" s="238">
+        <v>2</v>
+      </c>
       <c r="U5" s="245">
-        <v>45292</v>
+        <v>45293</v>
       </c>
       <c r="Y5" s="25" t="s">
         <v>245</v>
@@ -3146,15 +3164,14 @@
       <c r="Z5" s="215" t="s">
         <v>219</v>
       </c>
-      <c r="AA5" s="307"/>
-      <c r="AB5" s="308"/>
-      <c r="AC5" s="311">
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="1">
         <v>4</v>
       </c>
       <c r="AD5" s="240">
         <v>3</v>
       </c>
-      <c r="AE5" s="268"/>
+      <c r="AE5" s="271"/>
       <c r="AF5" s="25" t="s">
         <v>30</v>
       </c>
@@ -3167,14 +3184,16 @@
     </row>
     <row r="6" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
-        <v>3192</v>
+        <v>3332</v>
       </c>
       <c r="C6">
-        <v>5773</v>
+        <v>5633</v>
       </c>
       <c r="E6" s="218"/>
       <c r="F6" s="207"/>
-      <c r="G6" s="127"/>
+      <c r="G6" s="127">
+        <v>10</v>
+      </c>
       <c r="H6" s="9" t="s">
         <v>203</v>
       </c>
@@ -3184,7 +3203,9 @@
       <c r="J6" s="213" t="s">
         <v>165</v>
       </c>
-      <c r="K6" s="169"/>
+      <c r="K6" s="169" t="s">
+        <v>222</v>
+      </c>
       <c r="L6" s="83" t="s">
         <v>123</v>
       </c>
@@ -3206,8 +3227,11 @@
       <c r="S6" s="154">
         <v>0.88611111111111107</v>
       </c>
+      <c r="T6" s="241">
+        <v>1</v>
+      </c>
       <c r="U6" s="245">
-        <v>45292</v>
+        <v>45293</v>
       </c>
       <c r="Y6" s="25" t="s">
         <v>245</v>
@@ -3218,12 +3242,11 @@
       <c r="AA6" s="238">
         <v>3</v>
       </c>
-      <c r="AB6" s="26">
+      <c r="AB6" s="15">
         <v>1</v>
       </c>
-      <c r="AC6" s="311"/>
       <c r="AD6" s="49"/>
-      <c r="AE6" s="268"/>
+      <c r="AE6" s="271"/>
       <c r="AF6" s="25"/>
       <c r="AH6" s="24"/>
     </row>
@@ -3272,13 +3295,13 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="S7" s="154">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="T7" s="310">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="T7" s="251">
         <v>1</v>
       </c>
       <c r="U7" s="245">
-        <v>45292</v>
+        <v>45293</v>
       </c>
       <c r="Y7" s="25" t="s">
         <v>245</v>
@@ -3289,14 +3312,14 @@
       <c r="AA7" s="26">
         <v>1</v>
       </c>
-      <c r="AB7" s="26">
+      <c r="AB7" s="15">
         <v>6</v>
       </c>
-      <c r="AC7" s="311">
+      <c r="AC7" s="1">
         <v>4</v>
       </c>
       <c r="AD7" s="49"/>
-      <c r="AE7" s="268"/>
+      <c r="AE7" s="271"/>
       <c r="AF7" s="25"/>
       <c r="AG7" s="25" t="s">
         <v>46</v>
@@ -3354,15 +3377,15 @@
       <c r="Z8" s="169" t="s">
         <v>228</v>
       </c>
-      <c r="AA8" s="308"/>
-      <c r="AB8" s="26">
+      <c r="AA8" s="25"/>
+      <c r="AB8" s="15">
         <v>4</v>
       </c>
-      <c r="AC8" s="311">
+      <c r="AC8" s="1">
         <v>4</v>
       </c>
       <c r="AD8" s="49"/>
-      <c r="AE8" s="268"/>
+      <c r="AE8" s="271"/>
       <c r="AF8" s="25"/>
       <c r="AG8" s="25"/>
       <c r="AH8" s="24" t="s">
@@ -3375,7 +3398,7 @@
       </c>
       <c r="B9" s="8">
         <f>7000+B6+B5-C2</f>
-        <v>10192</v>
+        <v>10332</v>
       </c>
       <c r="E9" s="163"/>
       <c r="F9" s="165">
@@ -3427,20 +3450,21 @@
       <c r="Z9" s="169" t="s">
         <v>229</v>
       </c>
-      <c r="AA9" s="308"/>
-      <c r="AB9" s="26">
+      <c r="AA9" s="25"/>
+      <c r="AB9" s="15">
         <v>1</v>
       </c>
-      <c r="AC9" s="311"/>
       <c r="AD9" s="49"/>
-      <c r="AE9" s="268"/>
+      <c r="AE9" s="271"/>
       <c r="AF9" s="25"/>
       <c r="AH9" s="24"/>
     </row>
     <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="220"/>
       <c r="F10" s="206"/>
-      <c r="G10" s="177"/>
+      <c r="G10" s="177">
+        <v>40</v>
+      </c>
       <c r="H10" s="9" t="s">
         <v>81</v>
       </c>
@@ -3449,7 +3473,7 @@
       </c>
       <c r="J10" s="213"/>
       <c r="K10" s="169" t="s">
-        <v>222</v>
+        <v>262</v>
       </c>
       <c r="L10" s="83" t="s">
         <v>143</v>
@@ -3467,13 +3491,16 @@
         <v>66</v>
       </c>
       <c r="Q10" s="154">
-        <v>0.625</v>
+        <v>0.88611111111111107</v>
       </c>
       <c r="S10" s="154">
-        <v>0.625</v>
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="T10" s="252">
+        <v>2</v>
       </c>
       <c r="U10" s="245">
-        <v>45292</v>
+        <v>45293</v>
       </c>
       <c r="Y10" s="25" t="s">
         <v>259</v>
@@ -3481,15 +3508,13 @@
       <c r="Z10" s="169" t="s">
         <v>232</v>
       </c>
-      <c r="AA10" s="307"/>
-      <c r="AB10" s="26">
+      <c r="AB10" s="15">
         <v>1</v>
       </c>
-      <c r="AC10" s="311"/>
       <c r="AD10" s="49">
         <v>1</v>
       </c>
-      <c r="AE10" s="268"/>
+      <c r="AE10" s="271"/>
       <c r="AF10" s="25" t="s">
         <v>66</v>
       </c>
@@ -3514,7 +3539,9 @@
       <c r="F11" s="242">
         <v>5</v>
       </c>
-      <c r="G11" s="37"/>
+      <c r="G11" s="37">
+        <v>20</v>
+      </c>
       <c r="H11" s="9" t="s">
         <v>102</v>
       </c>
@@ -3525,7 +3552,7 @@
         <v>116</v>
       </c>
       <c r="K11" s="194" t="s">
-        <v>242</v>
+        <v>263</v>
       </c>
       <c r="L11" s="83" t="s">
         <v>124</v>
@@ -3563,15 +3590,14 @@
       <c r="Z11" s="169" t="s">
         <v>233</v>
       </c>
-      <c r="AA11" s="307"/>
-      <c r="AB11" s="26">
+      <c r="AB11" s="15">
         <v>2</v>
       </c>
-      <c r="AC11" s="311">
+      <c r="AC11" s="1">
         <v>5</v>
       </c>
       <c r="AD11" s="49"/>
-      <c r="AE11" s="268"/>
+      <c r="AE11" s="271"/>
       <c r="AF11" s="25" t="s">
         <v>261</v>
       </c>
@@ -3624,7 +3650,7 @@
         <v>3</v>
       </c>
       <c r="U12" s="245">
-        <v>45292</v>
+        <v>45293</v>
       </c>
       <c r="Y12" s="25" t="s">
         <v>245</v>
@@ -3632,17 +3658,16 @@
       <c r="Z12" s="169" t="s">
         <v>234</v>
       </c>
-      <c r="AA12" s="307"/>
-      <c r="AB12" s="26">
+      <c r="AB12" s="15">
         <v>1</v>
       </c>
-      <c r="AC12" s="312">
+      <c r="AC12" s="1">
         <v>1</v>
       </c>
       <c r="AD12" s="49">
         <v>1</v>
       </c>
-      <c r="AE12" s="268"/>
+      <c r="AE12" s="271"/>
       <c r="AF12" s="25" t="s">
         <v>65</v>
       </c>
@@ -3659,13 +3684,15 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>10192</v>
+        <v>10332</v>
       </c>
       <c r="E13" s="36"/>
       <c r="F13" s="206">
         <v>1</v>
       </c>
-      <c r="G13" s="246"/>
+      <c r="G13" s="246">
+        <v>5</v>
+      </c>
       <c r="H13" s="9" t="s">
         <v>189</v>
       </c>
@@ -3700,6 +3727,9 @@
       <c r="S13" s="154">
         <v>0.88611111111111107</v>
       </c>
+      <c r="T13" s="238">
+        <v>2</v>
+      </c>
       <c r="U13" s="245">
         <v>45293</v>
       </c>
@@ -3709,13 +3739,11 @@
       <c r="Z13" s="169" t="s">
         <v>235</v>
       </c>
-      <c r="AA13" s="307"/>
-      <c r="AB13" s="26">
+      <c r="AB13" s="15">
         <v>2</v>
       </c>
-      <c r="AC13" s="311"/>
       <c r="AD13" s="49"/>
-      <c r="AE13" s="268"/>
+      <c r="AE13" s="271"/>
       <c r="AF13" s="25"/>
       <c r="AG13" s="25"/>
       <c r="AH13" s="24"/>
@@ -3727,7 +3755,9 @@
       <c r="F14" s="205">
         <v>10</v>
       </c>
-      <c r="G14" s="184"/>
+      <c r="G14" s="127">
+        <v>10</v>
+      </c>
       <c r="H14" s="9" t="s">
         <v>9</v>
       </c>
@@ -3760,7 +3790,7 @@
       <c r="S14" s="154">
         <v>0.91666666666666663</v>
       </c>
-      <c r="T14" s="313">
+      <c r="T14" s="252">
         <v>2</v>
       </c>
       <c r="U14" s="245">
@@ -3775,14 +3805,13 @@
       <c r="AA14" s="239">
         <v>1</v>
       </c>
-      <c r="AB14" s="307"/>
       <c r="AC14" s="241">
         <v>1</v>
       </c>
       <c r="AD14" s="49">
         <v>1</v>
       </c>
-      <c r="AE14" s="268"/>
+      <c r="AE14" s="271"/>
       <c r="AF14" s="25" t="s">
         <v>65</v>
       </c>
@@ -3821,15 +3850,15 @@
       <c r="O15" s="8"/>
       <c r="P15" s="37"/>
       <c r="Q15" s="154">
-        <v>0.91666666666666663</v>
+        <v>0.88611111111111107</v>
       </c>
       <c r="R15"/>
       <c r="S15" s="154">
-        <v>0.91666666666666663</v>
+        <v>0.88611111111111107</v>
       </c>
       <c r="T15" s="24"/>
       <c r="U15" s="245">
-        <v>45292</v>
+        <v>45293</v>
       </c>
       <c r="Y15" s="25" t="s">
         <v>259</v>
@@ -3837,13 +3866,12 @@
       <c r="Z15" s="169" t="s">
         <v>238</v>
       </c>
-      <c r="AA15" s="307"/>
-      <c r="AB15" s="308"/>
-      <c r="AC15" s="311">
+      <c r="AB15" s="20"/>
+      <c r="AC15" s="1">
         <v>1</v>
       </c>
       <c r="AD15" s="49"/>
-      <c r="AE15" s="268"/>
+      <c r="AE15" s="271"/>
       <c r="AF15" s="25"/>
       <c r="AG15" s="25" t="s">
         <v>46</v>
@@ -3865,34 +3893,32 @@
       <c r="Z16" s="169" t="s">
         <v>239</v>
       </c>
-      <c r="AA16" s="307"/>
-      <c r="AB16" s="307"/>
-      <c r="AC16" s="311">
+      <c r="AC16" s="1">
         <v>4</v>
       </c>
       <c r="AD16" s="49"/>
-      <c r="AE16" s="268"/>
+      <c r="AE16" s="271"/>
       <c r="AF16" s="25"/>
       <c r="AH16" s="24"/>
     </row>
     <row r="17" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="262" t="s">
+      <c r="E17" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="263"/>
+      <c r="F17" s="264"/>
       <c r="G17" s="189"/>
       <c r="H17" s="9">
         <f>SUM(E4:G15)</f>
-        <v>305</v>
+        <v>445</v>
       </c>
       <c r="I17" s="26"/>
       <c r="J17" s="119"/>
       <c r="K17" s="216"/>
       <c r="L17" s="119"/>
-      <c r="Q17" s="256"/>
-      <c r="R17" s="257"/>
+      <c r="Q17" s="257"/>
+      <c r="R17" s="258"/>
       <c r="Y17" s="25" t="s">
         <v>245</v>
       </c>
@@ -3900,12 +3926,12 @@
         <v>240</v>
       </c>
       <c r="AA17" s="50"/>
-      <c r="AB17" s="26">
+      <c r="AB17" s="15">
         <v>2</v>
       </c>
       <c r="AC17" s="65"/>
       <c r="AD17" s="51"/>
-      <c r="AE17" s="268"/>
+      <c r="AE17" s="271"/>
       <c r="AF17" s="25" t="s">
         <v>65</v>
       </c>
@@ -3931,24 +3957,22 @@
       <c r="I18" s="226"/>
       <c r="J18" s="119"/>
       <c r="L18" s="119"/>
-      <c r="M18" s="255"/>
-      <c r="Q18" s="256"/>
-      <c r="R18" s="257"/>
+      <c r="M18" s="256"/>
+      <c r="Q18" s="257"/>
+      <c r="R18" s="258"/>
       <c r="Y18" s="25" t="s">
         <v>245</v>
       </c>
       <c r="Z18" s="169" t="s">
         <v>257</v>
       </c>
-      <c r="AA18" s="307"/>
-      <c r="AB18" s="307"/>
-      <c r="AC18" s="311">
+      <c r="AC18" s="1">
         <v>4</v>
       </c>
       <c r="AD18" s="49">
         <v>2</v>
       </c>
-      <c r="AE18" s="268"/>
+      <c r="AE18" s="271"/>
       <c r="AF18" s="25" t="s">
         <v>30</v>
       </c>
@@ -3962,7 +3986,7 @@
     <row r="19" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I19" s="226"/>
       <c r="L19" s="119"/>
-      <c r="M19" s="255"/>
+      <c r="M19" s="256"/>
       <c r="Y19" s="25" t="s">
         <v>245</v>
       </c>
@@ -3970,14 +3994,14 @@
         <v>258</v>
       </c>
       <c r="AA19" s="50"/>
-      <c r="AB19" s="50"/>
+      <c r="AB19" s="79"/>
       <c r="AC19" s="65">
         <v>4</v>
       </c>
       <c r="AD19" s="51">
         <v>2</v>
       </c>
-      <c r="AE19" s="269"/>
+      <c r="AE19" s="272"/>
       <c r="AF19" s="25" t="s">
         <v>243</v>
       </c>
@@ -4012,10 +4036,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:T58"/>
+  <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4039,18 +4063,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="285" t="s">
+      <c r="E1" s="273" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="287"/>
+      <c r="F1" s="275"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="285" t="s">
+      <c r="H1" s="273" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="286"/>
-      <c r="J1" s="287"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="275"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -4068,7 +4092,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="288">
+      <c r="B2" s="276">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -4095,26 +4119,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="291">
+      <c r="K2" s="279">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="283">
+      <c r="L2" s="294">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="273">
+      <c r="M2" s="284">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J58)</f>
-        <v>10152</v>
+        <f>SUM(E2:J59)</f>
+        <v>10292</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="289"/>
+      <c r="B3" s="277"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -4129,13 +4153,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="292"/>
-      <c r="L3" s="284"/>
-      <c r="M3" s="274"/>
+      <c r="K3" s="280"/>
+      <c r="L3" s="295"/>
+      <c r="M3" s="285"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="290"/>
+      <c r="B4" s="278"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -4150,9 +4174,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="292"/>
-      <c r="L4" s="284"/>
-      <c r="M4" s="274"/>
+      <c r="K4" s="280"/>
+      <c r="L4" s="295"/>
+      <c r="M4" s="285"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -4234,7 +4258,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="275">
+      <c r="B7" s="286">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -4251,22 +4275,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="277">
+      <c r="K7" s="288">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="279">
+      <c r="L7" s="290">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="281">
+      <c r="M7" s="292">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="276"/>
+      <c r="B8" s="287"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -4287,9 +4311,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="278"/>
-      <c r="L8" s="280"/>
-      <c r="M8" s="282"/>
+      <c r="K8" s="289"/>
+      <c r="L8" s="291"/>
+      <c r="M8" s="293"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -4369,7 +4393,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="275">
+      <c r="B11" s="286">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -4396,7 +4420,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="276"/>
+      <c r="B12" s="287"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -4453,7 +4477,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="275">
+      <c r="B14" s="286">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -4476,7 +4500,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="276"/>
+      <c r="B15" s="287"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -4500,7 +4524,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="288">
+      <c r="B16" s="276">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -4531,7 +4555,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="289"/>
+      <c r="B17" s="277"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -4549,7 +4573,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="288">
+      <c r="B18" s="276">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -4578,7 +4602,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="290"/>
+      <c r="B19" s="278"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -4638,7 +4662,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="293">
+      <c r="B21" s="282">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -4666,7 +4690,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="294"/>
+      <c r="B22" s="283"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -4718,7 +4742,7 @@
       <c r="M23" s="70"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="260">
+      <c r="B24" s="261">
         <v>16</v>
       </c>
       <c r="C24" s="141"/>
@@ -4747,7 +4771,7 @@
       <c r="A25" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="261"/>
+      <c r="B25" s="262"/>
       <c r="C25" s="142"/>
       <c r="D25" s="18">
         <v>130</v>
@@ -4775,7 +4799,7 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="260">
+      <c r="B26" s="261">
         <v>17</v>
       </c>
       <c r="C26" s="161"/>
@@ -4806,7 +4830,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="272"/>
+      <c r="B27" s="281"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -4837,7 +4861,7 @@
       <c r="A28" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="260">
+      <c r="B28" s="261">
         <v>18</v>
       </c>
       <c r="C28" s="141"/>
@@ -4859,7 +4883,7 @@
       <c r="M28" s="70"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="261"/>
+      <c r="B29" s="262"/>
       <c r="C29" s="142"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18">
@@ -4885,7 +4909,7 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="260">
+      <c r="B30" s="261">
         <v>19</v>
       </c>
       <c r="C30" s="142"/>
@@ -4908,7 +4932,7 @@
       <c r="A31" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="261"/>
+      <c r="B31" s="262"/>
       <c r="C31" s="142"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -4935,7 +4959,7 @@
       <c r="A32" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="260">
+      <c r="B32" s="261">
         <v>20</v>
       </c>
       <c r="C32" s="142"/>
@@ -4957,7 +4981,7 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="261"/>
+      <c r="B33" s="262"/>
       <c r="C33" s="142"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -5010,7 +5034,7 @@
       <c r="M34" s="82"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="260">
+      <c r="B35" s="261">
         <v>22</v>
       </c>
       <c r="C35" s="96"/>
@@ -5037,7 +5061,7 @@
       <c r="A36" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="261"/>
+      <c r="B36" s="262"/>
       <c r="C36" s="142"/>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -5059,7 +5083,7 @@
       <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="260">
+      <c r="B37" s="261">
         <v>23</v>
       </c>
       <c r="C37" s="142"/>
@@ -5092,7 +5116,7 @@
       <c r="A38" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="261"/>
+      <c r="B38" s="262"/>
       <c r="C38" s="96"/>
       <c r="D38" s="82"/>
       <c r="E38" s="82"/>
@@ -5110,7 +5134,7 @@
       <c r="M38" s="82"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="260">
+      <c r="B39" s="261">
         <v>24</v>
       </c>
       <c r="C39" s="142"/>
@@ -5137,7 +5161,7 @@
       <c r="A40" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="272"/>
+      <c r="B40" s="281"/>
       <c r="C40" s="96"/>
       <c r="D40" s="82">
         <v>210</v>
@@ -5165,7 +5189,7 @@
       <c r="M40" s="82"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="260">
+      <c r="B41" s="261">
         <v>25</v>
       </c>
       <c r="C41" s="142"/>
@@ -5192,7 +5216,7 @@
       <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="272"/>
+      <c r="B42" s="281"/>
       <c r="C42" s="142"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -5210,7 +5234,7 @@
       <c r="M42" s="18"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="261"/>
+      <c r="B43" s="262"/>
       <c r="C43" s="142"/>
       <c r="D43" s="18">
         <v>190</v>
@@ -5239,7 +5263,7 @@
       <c r="A44" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="260">
+      <c r="B44" s="261">
         <v>26</v>
       </c>
       <c r="C44" s="142"/>
@@ -5265,7 +5289,7 @@
       <c r="M44" s="18"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="261"/>
+      <c r="B45" s="262"/>
       <c r="C45" s="142"/>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
@@ -5290,7 +5314,7 @@
       <c r="A46" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="260">
+      <c r="B46" s="261">
         <v>27</v>
       </c>
       <c r="C46" s="142"/>
@@ -5312,7 +5336,7 @@
       <c r="M46" s="18"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="272"/>
+      <c r="B47" s="281"/>
       <c r="C47" s="211"/>
       <c r="D47" s="132"/>
       <c r="E47" s="132"/>
@@ -5333,7 +5357,7 @@
       <c r="A48" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="260">
+      <c r="B48" s="261">
         <v>28</v>
       </c>
       <c r="C48" s="142"/>
@@ -5353,7 +5377,7 @@
       <c r="M48" s="18"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="272"/>
+      <c r="B49" s="281"/>
       <c r="C49" s="142"/>
       <c r="D49" s="18">
         <v>175</v>
@@ -5379,7 +5403,7 @@
       <c r="M49" s="18"/>
     </row>
     <row r="50" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="272"/>
+      <c r="B50" s="281"/>
       <c r="C50" s="96"/>
       <c r="D50" s="82"/>
       <c r="E50" s="82"/>
@@ -5406,7 +5430,7 @@
       <c r="A51" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="260">
+      <c r="B51" s="261">
         <v>29</v>
       </c>
       <c r="C51" s="142"/>
@@ -5428,7 +5452,7 @@
       <c r="M51" s="18"/>
     </row>
     <row r="52" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="261"/>
+      <c r="B52" s="262"/>
       <c r="C52" s="142"/>
       <c r="D52" s="18">
         <v>190</v>
@@ -5461,7 +5485,7 @@
       <c r="A53" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="260">
+      <c r="B53" s="261">
         <v>30</v>
       </c>
       <c r="C53" s="142"/>
@@ -5491,7 +5515,7 @@
       <c r="T53" s="49"/>
     </row>
     <row r="54" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="272"/>
+      <c r="B54" s="281"/>
       <c r="C54" s="96"/>
       <c r="D54" s="82"/>
       <c r="E54" s="82"/>
@@ -5518,7 +5542,7 @@
       <c r="A55" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B55" s="260">
+      <c r="B55" s="261">
         <v>31</v>
       </c>
       <c r="C55" s="96"/>
@@ -5546,7 +5570,7 @@
       <c r="M55" s="82"/>
     </row>
     <row r="56" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="261"/>
+      <c r="B56" s="262"/>
       <c r="C56" s="96"/>
       <c r="D56" s="82"/>
       <c r="E56" s="82">
@@ -5572,7 +5596,7 @@
       <c r="M56" s="82"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B57" s="260">
+      <c r="B57" s="309">
         <v>1</v>
       </c>
       <c r="C57" s="142"/>
@@ -5592,15 +5616,15 @@
       <c r="M57" s="18"/>
     </row>
     <row r="58" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="261"/>
+      <c r="B58" s="310"/>
       <c r="C58" s="142"/>
       <c r="D58" s="18"/>
-      <c r="E58" s="309">
+      <c r="E58" s="18">
         <v>200</v>
       </c>
       <c r="F58" s="18"/>
       <c r="G58" s="18"/>
-      <c r="H58" s="309">
+      <c r="H58" s="18">
         <v>20</v>
       </c>
       <c r="I58" s="18">
@@ -5613,9 +5637,53 @@
       <c r="L58" s="18"/>
       <c r="M58" s="18"/>
     </row>
+    <row r="59" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59" s="311"/>
+      <c r="C59" s="142"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="308">
+        <v>15</v>
+      </c>
+      <c r="F59" s="18">
+        <v>40</v>
+      </c>
+      <c r="G59" s="308">
+        <v>20</v>
+      </c>
+      <c r="H59" s="308">
+        <v>20</v>
+      </c>
+      <c r="I59" s="308">
+        <v>20</v>
+      </c>
+      <c r="J59" s="308">
+        <v>25</v>
+      </c>
+      <c r="K59" s="18"/>
+      <c r="L59" s="18"/>
+      <c r="M59" s="18"/>
+    </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B53:B54"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="K2:K4"/>
@@ -5631,21 +5699,6 @@
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B53:B54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8852,10 +8905,10 @@
       <c r="CG23" s="49"/>
     </row>
     <row r="24" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AG24" s="262" t="s">
+      <c r="AG24" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="AH24" s="263"/>
+      <c r="AH24" s="264"/>
       <c r="AI24" s="9">
         <f>SUM(AG16:AH23)</f>
         <v>40</v>
@@ -8875,10 +8928,10 @@
       <c r="AV24" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AZ24" s="262" t="s">
+      <c r="AZ24" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="BA24" s="263"/>
+      <c r="BA24" s="264"/>
       <c r="BB24" s="9">
         <f>SUM(AZ16:BA23)</f>
         <v>335</v>
@@ -8898,10 +8951,10 @@
       <c r="BO24" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="BR24" s="262" t="s">
+      <c r="BR24" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="BS24" s="263"/>
+      <c r="BS24" s="264"/>
       <c r="BT24" s="9">
         <f>SUM(BR16:BS23)</f>
         <v>275</v>
@@ -8924,10 +8977,10 @@
     </row>
     <row r="25" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="264" t="s">
+      <c r="B26" s="265" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="266"/>
+      <c r="C26" s="267"/>
       <c r="D26" s="26" t="s">
         <v>43</v>
       </c>
@@ -8964,10 +9017,10 @@
       <c r="O26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="R26" s="264" t="s">
+      <c r="R26" s="265" t="s">
         <v>145</v>
       </c>
-      <c r="S26" s="266"/>
+      <c r="S26" s="267"/>
       <c r="T26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9004,10 +9057,10 @@
       <c r="AE26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AG26" s="264" t="s">
+      <c r="AG26" s="265" t="s">
         <v>145</v>
       </c>
-      <c r="AH26" s="266"/>
+      <c r="AH26" s="267"/>
       <c r="AI26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9044,10 +9097,10 @@
       <c r="AT26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AW26" s="264" t="s">
+      <c r="AW26" s="265" t="s">
         <v>145</v>
       </c>
-      <c r="AX26" s="266"/>
+      <c r="AX26" s="267"/>
       <c r="AY26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9084,10 +9137,10 @@
       <c r="BJ26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="BM26" s="264" t="s">
+      <c r="BM26" s="265" t="s">
         <v>145</v>
       </c>
-      <c r="BN26" s="266"/>
+      <c r="BN26" s="267"/>
       <c r="BO26" s="26" t="s">
         <v>43</v>
       </c>
@@ -10081,7 +10134,7 @@
       <c r="AW32" s="163">
         <v>25</v>
       </c>
-      <c r="AX32" s="295">
+      <c r="AX32" s="305">
         <v>70</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -10119,7 +10172,7 @@
       <c r="BM32" s="163">
         <v>50</v>
       </c>
-      <c r="BN32" s="295">
+      <c r="BN32" s="305">
         <v>20</v>
       </c>
       <c r="BO32" s="9" t="s">
@@ -10268,7 +10321,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="163"/>
-      <c r="AX33" s="296"/>
+      <c r="AX33" s="306"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -10304,7 +10357,7 @@
       <c r="BM33" s="140">
         <v>10</v>
       </c>
-      <c r="BN33" s="296"/>
+      <c r="BN33" s="306"/>
       <c r="BO33" s="9" t="s">
         <v>71</v>
       </c>
@@ -10455,7 +10508,7 @@
         <v>148</v>
       </c>
       <c r="AW34" s="140"/>
-      <c r="AX34" s="297"/>
+      <c r="AX34" s="307"/>
       <c r="AY34" s="9" t="s">
         <v>81</v>
       </c>
@@ -10493,7 +10546,7 @@
       <c r="BM34" s="165">
         <v>70</v>
       </c>
-      <c r="BN34" s="297"/>
+      <c r="BN34" s="307"/>
       <c r="BO34" s="9" t="s">
         <v>81</v>
       </c>
@@ -10724,10 +10777,10 @@
       </c>
     </row>
     <row r="36" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="262" t="s">
+      <c r="B36" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="263"/>
+      <c r="C36" s="264"/>
       <c r="D36" s="9">
         <f>SUM(B28:C35)</f>
         <v>512</v>
@@ -10745,10 +10798,10 @@
       <c r="M36" s="65"/>
       <c r="N36" s="65"/>
       <c r="O36" s="102"/>
-      <c r="R36" s="262" t="s">
+      <c r="R36" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="S36" s="263"/>
+      <c r="S36" s="264"/>
       <c r="T36" s="9">
         <f>SUM(R28:S35)</f>
         <v>182</v>
@@ -10766,10 +10819,10 @@
       <c r="AC36" s="65"/>
       <c r="AD36" s="65"/>
       <c r="AE36" s="102"/>
-      <c r="AG36" s="262" t="s">
+      <c r="AG36" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="AH36" s="263"/>
+      <c r="AH36" s="264"/>
       <c r="AI36" s="9">
         <f>SUM(AG28:AH35)</f>
         <v>360</v>
@@ -10787,10 +10840,10 @@
       <c r="AR36" s="65"/>
       <c r="AS36" s="65"/>
       <c r="AT36" s="102"/>
-      <c r="AW36" s="262" t="s">
+      <c r="AW36" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="AX36" s="263"/>
+      <c r="AX36" s="264"/>
       <c r="AY36" s="9">
         <f>SUM(AW28:AX35)</f>
         <v>200</v>
@@ -10808,10 +10861,10 @@
       <c r="BH36" s="65"/>
       <c r="BI36" s="65"/>
       <c r="BJ36" s="102"/>
-      <c r="BM36" s="262" t="s">
+      <c r="BM36" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="BN36" s="263"/>
+      <c r="BN36" s="264"/>
       <c r="BO36" s="9">
         <f>SUM(BM28:BN35)</f>
         <v>260</v>
@@ -10831,10 +10884,10 @@
     </row>
     <row r="37" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="264" t="s">
+      <c r="B38" s="265" t="s">
         <v>145</v>
       </c>
-      <c r="C38" s="266"/>
+      <c r="C38" s="267"/>
       <c r="D38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10874,10 +10927,10 @@
       <c r="P38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="S38" s="264" t="s">
+      <c r="S38" s="265" t="s">
         <v>145</v>
       </c>
-      <c r="T38" s="266"/>
+      <c r="T38" s="267"/>
       <c r="U38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10917,11 +10970,11 @@
       <c r="AG38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="AJ38" s="264" t="s">
+      <c r="AJ38" s="265" t="s">
         <v>145</v>
       </c>
-      <c r="AK38" s="265"/>
-      <c r="AL38" s="266"/>
+      <c r="AK38" s="266"/>
+      <c r="AL38" s="267"/>
       <c r="AM38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10966,11 +11019,11 @@
         <f ca="1">TODAY()</f>
         <v>45292</v>
       </c>
-      <c r="BD38" s="264" t="s">
+      <c r="BD38" s="265" t="s">
         <v>145</v>
       </c>
-      <c r="BE38" s="265"/>
-      <c r="BF38" s="266"/>
+      <c r="BE38" s="266"/>
+      <c r="BF38" s="267"/>
       <c r="BG38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11010,11 +11063,11 @@
       <c r="BS38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="BW38" s="264" t="s">
+      <c r="BW38" s="265" t="s">
         <v>145</v>
       </c>
-      <c r="BX38" s="265"/>
-      <c r="BY38" s="266"/>
+      <c r="BX38" s="266"/>
+      <c r="BY38" s="267"/>
       <c r="BZ38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11966,7 +12019,7 @@
     </row>
     <row r="44" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="163"/>
-      <c r="C44" s="295">
+      <c r="C44" s="305">
         <v>55</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -12004,10 +12057,10 @@
       <c r="P44" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S44" s="304">
+      <c r="S44" s="298">
         <v>25</v>
       </c>
-      <c r="T44" s="295">
+      <c r="T44" s="305">
         <v>55</v>
       </c>
       <c r="U44" s="9" t="s">
@@ -12016,7 +12069,7 @@
       <c r="V44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="W44" s="298" t="s">
+      <c r="W44" s="300" t="s">
         <v>105</v>
       </c>
       <c r="X44" s="83" t="s">
@@ -12045,10 +12098,10 @@
       <c r="AG44" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="AJ44" s="304">
+      <c r="AJ44" s="298">
         <v>50</v>
       </c>
-      <c r="AK44" s="295">
+      <c r="AK44" s="305">
         <v>10</v>
       </c>
       <c r="AL44" s="190"/>
@@ -12058,7 +12111,7 @@
       <c r="AN44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO44" s="298" t="s">
+      <c r="AO44" s="300" t="s">
         <v>105</v>
       </c>
       <c r="AP44" s="83" t="s">
@@ -12088,7 +12141,7 @@
         <v>168</v>
       </c>
       <c r="AZ44" s="49"/>
-      <c r="BD44" s="304">
+      <c r="BD44" s="298">
         <v>50</v>
       </c>
       <c r="BE44" s="208"/>
@@ -12099,7 +12152,7 @@
       <c r="BH44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI44" s="298" t="s">
+      <c r="BI44" s="300" t="s">
         <v>105</v>
       </c>
       <c r="BJ44" s="83" t="s">
@@ -12128,7 +12181,7 @@
       <c r="BS44" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW44" s="304">
+      <c r="BW44" s="298">
         <v>25</v>
       </c>
       <c r="BX44" s="208"/>
@@ -12139,7 +12192,7 @@
       <c r="CA44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB44" s="298" t="s">
+      <c r="CB44" s="300" t="s">
         <v>105</v>
       </c>
       <c r="CC44" s="83" t="s">
@@ -12171,7 +12224,7 @@
     </row>
     <row r="45" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="140"/>
-      <c r="C45" s="296"/>
+      <c r="C45" s="306"/>
       <c r="D45" s="9" t="s">
         <v>71</v>
       </c>
@@ -12205,15 +12258,15 @@
       <c r="P45" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S45" s="305"/>
-      <c r="T45" s="297"/>
+      <c r="S45" s="299"/>
+      <c r="T45" s="307"/>
       <c r="U45" s="9" t="s">
         <v>71</v>
       </c>
       <c r="V45" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="W45" s="299"/>
+      <c r="W45" s="301"/>
       <c r="X45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12240,8 +12293,8 @@
       <c r="AG45" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="AJ45" s="305"/>
-      <c r="AK45" s="297"/>
+      <c r="AJ45" s="299"/>
+      <c r="AK45" s="307"/>
       <c r="AL45" s="191"/>
       <c r="AM45" s="9" t="s">
         <v>71</v>
@@ -12249,7 +12302,7 @@
       <c r="AN45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO45" s="299"/>
+      <c r="AO45" s="301"/>
       <c r="AP45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12277,7 +12330,7 @@
         <v>168</v>
       </c>
       <c r="AZ45" s="49"/>
-      <c r="BD45" s="305"/>
+      <c r="BD45" s="299"/>
       <c r="BE45" s="165">
         <v>20</v>
       </c>
@@ -12288,7 +12341,7 @@
       <c r="BH45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI45" s="299"/>
+      <c r="BI45" s="301"/>
       <c r="BJ45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12315,7 +12368,7 @@
       <c r="BS45" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW45" s="305"/>
+      <c r="BW45" s="299"/>
       <c r="BX45" s="165"/>
       <c r="BY45" s="191"/>
       <c r="BZ45" s="9" t="s">
@@ -12324,7 +12377,7 @@
       <c r="CA45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB45" s="299"/>
+      <c r="CB45" s="301"/>
       <c r="CC45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12354,7 +12407,7 @@
     </row>
     <row r="46" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="165"/>
-      <c r="C46" s="297"/>
+      <c r="C46" s="307"/>
       <c r="D46" s="9" t="s">
         <v>81</v>
       </c>
@@ -12781,10 +12834,10 @@
       </c>
     </row>
     <row r="48" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="262" t="s">
+      <c r="B48" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="263"/>
+      <c r="C48" s="264"/>
       <c r="D48" s="9">
         <f>SUM(B40:C47)</f>
         <v>200</v>
@@ -12803,10 +12856,10 @@
       <c r="N48" s="65"/>
       <c r="O48" s="65"/>
       <c r="P48" s="168"/>
-      <c r="S48" s="262" t="s">
+      <c r="S48" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="T48" s="263"/>
+      <c r="T48" s="264"/>
       <c r="U48" s="9">
         <f>SUM(S40:T47)</f>
         <v>296</v>
@@ -12959,11 +13012,11 @@
       <c r="AN49" s="25"/>
       <c r="AO49" s="119"/>
       <c r="AP49" s="119"/>
-      <c r="AQ49" s="300"/>
+      <c r="AQ49" s="302"/>
       <c r="AS49" s="192"/>
       <c r="AT49" s="2"/>
-      <c r="AU49" s="256"/>
-      <c r="AV49" s="257"/>
+      <c r="AU49" s="257"/>
+      <c r="AV49" s="258"/>
       <c r="AW49" s="1"/>
       <c r="AX49" s="1"/>
       <c r="AY49" s="24"/>
@@ -12975,11 +13028,11 @@
       <c r="BH49" s="25"/>
       <c r="BI49" s="119"/>
       <c r="BJ49" s="119"/>
-      <c r="BK49" s="300"/>
+      <c r="BK49" s="302"/>
       <c r="BM49" s="192"/>
       <c r="BN49" s="2"/>
-      <c r="BO49" s="256"/>
-      <c r="BP49" s="257"/>
+      <c r="BO49" s="257"/>
+      <c r="BP49" s="258"/>
       <c r="BQ49" s="1"/>
       <c r="BR49" s="1"/>
       <c r="BS49" s="46"/>
@@ -12990,20 +13043,20 @@
       <c r="CA49" s="25"/>
       <c r="CB49" s="119"/>
       <c r="CC49" s="119"/>
-      <c r="CD49" s="300"/>
+      <c r="CD49" s="302"/>
       <c r="CF49" s="192"/>
       <c r="CG49" s="2"/>
-      <c r="CH49" s="256"/>
-      <c r="CI49" s="257"/>
+      <c r="CH49" s="257"/>
+      <c r="CI49" s="258"/>
       <c r="CJ49" s="1"/>
       <c r="CK49" s="1"/>
       <c r="CL49" s="46"/>
     </row>
     <row r="50" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AJ50" s="262" t="s">
+      <c r="AJ50" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="AK50" s="263"/>
+      <c r="AK50" s="264"/>
       <c r="AL50" s="189" t="s">
         <v>179</v>
       </c>
@@ -13014,19 +13067,19 @@
       <c r="AN50" s="25"/>
       <c r="AO50" s="119"/>
       <c r="AP50" s="119"/>
-      <c r="AQ50" s="300"/>
+      <c r="AQ50" s="302"/>
       <c r="AS50" s="192"/>
       <c r="AT50" s="2"/>
-      <c r="AU50" s="256"/>
-      <c r="AV50" s="257"/>
+      <c r="AU50" s="257"/>
+      <c r="AV50" s="258"/>
       <c r="AW50" s="1"/>
       <c r="AX50" s="1"/>
       <c r="AY50" s="24"/>
       <c r="AZ50" s="49"/>
-      <c r="BD50" s="262" t="s">
+      <c r="BD50" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="BE50" s="263"/>
+      <c r="BE50" s="264"/>
       <c r="BF50" s="189"/>
       <c r="BG50" s="9">
         <f>SUM(BD40:BF48)</f>
@@ -13035,18 +13088,18 @@
       <c r="BH50" s="25"/>
       <c r="BI50" s="119"/>
       <c r="BJ50" s="119"/>
-      <c r="BK50" s="300"/>
+      <c r="BK50" s="302"/>
       <c r="BM50" s="192"/>
       <c r="BN50" s="2"/>
-      <c r="BO50" s="256"/>
-      <c r="BP50" s="257"/>
+      <c r="BO50" s="257"/>
+      <c r="BP50" s="258"/>
       <c r="BQ50" s="1"/>
       <c r="BR50" s="1"/>
       <c r="BS50" s="46"/>
-      <c r="BW50" s="262" t="s">
+      <c r="BW50" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="BX50" s="263"/>
+      <c r="BX50" s="264"/>
       <c r="BY50" s="189"/>
       <c r="BZ50" s="9">
         <f>SUM(BW40:BY48)</f>
@@ -13055,21 +13108,21 @@
       <c r="CA50" s="25"/>
       <c r="CB50" s="119"/>
       <c r="CC50" s="119"/>
-      <c r="CD50" s="300"/>
+      <c r="CD50" s="302"/>
       <c r="CF50" s="192"/>
       <c r="CG50" s="2"/>
-      <c r="CH50" s="256"/>
-      <c r="CI50" s="257"/>
+      <c r="CH50" s="257"/>
+      <c r="CI50" s="258"/>
       <c r="CJ50" s="1"/>
       <c r="CK50" s="1"/>
       <c r="CL50" s="46"/>
     </row>
     <row r="51" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="264" t="s">
+      <c r="B51" s="265" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="265"/>
-      <c r="D51" s="266"/>
+      <c r="C51" s="266"/>
+      <c r="D51" s="267"/>
       <c r="E51" s="26" t="s">
         <v>43</v>
       </c>
@@ -13119,14 +13172,14 @@
       <c r="AN51" s="114"/>
       <c r="AO51" s="201"/>
       <c r="AP51" s="202"/>
-      <c r="AQ51" s="301"/>
+      <c r="AQ51" s="303"/>
       <c r="AR51" s="201"/>
       <c r="AS51" s="203"/>
       <c r="AT51" s="116" t="s">
         <v>160</v>
       </c>
-      <c r="AU51" s="302"/>
-      <c r="AV51" s="303"/>
+      <c r="AU51" s="304"/>
+      <c r="AV51" s="297"/>
       <c r="AW51" s="65"/>
       <c r="AX51" s="65"/>
       <c r="AY51" s="115"/>
@@ -13138,14 +13191,14 @@
       <c r="BH51" s="114"/>
       <c r="BI51" s="201"/>
       <c r="BJ51" s="202"/>
-      <c r="BK51" s="301"/>
+      <c r="BK51" s="303"/>
       <c r="BL51" s="201"/>
       <c r="BM51" s="203"/>
       <c r="BN51" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="BO51" s="302"/>
-      <c r="BP51" s="303"/>
+      <c r="BO51" s="304"/>
+      <c r="BP51" s="297"/>
       <c r="BQ51" s="65"/>
       <c r="BR51" s="65"/>
       <c r="BS51" s="168"/>
@@ -13156,14 +13209,14 @@
       <c r="CA51" s="114"/>
       <c r="CB51" s="201"/>
       <c r="CC51" s="202"/>
-      <c r="CD51" s="301"/>
+      <c r="CD51" s="303"/>
       <c r="CE51" s="201"/>
       <c r="CF51" s="203" t="s">
         <v>180</v>
       </c>
       <c r="CG51" s="79"/>
-      <c r="CH51" s="302"/>
-      <c r="CI51" s="303"/>
+      <c r="CH51" s="304"/>
+      <c r="CI51" s="297"/>
       <c r="CJ51" s="65"/>
       <c r="CK51" s="65"/>
       <c r="CL51" s="168"/>
@@ -13184,11 +13237,11 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="46"/>
-      <c r="V52" s="264" t="s">
+      <c r="V52" s="265" t="s">
         <v>145</v>
       </c>
-      <c r="W52" s="265"/>
-      <c r="X52" s="266"/>
+      <c r="W52" s="266"/>
+      <c r="X52" s="267"/>
       <c r="Y52" s="26" t="s">
         <v>43</v>
       </c>
@@ -13290,11 +13343,11 @@
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
       <c r="AL53" s="46"/>
-      <c r="AO53" s="264" t="s">
+      <c r="AO53" s="265" t="s">
         <v>145</v>
       </c>
-      <c r="AP53" s="265"/>
-      <c r="AQ53" s="266"/>
+      <c r="AP53" s="266"/>
+      <c r="AQ53" s="267"/>
       <c r="AR53" s="26" t="s">
         <v>43</v>
       </c>
@@ -13341,11 +13394,11 @@
         <f ca="1">TODAY()</f>
         <v>45292</v>
       </c>
-      <c r="BJ53" s="264" t="s">
+      <c r="BJ53" s="265" t="s">
         <v>145</v>
       </c>
-      <c r="BK53" s="265"/>
-      <c r="BL53" s="266"/>
+      <c r="BK53" s="266"/>
+      <c r="BL53" s="267"/>
       <c r="BM53" s="26" t="s">
         <v>43</v>
       </c>
@@ -15394,10 +15447,10 @@
       </c>
     </row>
     <row r="66" spans="2:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="262" t="s">
+      <c r="B66" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="C66" s="263"/>
+      <c r="C66" s="264"/>
       <c r="D66" s="189"/>
       <c r="E66" s="9">
         <f>SUM(B53:D64)</f>
@@ -15410,8 +15463,8 @@
       <c r="J66" s="117"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="256"/>
-      <c r="O66" s="257"/>
+      <c r="N66" s="257"/>
+      <c r="O66" s="258"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
       <c r="R66" s="46"/>
@@ -15494,18 +15547,18 @@
       <c r="G67" s="119"/>
       <c r="H67" s="216"/>
       <c r="I67" s="119"/>
-      <c r="J67" s="255"/>
+      <c r="J67" s="256"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="256"/>
-      <c r="O67" s="257"/>
+      <c r="N67" s="257"/>
+      <c r="O67" s="258"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
       <c r="R67" s="46"/>
-      <c r="V67" s="262" t="s">
+      <c r="V67" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="W67" s="263"/>
+      <c r="W67" s="264"/>
       <c r="X67" s="189"/>
       <c r="Y67" s="9">
         <f>SUM(V54:X65)</f>
@@ -15517,8 +15570,8 @@
       <c r="AC67" s="119"/>
       <c r="AD67" s="117"/>
       <c r="AG67" s="2"/>
-      <c r="AH67" s="256"/>
-      <c r="AI67" s="257"/>
+      <c r="AH67" s="257"/>
+      <c r="AI67" s="258"/>
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
       <c r="AL67" s="46"/>
@@ -15560,7 +15613,7 @@
       <c r="G68" s="137"/>
       <c r="H68" s="203"/>
       <c r="I68" s="137"/>
-      <c r="J68" s="306"/>
+      <c r="J68" s="296"/>
       <c r="K68" s="50"/>
       <c r="L68" s="79"/>
       <c r="M68" s="79"/>
@@ -15576,17 +15629,17 @@
       <c r="AA68" s="119"/>
       <c r="AB68" s="216"/>
       <c r="AC68" s="119"/>
-      <c r="AD68" s="255"/>
+      <c r="AD68" s="256"/>
       <c r="AG68" s="2"/>
-      <c r="AH68" s="256"/>
-      <c r="AI68" s="257"/>
+      <c r="AH68" s="257"/>
+      <c r="AI68" s="258"/>
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
       <c r="AL68" s="46"/>
-      <c r="AO68" s="262" t="s">
+      <c r="AO68" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="AP68" s="263"/>
+      <c r="AP68" s="264"/>
       <c r="AQ68" s="189"/>
       <c r="AR68" s="9">
         <f>SUM(AO55:AQ66)</f>
@@ -15598,15 +15651,15 @@
       <c r="AV68" s="119"/>
       <c r="AW68" s="117"/>
       <c r="AZ68" s="2"/>
-      <c r="BA68" s="256"/>
-      <c r="BB68" s="257"/>
+      <c r="BA68" s="257"/>
+      <c r="BB68" s="258"/>
       <c r="BC68" s="1"/>
       <c r="BD68" s="1"/>
       <c r="BE68" s="46"/>
-      <c r="BJ68" s="262" t="s">
+      <c r="BJ68" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="BK68" s="263"/>
+      <c r="BK68" s="264"/>
       <c r="BL68" s="189"/>
       <c r="BM68" s="9">
         <f>SUM(BJ55:BL66)</f>
@@ -15618,8 +15671,8 @@
       <c r="BQ68" s="119"/>
       <c r="BR68" s="117"/>
       <c r="BU68" s="2"/>
-      <c r="BV68" s="256"/>
-      <c r="BW68" s="257"/>
+      <c r="BV68" s="257"/>
+      <c r="BW68" s="258"/>
       <c r="BX68" s="1"/>
       <c r="BY68" s="1"/>
       <c r="BZ68" s="46"/>
@@ -15635,7 +15688,7 @@
       <c r="AC69" s="137" t="s">
         <v>184</v>
       </c>
-      <c r="AD69" s="306"/>
+      <c r="AD69" s="296"/>
       <c r="AE69" s="50"/>
       <c r="AF69" s="50"/>
       <c r="AG69" s="79"/>
@@ -15651,10 +15704,10 @@
       <c r="AT69" s="119"/>
       <c r="AU69" s="192"/>
       <c r="AV69" s="119"/>
-      <c r="AW69" s="255"/>
+      <c r="AW69" s="256"/>
       <c r="AZ69" s="2"/>
-      <c r="BA69" s="256"/>
-      <c r="BB69" s="257"/>
+      <c r="BA69" s="257"/>
+      <c r="BB69" s="258"/>
       <c r="BC69" s="1"/>
       <c r="BD69" s="1"/>
       <c r="BE69" s="46"/>
@@ -15665,10 +15718,10 @@
       <c r="BO69" s="119"/>
       <c r="BP69" s="192"/>
       <c r="BQ69" s="119"/>
-      <c r="BR69" s="255"/>
+      <c r="BR69" s="256"/>
       <c r="BU69" s="2"/>
-      <c r="BV69" s="256"/>
-      <c r="BW69" s="257"/>
+      <c r="BV69" s="257"/>
+      <c r="BW69" s="258"/>
       <c r="BX69" s="1"/>
       <c r="BY69" s="1"/>
       <c r="BZ69" s="46"/>
@@ -15681,7 +15734,7 @@
       <c r="AT70" s="117"/>
       <c r="AU70" s="192"/>
       <c r="AV70" s="119"/>
-      <c r="AW70" s="255"/>
+      <c r="AW70" s="256"/>
       <c r="AZ70" s="2"/>
       <c r="BA70" s="152"/>
       <c r="BB70" s="1"/>
@@ -15695,7 +15748,7 @@
       <c r="BO70" s="117"/>
       <c r="BP70" s="192"/>
       <c r="BQ70" s="119"/>
-      <c r="BR70" s="255"/>
+      <c r="BR70" s="256"/>
       <c r="BU70" s="2"/>
       <c r="BV70" s="152"/>
       <c r="BW70" s="1"/>
@@ -15743,40 +15796,22 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="BJ53:BL53"/>
-    <mergeCell ref="BJ68:BK68"/>
-    <mergeCell ref="BV68:BV69"/>
-    <mergeCell ref="BW68:BW69"/>
-    <mergeCell ref="BR69:BR70"/>
-    <mergeCell ref="AO53:AQ53"/>
-    <mergeCell ref="AO68:AP68"/>
-    <mergeCell ref="BA68:BA69"/>
-    <mergeCell ref="BB68:BB69"/>
-    <mergeCell ref="AW69:AW70"/>
-    <mergeCell ref="V52:X52"/>
-    <mergeCell ref="V67:W67"/>
-    <mergeCell ref="AH67:AH68"/>
-    <mergeCell ref="AI67:AI68"/>
-    <mergeCell ref="AD68:AD69"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="N66:N67"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="CI49:CI51"/>
-    <mergeCell ref="BW50:BX50"/>
-    <mergeCell ref="BW38:BY38"/>
-    <mergeCell ref="BW44:BW45"/>
-    <mergeCell ref="CB44:CB45"/>
-    <mergeCell ref="CD49:CD51"/>
-    <mergeCell ref="CH49:CH51"/>
-    <mergeCell ref="BP49:BP51"/>
-    <mergeCell ref="BD50:BE50"/>
-    <mergeCell ref="BD38:BF38"/>
-    <mergeCell ref="BD44:BD45"/>
-    <mergeCell ref="BI44:BI45"/>
-    <mergeCell ref="BK49:BK51"/>
-    <mergeCell ref="BO49:BO51"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="AO44:AO45"/>
+    <mergeCell ref="AQ49:AQ51"/>
+    <mergeCell ref="AU49:AU51"/>
+    <mergeCell ref="AV49:AV51"/>
+    <mergeCell ref="AJ50:AK50"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="S44:S45"/>
+    <mergeCell ref="T44:T45"/>
+    <mergeCell ref="W44:W45"/>
+    <mergeCell ref="AJ38:AL38"/>
+    <mergeCell ref="AJ44:AJ45"/>
+    <mergeCell ref="AK44:AK45"/>
     <mergeCell ref="BR24:BS24"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B36:C36"/>
@@ -15792,22 +15827,40 @@
     <mergeCell ref="BM36:BN36"/>
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="AQ49:AQ51"/>
-    <mergeCell ref="AU49:AU51"/>
-    <mergeCell ref="AV49:AV51"/>
-    <mergeCell ref="AJ50:AK50"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="S44:S45"/>
-    <mergeCell ref="T44:T45"/>
-    <mergeCell ref="W44:W45"/>
-    <mergeCell ref="AJ38:AL38"/>
-    <mergeCell ref="AJ44:AJ45"/>
-    <mergeCell ref="AK44:AK45"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="AO44:AO45"/>
+    <mergeCell ref="BP49:BP51"/>
+    <mergeCell ref="BD50:BE50"/>
+    <mergeCell ref="BD38:BF38"/>
+    <mergeCell ref="BD44:BD45"/>
+    <mergeCell ref="BI44:BI45"/>
+    <mergeCell ref="BK49:BK51"/>
+    <mergeCell ref="BO49:BO51"/>
+    <mergeCell ref="CI49:CI51"/>
+    <mergeCell ref="BW50:BX50"/>
+    <mergeCell ref="BW38:BY38"/>
+    <mergeCell ref="BW44:BW45"/>
+    <mergeCell ref="CB44:CB45"/>
+    <mergeCell ref="CD49:CD51"/>
+    <mergeCell ref="CH49:CH51"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="N66:N67"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="J67:J68"/>
+    <mergeCell ref="V52:X52"/>
+    <mergeCell ref="V67:W67"/>
+    <mergeCell ref="AH67:AH68"/>
+    <mergeCell ref="AI67:AI68"/>
+    <mergeCell ref="AD68:AD69"/>
+    <mergeCell ref="AO53:AQ53"/>
+    <mergeCell ref="AO68:AP68"/>
+    <mergeCell ref="BA68:BA69"/>
+    <mergeCell ref="BB68:BB69"/>
+    <mergeCell ref="AW69:AW70"/>
+    <mergeCell ref="BJ53:BL53"/>
+    <mergeCell ref="BJ68:BK68"/>
+    <mergeCell ref="BV68:BV69"/>
+    <mergeCell ref="BW68:BW69"/>
+    <mergeCell ref="BR69:BR70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.1.1 _10:35PM
Rw Usage Updates S.1.0.1.1 _10:35PM
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.9.xlsx
+++ b/Usage_S_1.0.9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7C6DB4-0965-423E-AEC4-87BED4D729D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BCB33F-902C-4B9D-A2B8-1F350AE49C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1764,7 +1764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="313">
+  <cellXfs count="312">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2384,6 +2384,9 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2444,6 +2447,54 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2468,61 +2519,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2536,27 +2545,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2847,8 +2846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2886,7 +2885,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z1" s="268" t="s">
+      <c r="Z1" s="269" t="s">
         <v>250</v>
       </c>
       <c r="AA1" s="36" t="s">
@@ -2901,12 +2900,12 @@
       <c r="AD1" s="249" t="s">
         <v>224</v>
       </c>
-      <c r="AF1" s="253" t="s">
+      <c r="AF1" s="254" t="s">
         <v>241</v>
       </c>
-      <c r="AG1" s="254"/>
-      <c r="AH1" s="254"/>
-      <c r="AI1" s="255"/>
+      <c r="AG1" s="255"/>
+      <c r="AH1" s="255"/>
+      <c r="AI1" s="256"/>
     </row>
     <row r="2" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -2915,15 +2914,15 @@
       <c r="B2" s="34">
         <v>40.380000000000003</v>
       </c>
-      <c r="C2" s="261">
+      <c r="C2" s="262">
         <f>B3+B4</f>
         <v>0</v>
       </c>
-      <c r="E2" s="265" t="s">
+      <c r="E2" s="266" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="266"/>
-      <c r="G2" s="267"/>
+      <c r="F2" s="267"/>
+      <c r="G2" s="268"/>
       <c r="H2" s="26" t="s">
         <v>43</v>
       </c>
@@ -2973,7 +2972,7 @@
       <c r="Y2" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="Z2" s="269"/>
+      <c r="Z2" s="270"/>
       <c r="AA2" s="36">
         <f>SUM(AA3:AA19)</f>
         <v>6</v>
@@ -3002,13 +3001,13 @@
       <c r="AI2" s="8"/>
     </row>
     <row r="3" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="259" t="s">
+      <c r="A3" s="260" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="34">
         <v>0</v>
       </c>
-      <c r="C3" s="262"/>
+      <c r="C3" s="263"/>
       <c r="D3" s="162" t="s">
         <v>36</v>
       </c>
@@ -3021,15 +3020,15 @@
       <c r="AA3" s="238">
         <v>1</v>
       </c>
-      <c r="AB3" s="312"/>
+      <c r="AB3" s="253"/>
       <c r="AC3" s="59">
         <v>4</v>
       </c>
       <c r="AD3" s="44"/>
-      <c r="AE3" s="270"/>
+      <c r="AE3" s="271"/>
     </row>
     <row r="4" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="260"/>
+      <c r="A4" s="261"/>
       <c r="B4" s="34">
         <v>0</v>
       </c>
@@ -3098,7 +3097,7 @@
       <c r="AD4" s="240">
         <v>3</v>
       </c>
-      <c r="AE4" s="271"/>
+      <c r="AE4" s="272"/>
       <c r="AF4" s="25" t="s">
         <v>181</v>
       </c>
@@ -3171,7 +3170,7 @@
       <c r="AD5" s="240">
         <v>3</v>
       </c>
-      <c r="AE5" s="271"/>
+      <c r="AE5" s="272"/>
       <c r="AF5" s="25" t="s">
         <v>30</v>
       </c>
@@ -3184,10 +3183,10 @@
     </row>
     <row r="6" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
-        <v>3332</v>
+        <v>3572</v>
       </c>
       <c r="C6">
-        <v>5633</v>
+        <v>5393</v>
       </c>
       <c r="E6" s="218"/>
       <c r="F6" s="207"/>
@@ -3246,7 +3245,7 @@
         <v>1</v>
       </c>
       <c r="AD6" s="49"/>
-      <c r="AE6" s="271"/>
+      <c r="AE6" s="272"/>
       <c r="AF6" s="25"/>
       <c r="AH6" s="24"/>
     </row>
@@ -3319,7 +3318,7 @@
         <v>4</v>
       </c>
       <c r="AD7" s="49"/>
-      <c r="AE7" s="271"/>
+      <c r="AE7" s="272"/>
       <c r="AF7" s="25"/>
       <c r="AG7" s="25" t="s">
         <v>46</v>
@@ -3385,7 +3384,7 @@
         <v>4</v>
       </c>
       <c r="AD8" s="49"/>
-      <c r="AE8" s="271"/>
+      <c r="AE8" s="272"/>
       <c r="AF8" s="25"/>
       <c r="AG8" s="25"/>
       <c r="AH8" s="24" t="s">
@@ -3398,7 +3397,7 @@
       </c>
       <c r="B9" s="8">
         <f>7000+B6+B5-C2</f>
-        <v>10332</v>
+        <v>10572</v>
       </c>
       <c r="E9" s="163"/>
       <c r="F9" s="165">
@@ -3455,7 +3454,7 @@
         <v>1</v>
       </c>
       <c r="AD9" s="49"/>
-      <c r="AE9" s="271"/>
+      <c r="AE9" s="272"/>
       <c r="AF9" s="25"/>
       <c r="AH9" s="24"/>
     </row>
@@ -3514,7 +3513,7 @@
       <c r="AD10" s="49">
         <v>1</v>
       </c>
-      <c r="AE10" s="271"/>
+      <c r="AE10" s="272"/>
       <c r="AF10" s="25" t="s">
         <v>66</v>
       </c>
@@ -3597,7 +3596,7 @@
         <v>5</v>
       </c>
       <c r="AD11" s="49"/>
-      <c r="AE11" s="271"/>
+      <c r="AE11" s="272"/>
       <c r="AF11" s="25" t="s">
         <v>261</v>
       </c>
@@ -3613,7 +3612,9 @@
       <c r="F12" s="205">
         <v>200</v>
       </c>
-      <c r="G12" s="164"/>
+      <c r="G12" s="164">
+        <v>1</v>
+      </c>
       <c r="H12" s="28" t="s">
         <v>128</v>
       </c>
@@ -3640,11 +3641,11 @@
         <v>181</v>
       </c>
       <c r="Q12" s="154">
-        <v>0.64583333333333337</v>
+        <v>0.94097222222222221</v>
       </c>
       <c r="R12" s="24"/>
       <c r="S12" s="154">
-        <v>0.64583333333333337</v>
+        <v>0.94097222222222221</v>
       </c>
       <c r="T12" s="238">
         <v>3</v>
@@ -3667,7 +3668,7 @@
       <c r="AD12" s="49">
         <v>1</v>
       </c>
-      <c r="AE12" s="271"/>
+      <c r="AE12" s="272"/>
       <c r="AF12" s="25" t="s">
         <v>65</v>
       </c>
@@ -3684,7 +3685,7 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>10332</v>
+        <v>10572</v>
       </c>
       <c r="E13" s="36"/>
       <c r="F13" s="206">
@@ -3743,7 +3744,7 @@
         <v>2</v>
       </c>
       <c r="AD13" s="49"/>
-      <c r="AE13" s="271"/>
+      <c r="AE13" s="272"/>
       <c r="AF13" s="25"/>
       <c r="AG13" s="25"/>
       <c r="AH13" s="24"/>
@@ -3751,7 +3752,9 @@
     <row r="14" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="165"/>
+      <c r="E14" s="165">
+        <v>239</v>
+      </c>
       <c r="F14" s="205">
         <v>10</v>
       </c>
@@ -3784,11 +3787,11 @@
         <v>29</v>
       </c>
       <c r="Q14" s="154">
-        <v>0.64583333333333337</v>
+        <v>0.94097222222222221</v>
       </c>
       <c r="R14"/>
       <c r="S14" s="154">
-        <v>0.91666666666666663</v>
+        <v>0.94097222222222221</v>
       </c>
       <c r="T14" s="252">
         <v>2</v>
@@ -3811,7 +3814,7 @@
       <c r="AD14" s="49">
         <v>1</v>
       </c>
-      <c r="AE14" s="271"/>
+      <c r="AE14" s="272"/>
       <c r="AF14" s="25" t="s">
         <v>65</v>
       </c>
@@ -3871,7 +3874,7 @@
         <v>1</v>
       </c>
       <c r="AD15" s="49"/>
-      <c r="AE15" s="271"/>
+      <c r="AE15" s="272"/>
       <c r="AF15" s="25"/>
       <c r="AG15" s="25" t="s">
         <v>46</v>
@@ -3897,28 +3900,28 @@
         <v>4</v>
       </c>
       <c r="AD16" s="49"/>
-      <c r="AE16" s="271"/>
+      <c r="AE16" s="272"/>
       <c r="AF16" s="25"/>
       <c r="AH16" s="24"/>
     </row>
     <row r="17" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="263" t="s">
+      <c r="E17" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="264"/>
+      <c r="F17" s="265"/>
       <c r="G17" s="189"/>
       <c r="H17" s="9">
         <f>SUM(E4:G15)</f>
-        <v>445</v>
+        <v>685</v>
       </c>
       <c r="I17" s="26"/>
       <c r="J17" s="119"/>
       <c r="K17" s="216"/>
       <c r="L17" s="119"/>
-      <c r="Q17" s="257"/>
-      <c r="R17" s="258"/>
+      <c r="Q17" s="258"/>
+      <c r="R17" s="259"/>
       <c r="Y17" s="25" t="s">
         <v>245</v>
       </c>
@@ -3931,7 +3934,7 @@
       </c>
       <c r="AC17" s="65"/>
       <c r="AD17" s="51"/>
-      <c r="AE17" s="271"/>
+      <c r="AE17" s="272"/>
       <c r="AF17" s="25" t="s">
         <v>65</v>
       </c>
@@ -3957,9 +3960,9 @@
       <c r="I18" s="226"/>
       <c r="J18" s="119"/>
       <c r="L18" s="119"/>
-      <c r="M18" s="256"/>
-      <c r="Q18" s="257"/>
-      <c r="R18" s="258"/>
+      <c r="M18" s="257"/>
+      <c r="Q18" s="258"/>
+      <c r="R18" s="259"/>
       <c r="Y18" s="25" t="s">
         <v>245</v>
       </c>
@@ -3972,7 +3975,7 @@
       <c r="AD18" s="49">
         <v>2</v>
       </c>
-      <c r="AE18" s="271"/>
+      <c r="AE18" s="272"/>
       <c r="AF18" s="25" t="s">
         <v>30</v>
       </c>
@@ -3986,7 +3989,7 @@
     <row r="19" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I19" s="226"/>
       <c r="L19" s="119"/>
-      <c r="M19" s="256"/>
+      <c r="M19" s="257"/>
       <c r="Y19" s="25" t="s">
         <v>245</v>
       </c>
@@ -4001,7 +4004,7 @@
       <c r="AD19" s="51">
         <v>2</v>
       </c>
-      <c r="AE19" s="272"/>
+      <c r="AE19" s="273"/>
       <c r="AF19" s="25" t="s">
         <v>243</v>
       </c>
@@ -4039,7 +4042,7 @@
   <dimension ref="A1:T59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4063,18 +4066,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="273" t="s">
+      <c r="E1" s="290" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="275"/>
+      <c r="F1" s="292"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="273" t="s">
+      <c r="H1" s="290" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="274"/>
-      <c r="J1" s="275"/>
+      <c r="I1" s="291"/>
+      <c r="J1" s="292"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -4092,7 +4095,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="276">
+      <c r="B2" s="293">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -4119,26 +4122,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="279">
+      <c r="K2" s="296">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="294">
+      <c r="L2" s="287">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="284">
+      <c r="M2" s="277">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
         <f>SUM(E2:J59)</f>
-        <v>10292</v>
+        <v>10532</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="277"/>
+      <c r="B3" s="294"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -4153,13 +4156,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="280"/>
-      <c r="L3" s="295"/>
-      <c r="M3" s="285"/>
+      <c r="K3" s="297"/>
+      <c r="L3" s="288"/>
+      <c r="M3" s="278"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="278"/>
+      <c r="B4" s="295"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -4174,9 +4177,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="280"/>
-      <c r="L4" s="295"/>
-      <c r="M4" s="285"/>
+      <c r="K4" s="297"/>
+      <c r="L4" s="288"/>
+      <c r="M4" s="278"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -4258,7 +4261,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="286">
+      <c r="B7" s="279">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -4275,22 +4278,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="288">
+      <c r="K7" s="281">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="290">
+      <c r="L7" s="283">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="292">
+      <c r="M7" s="285">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="287"/>
+      <c r="B8" s="280"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -4311,9 +4314,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="289"/>
-      <c r="L8" s="291"/>
-      <c r="M8" s="293"/>
+      <c r="K8" s="282"/>
+      <c r="L8" s="284"/>
+      <c r="M8" s="286"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -4393,7 +4396,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="286">
+      <c r="B11" s="279">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -4420,7 +4423,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="287"/>
+      <c r="B12" s="280"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -4477,7 +4480,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="286">
+      <c r="B14" s="279">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -4500,7 +4503,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="287"/>
+      <c r="B15" s="280"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -4524,7 +4527,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="276">
+      <c r="B16" s="293">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -4555,7 +4558,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="277"/>
+      <c r="B17" s="294"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -4573,7 +4576,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="276">
+      <c r="B18" s="293">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -4602,7 +4605,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="278"/>
+      <c r="B19" s="295"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -4662,7 +4665,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="282">
+      <c r="B21" s="298">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -4690,7 +4693,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="283"/>
+      <c r="B22" s="299"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -4742,7 +4745,7 @@
       <c r="M23" s="70"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="261">
+      <c r="B24" s="262">
         <v>16</v>
       </c>
       <c r="C24" s="141"/>
@@ -4771,7 +4774,7 @@
       <c r="A25" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="262"/>
+      <c r="B25" s="263"/>
       <c r="C25" s="142"/>
       <c r="D25" s="18">
         <v>130</v>
@@ -4799,7 +4802,7 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="261">
+      <c r="B26" s="262">
         <v>17</v>
       </c>
       <c r="C26" s="161"/>
@@ -4830,7 +4833,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="281"/>
+      <c r="B27" s="289"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -4861,7 +4864,7 @@
       <c r="A28" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="261">
+      <c r="B28" s="262">
         <v>18</v>
       </c>
       <c r="C28" s="141"/>
@@ -4883,7 +4886,7 @@
       <c r="M28" s="70"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="262"/>
+      <c r="B29" s="263"/>
       <c r="C29" s="142"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18">
@@ -4909,7 +4912,7 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="261">
+      <c r="B30" s="262">
         <v>19</v>
       </c>
       <c r="C30" s="142"/>
@@ -4932,7 +4935,7 @@
       <c r="A31" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="262"/>
+      <c r="B31" s="263"/>
       <c r="C31" s="142"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -4959,7 +4962,7 @@
       <c r="A32" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="261">
+      <c r="B32" s="262">
         <v>20</v>
       </c>
       <c r="C32" s="142"/>
@@ -4981,7 +4984,7 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="262"/>
+      <c r="B33" s="263"/>
       <c r="C33" s="142"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -5034,7 +5037,7 @@
       <c r="M34" s="82"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="261">
+      <c r="B35" s="262">
         <v>22</v>
       </c>
       <c r="C35" s="96"/>
@@ -5061,7 +5064,7 @@
       <c r="A36" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="262"/>
+      <c r="B36" s="263"/>
       <c r="C36" s="142"/>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -5083,7 +5086,7 @@
       <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="261">
+      <c r="B37" s="262">
         <v>23</v>
       </c>
       <c r="C37" s="142"/>
@@ -5116,7 +5119,7 @@
       <c r="A38" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="262"/>
+      <c r="B38" s="263"/>
       <c r="C38" s="96"/>
       <c r="D38" s="82"/>
       <c r="E38" s="82"/>
@@ -5134,7 +5137,7 @@
       <c r="M38" s="82"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="261">
+      <c r="B39" s="262">
         <v>24</v>
       </c>
       <c r="C39" s="142"/>
@@ -5161,7 +5164,7 @@
       <c r="A40" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="281"/>
+      <c r="B40" s="289"/>
       <c r="C40" s="96"/>
       <c r="D40" s="82">
         <v>210</v>
@@ -5189,7 +5192,7 @@
       <c r="M40" s="82"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="261">
+      <c r="B41" s="262">
         <v>25</v>
       </c>
       <c r="C41" s="142"/>
@@ -5216,7 +5219,7 @@
       <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="281"/>
+      <c r="B42" s="289"/>
       <c r="C42" s="142"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -5234,7 +5237,7 @@
       <c r="M42" s="18"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="262"/>
+      <c r="B43" s="263"/>
       <c r="C43" s="142"/>
       <c r="D43" s="18">
         <v>190</v>
@@ -5263,7 +5266,7 @@
       <c r="A44" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="261">
+      <c r="B44" s="262">
         <v>26</v>
       </c>
       <c r="C44" s="142"/>
@@ -5289,7 +5292,7 @@
       <c r="M44" s="18"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="262"/>
+      <c r="B45" s="263"/>
       <c r="C45" s="142"/>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
@@ -5314,7 +5317,7 @@
       <c r="A46" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="261">
+      <c r="B46" s="262">
         <v>27</v>
       </c>
       <c r="C46" s="142"/>
@@ -5336,7 +5339,7 @@
       <c r="M46" s="18"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="281"/>
+      <c r="B47" s="289"/>
       <c r="C47" s="211"/>
       <c r="D47" s="132"/>
       <c r="E47" s="132"/>
@@ -5357,7 +5360,7 @@
       <c r="A48" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="261">
+      <c r="B48" s="262">
         <v>28</v>
       </c>
       <c r="C48" s="142"/>
@@ -5377,7 +5380,7 @@
       <c r="M48" s="18"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="281"/>
+      <c r="B49" s="289"/>
       <c r="C49" s="142"/>
       <c r="D49" s="18">
         <v>175</v>
@@ -5403,7 +5406,7 @@
       <c r="M49" s="18"/>
     </row>
     <row r="50" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="281"/>
+      <c r="B50" s="289"/>
       <c r="C50" s="96"/>
       <c r="D50" s="82"/>
       <c r="E50" s="82"/>
@@ -5430,7 +5433,7 @@
       <c r="A51" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="261">
+      <c r="B51" s="262">
         <v>29</v>
       </c>
       <c r="C51" s="142"/>
@@ -5452,7 +5455,7 @@
       <c r="M51" s="18"/>
     </row>
     <row r="52" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="262"/>
+      <c r="B52" s="263"/>
       <c r="C52" s="142"/>
       <c r="D52" s="18">
         <v>190</v>
@@ -5485,7 +5488,7 @@
       <c r="A53" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="261">
+      <c r="B53" s="262">
         <v>30</v>
       </c>
       <c r="C53" s="142"/>
@@ -5515,7 +5518,7 @@
       <c r="T53" s="49"/>
     </row>
     <row r="54" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="281"/>
+      <c r="B54" s="289"/>
       <c r="C54" s="96"/>
       <c r="D54" s="82"/>
       <c r="E54" s="82"/>
@@ -5542,7 +5545,7 @@
       <c r="A55" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B55" s="261">
+      <c r="B55" s="262">
         <v>31</v>
       </c>
       <c r="C55" s="96"/>
@@ -5570,7 +5573,7 @@
       <c r="M55" s="82"/>
     </row>
     <row r="56" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="262"/>
+      <c r="B56" s="263"/>
       <c r="C56" s="96"/>
       <c r="D56" s="82"/>
       <c r="E56" s="82">
@@ -5596,7 +5599,7 @@
       <c r="M56" s="82"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B57" s="309">
+      <c r="B57" s="274">
         <v>1</v>
       </c>
       <c r="C57" s="142"/>
@@ -5616,14 +5619,18 @@
       <c r="M57" s="18"/>
     </row>
     <row r="58" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="310"/>
+      <c r="B58" s="275"/>
       <c r="C58" s="142"/>
       <c r="D58" s="18"/>
       <c r="E58" s="18">
         <v>200</v>
       </c>
-      <c r="F58" s="18"/>
-      <c r="G58" s="18"/>
+      <c r="F58" s="18">
+        <v>239</v>
+      </c>
+      <c r="G58" s="18">
+        <v>1</v>
+      </c>
       <c r="H58" s="18">
         <v>20</v>
       </c>
@@ -5641,25 +5648,25 @@
       <c r="A59" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="311"/>
+      <c r="B59" s="276"/>
       <c r="C59" s="142"/>
       <c r="D59" s="18"/>
-      <c r="E59" s="308">
+      <c r="E59" s="18">
         <v>15</v>
       </c>
       <c r="F59" s="18">
         <v>40</v>
       </c>
-      <c r="G59" s="308">
+      <c r="G59" s="18">
         <v>20</v>
       </c>
-      <c r="H59" s="308">
+      <c r="H59" s="18">
         <v>20</v>
       </c>
-      <c r="I59" s="308">
+      <c r="I59" s="18">
         <v>20</v>
       </c>
-      <c r="J59" s="308">
+      <c r="J59" s="18">
         <v>25</v>
       </c>
       <c r="K59" s="18"/>
@@ -5668,6 +5675,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B35:B36"/>
     <mergeCell ref="B57:B59"/>
     <mergeCell ref="B55:B56"/>
     <mergeCell ref="B37:B38"/>
@@ -5684,21 +5706,6 @@
     <mergeCell ref="B46:B47"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="B53:B54"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B35:B36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8905,10 +8912,10 @@
       <c r="CG23" s="49"/>
     </row>
     <row r="24" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AG24" s="263" t="s">
+      <c r="AG24" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="AH24" s="264"/>
+      <c r="AH24" s="265"/>
       <c r="AI24" s="9">
         <f>SUM(AG16:AH23)</f>
         <v>40</v>
@@ -8928,10 +8935,10 @@
       <c r="AV24" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AZ24" s="263" t="s">
+      <c r="AZ24" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="BA24" s="264"/>
+      <c r="BA24" s="265"/>
       <c r="BB24" s="9">
         <f>SUM(AZ16:BA23)</f>
         <v>335</v>
@@ -8951,10 +8958,10 @@
       <c r="BO24" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="BR24" s="263" t="s">
+      <c r="BR24" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="BS24" s="264"/>
+      <c r="BS24" s="265"/>
       <c r="BT24" s="9">
         <f>SUM(BR16:BS23)</f>
         <v>275</v>
@@ -8977,10 +8984,10 @@
     </row>
     <row r="25" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="265" t="s">
+      <c r="B26" s="266" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="267"/>
+      <c r="C26" s="268"/>
       <c r="D26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9017,10 +9024,10 @@
       <c r="O26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="R26" s="265" t="s">
+      <c r="R26" s="266" t="s">
         <v>145</v>
       </c>
-      <c r="S26" s="267"/>
+      <c r="S26" s="268"/>
       <c r="T26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9057,10 +9064,10 @@
       <c r="AE26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AG26" s="265" t="s">
+      <c r="AG26" s="266" t="s">
         <v>145</v>
       </c>
-      <c r="AH26" s="267"/>
+      <c r="AH26" s="268"/>
       <c r="AI26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9097,10 +9104,10 @@
       <c r="AT26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AW26" s="265" t="s">
+      <c r="AW26" s="266" t="s">
         <v>145</v>
       </c>
-      <c r="AX26" s="267"/>
+      <c r="AX26" s="268"/>
       <c r="AY26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9137,10 +9144,10 @@
       <c r="BJ26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="BM26" s="265" t="s">
+      <c r="BM26" s="266" t="s">
         <v>145</v>
       </c>
-      <c r="BN26" s="267"/>
+      <c r="BN26" s="268"/>
       <c r="BO26" s="26" t="s">
         <v>43</v>
       </c>
@@ -10134,7 +10141,7 @@
       <c r="AW32" s="163">
         <v>25</v>
       </c>
-      <c r="AX32" s="305">
+      <c r="AX32" s="300">
         <v>70</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -10172,7 +10179,7 @@
       <c r="BM32" s="163">
         <v>50</v>
       </c>
-      <c r="BN32" s="305">
+      <c r="BN32" s="300">
         <v>20</v>
       </c>
       <c r="BO32" s="9" t="s">
@@ -10321,7 +10328,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="163"/>
-      <c r="AX33" s="306"/>
+      <c r="AX33" s="301"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -10357,7 +10364,7 @@
       <c r="BM33" s="140">
         <v>10</v>
       </c>
-      <c r="BN33" s="306"/>
+      <c r="BN33" s="301"/>
       <c r="BO33" s="9" t="s">
         <v>71</v>
       </c>
@@ -10508,7 +10515,7 @@
         <v>148</v>
       </c>
       <c r="AW34" s="140"/>
-      <c r="AX34" s="307"/>
+      <c r="AX34" s="302"/>
       <c r="AY34" s="9" t="s">
         <v>81</v>
       </c>
@@ -10546,7 +10553,7 @@
       <c r="BM34" s="165">
         <v>70</v>
       </c>
-      <c r="BN34" s="307"/>
+      <c r="BN34" s="302"/>
       <c r="BO34" s="9" t="s">
         <v>81</v>
       </c>
@@ -10777,10 +10784,10 @@
       </c>
     </row>
     <row r="36" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="263" t="s">
+      <c r="B36" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="264"/>
+      <c r="C36" s="265"/>
       <c r="D36" s="9">
         <f>SUM(B28:C35)</f>
         <v>512</v>
@@ -10798,10 +10805,10 @@
       <c r="M36" s="65"/>
       <c r="N36" s="65"/>
       <c r="O36" s="102"/>
-      <c r="R36" s="263" t="s">
+      <c r="R36" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="S36" s="264"/>
+      <c r="S36" s="265"/>
       <c r="T36" s="9">
         <f>SUM(R28:S35)</f>
         <v>182</v>
@@ -10819,10 +10826,10 @@
       <c r="AC36" s="65"/>
       <c r="AD36" s="65"/>
       <c r="AE36" s="102"/>
-      <c r="AG36" s="263" t="s">
+      <c r="AG36" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="AH36" s="264"/>
+      <c r="AH36" s="265"/>
       <c r="AI36" s="9">
         <f>SUM(AG28:AH35)</f>
         <v>360</v>
@@ -10840,10 +10847,10 @@
       <c r="AR36" s="65"/>
       <c r="AS36" s="65"/>
       <c r="AT36" s="102"/>
-      <c r="AW36" s="263" t="s">
+      <c r="AW36" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="AX36" s="264"/>
+      <c r="AX36" s="265"/>
       <c r="AY36" s="9">
         <f>SUM(AW28:AX35)</f>
         <v>200</v>
@@ -10861,10 +10868,10 @@
       <c r="BH36" s="65"/>
       <c r="BI36" s="65"/>
       <c r="BJ36" s="102"/>
-      <c r="BM36" s="263" t="s">
+      <c r="BM36" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="BN36" s="264"/>
+      <c r="BN36" s="265"/>
       <c r="BO36" s="9">
         <f>SUM(BM28:BN35)</f>
         <v>260</v>
@@ -10884,10 +10891,10 @@
     </row>
     <row r="37" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="265" t="s">
+      <c r="B38" s="266" t="s">
         <v>145</v>
       </c>
-      <c r="C38" s="267"/>
+      <c r="C38" s="268"/>
       <c r="D38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10927,10 +10934,10 @@
       <c r="P38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="S38" s="265" t="s">
+      <c r="S38" s="266" t="s">
         <v>145</v>
       </c>
-      <c r="T38" s="267"/>
+      <c r="T38" s="268"/>
       <c r="U38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10970,11 +10977,11 @@
       <c r="AG38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="AJ38" s="265" t="s">
+      <c r="AJ38" s="266" t="s">
         <v>145</v>
       </c>
-      <c r="AK38" s="266"/>
-      <c r="AL38" s="267"/>
+      <c r="AK38" s="267"/>
+      <c r="AL38" s="268"/>
       <c r="AM38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11019,11 +11026,11 @@
         <f ca="1">TODAY()</f>
         <v>45292</v>
       </c>
-      <c r="BD38" s="265" t="s">
+      <c r="BD38" s="266" t="s">
         <v>145</v>
       </c>
-      <c r="BE38" s="266"/>
-      <c r="BF38" s="267"/>
+      <c r="BE38" s="267"/>
+      <c r="BF38" s="268"/>
       <c r="BG38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11063,11 +11070,11 @@
       <c r="BS38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="BW38" s="265" t="s">
+      <c r="BW38" s="266" t="s">
         <v>145</v>
       </c>
-      <c r="BX38" s="266"/>
-      <c r="BY38" s="267"/>
+      <c r="BX38" s="267"/>
+      <c r="BY38" s="268"/>
       <c r="BZ38" s="26" t="s">
         <v>43</v>
       </c>
@@ -12019,7 +12026,7 @@
     </row>
     <row r="44" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="163"/>
-      <c r="C44" s="305">
+      <c r="C44" s="300">
         <v>55</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -12057,10 +12064,10 @@
       <c r="P44" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S44" s="298">
+      <c r="S44" s="309">
         <v>25</v>
       </c>
-      <c r="T44" s="305">
+      <c r="T44" s="300">
         <v>55</v>
       </c>
       <c r="U44" s="9" t="s">
@@ -12069,7 +12076,7 @@
       <c r="V44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="W44" s="300" t="s">
+      <c r="W44" s="303" t="s">
         <v>105</v>
       </c>
       <c r="X44" s="83" t="s">
@@ -12098,10 +12105,10 @@
       <c r="AG44" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="AJ44" s="298">
+      <c r="AJ44" s="309">
         <v>50</v>
       </c>
-      <c r="AK44" s="305">
+      <c r="AK44" s="300">
         <v>10</v>
       </c>
       <c r="AL44" s="190"/>
@@ -12111,7 +12118,7 @@
       <c r="AN44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO44" s="300" t="s">
+      <c r="AO44" s="303" t="s">
         <v>105</v>
       </c>
       <c r="AP44" s="83" t="s">
@@ -12141,7 +12148,7 @@
         <v>168</v>
       </c>
       <c r="AZ44" s="49"/>
-      <c r="BD44" s="298">
+      <c r="BD44" s="309">
         <v>50</v>
       </c>
       <c r="BE44" s="208"/>
@@ -12152,7 +12159,7 @@
       <c r="BH44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI44" s="300" t="s">
+      <c r="BI44" s="303" t="s">
         <v>105</v>
       </c>
       <c r="BJ44" s="83" t="s">
@@ -12181,7 +12188,7 @@
       <c r="BS44" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW44" s="298">
+      <c r="BW44" s="309">
         <v>25</v>
       </c>
       <c r="BX44" s="208"/>
@@ -12192,7 +12199,7 @@
       <c r="CA44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB44" s="300" t="s">
+      <c r="CB44" s="303" t="s">
         <v>105</v>
       </c>
       <c r="CC44" s="83" t="s">
@@ -12224,7 +12231,7 @@
     </row>
     <row r="45" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="140"/>
-      <c r="C45" s="306"/>
+      <c r="C45" s="301"/>
       <c r="D45" s="9" t="s">
         <v>71</v>
       </c>
@@ -12258,15 +12265,15 @@
       <c r="P45" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S45" s="299"/>
-      <c r="T45" s="307"/>
+      <c r="S45" s="310"/>
+      <c r="T45" s="302"/>
       <c r="U45" s="9" t="s">
         <v>71</v>
       </c>
       <c r="V45" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="W45" s="301"/>
+      <c r="W45" s="304"/>
       <c r="X45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12293,8 +12300,8 @@
       <c r="AG45" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="AJ45" s="299"/>
-      <c r="AK45" s="307"/>
+      <c r="AJ45" s="310"/>
+      <c r="AK45" s="302"/>
       <c r="AL45" s="191"/>
       <c r="AM45" s="9" t="s">
         <v>71</v>
@@ -12302,7 +12309,7 @@
       <c r="AN45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO45" s="301"/>
+      <c r="AO45" s="304"/>
       <c r="AP45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12330,7 +12337,7 @@
         <v>168</v>
       </c>
       <c r="AZ45" s="49"/>
-      <c r="BD45" s="299"/>
+      <c r="BD45" s="310"/>
       <c r="BE45" s="165">
         <v>20</v>
       </c>
@@ -12341,7 +12348,7 @@
       <c r="BH45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI45" s="301"/>
+      <c r="BI45" s="304"/>
       <c r="BJ45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12368,7 +12375,7 @@
       <c r="BS45" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW45" s="299"/>
+      <c r="BW45" s="310"/>
       <c r="BX45" s="165"/>
       <c r="BY45" s="191"/>
       <c r="BZ45" s="9" t="s">
@@ -12377,7 +12384,7 @@
       <c r="CA45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB45" s="301"/>
+      <c r="CB45" s="304"/>
       <c r="CC45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12407,7 +12414,7 @@
     </row>
     <row r="46" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="165"/>
-      <c r="C46" s="307"/>
+      <c r="C46" s="302"/>
       <c r="D46" s="9" t="s">
         <v>81</v>
       </c>
@@ -12834,10 +12841,10 @@
       </c>
     </row>
     <row r="48" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="263" t="s">
+      <c r="B48" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="264"/>
+      <c r="C48" s="265"/>
       <c r="D48" s="9">
         <f>SUM(B40:C47)</f>
         <v>200</v>
@@ -12856,10 +12863,10 @@
       <c r="N48" s="65"/>
       <c r="O48" s="65"/>
       <c r="P48" s="168"/>
-      <c r="S48" s="263" t="s">
+      <c r="S48" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="T48" s="264"/>
+      <c r="T48" s="265"/>
       <c r="U48" s="9">
         <f>SUM(S40:T47)</f>
         <v>296</v>
@@ -13012,11 +13019,11 @@
       <c r="AN49" s="25"/>
       <c r="AO49" s="119"/>
       <c r="AP49" s="119"/>
-      <c r="AQ49" s="302"/>
+      <c r="AQ49" s="305"/>
       <c r="AS49" s="192"/>
       <c r="AT49" s="2"/>
-      <c r="AU49" s="257"/>
-      <c r="AV49" s="258"/>
+      <c r="AU49" s="258"/>
+      <c r="AV49" s="259"/>
       <c r="AW49" s="1"/>
       <c r="AX49" s="1"/>
       <c r="AY49" s="24"/>
@@ -13028,11 +13035,11 @@
       <c r="BH49" s="25"/>
       <c r="BI49" s="119"/>
       <c r="BJ49" s="119"/>
-      <c r="BK49" s="302"/>
+      <c r="BK49" s="305"/>
       <c r="BM49" s="192"/>
       <c r="BN49" s="2"/>
-      <c r="BO49" s="257"/>
-      <c r="BP49" s="258"/>
+      <c r="BO49" s="258"/>
+      <c r="BP49" s="259"/>
       <c r="BQ49" s="1"/>
       <c r="BR49" s="1"/>
       <c r="BS49" s="46"/>
@@ -13043,20 +13050,20 @@
       <c r="CA49" s="25"/>
       <c r="CB49" s="119"/>
       <c r="CC49" s="119"/>
-      <c r="CD49" s="302"/>
+      <c r="CD49" s="305"/>
       <c r="CF49" s="192"/>
       <c r="CG49" s="2"/>
-      <c r="CH49" s="257"/>
-      <c r="CI49" s="258"/>
+      <c r="CH49" s="258"/>
+      <c r="CI49" s="259"/>
       <c r="CJ49" s="1"/>
       <c r="CK49" s="1"/>
       <c r="CL49" s="46"/>
     </row>
     <row r="50" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AJ50" s="263" t="s">
+      <c r="AJ50" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="AK50" s="264"/>
+      <c r="AK50" s="265"/>
       <c r="AL50" s="189" t="s">
         <v>179</v>
       </c>
@@ -13067,19 +13074,19 @@
       <c r="AN50" s="25"/>
       <c r="AO50" s="119"/>
       <c r="AP50" s="119"/>
-      <c r="AQ50" s="302"/>
+      <c r="AQ50" s="305"/>
       <c r="AS50" s="192"/>
       <c r="AT50" s="2"/>
-      <c r="AU50" s="257"/>
-      <c r="AV50" s="258"/>
+      <c r="AU50" s="258"/>
+      <c r="AV50" s="259"/>
       <c r="AW50" s="1"/>
       <c r="AX50" s="1"/>
       <c r="AY50" s="24"/>
       <c r="AZ50" s="49"/>
-      <c r="BD50" s="263" t="s">
+      <c r="BD50" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="BE50" s="264"/>
+      <c r="BE50" s="265"/>
       <c r="BF50" s="189"/>
       <c r="BG50" s="9">
         <f>SUM(BD40:BF48)</f>
@@ -13088,18 +13095,18 @@
       <c r="BH50" s="25"/>
       <c r="BI50" s="119"/>
       <c r="BJ50" s="119"/>
-      <c r="BK50" s="302"/>
+      <c r="BK50" s="305"/>
       <c r="BM50" s="192"/>
       <c r="BN50" s="2"/>
-      <c r="BO50" s="257"/>
-      <c r="BP50" s="258"/>
+      <c r="BO50" s="258"/>
+      <c r="BP50" s="259"/>
       <c r="BQ50" s="1"/>
       <c r="BR50" s="1"/>
       <c r="BS50" s="46"/>
-      <c r="BW50" s="263" t="s">
+      <c r="BW50" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="BX50" s="264"/>
+      <c r="BX50" s="265"/>
       <c r="BY50" s="189"/>
       <c r="BZ50" s="9">
         <f>SUM(BW40:BY48)</f>
@@ -13108,21 +13115,21 @@
       <c r="CA50" s="25"/>
       <c r="CB50" s="119"/>
       <c r="CC50" s="119"/>
-      <c r="CD50" s="302"/>
+      <c r="CD50" s="305"/>
       <c r="CF50" s="192"/>
       <c r="CG50" s="2"/>
-      <c r="CH50" s="257"/>
-      <c r="CI50" s="258"/>
+      <c r="CH50" s="258"/>
+      <c r="CI50" s="259"/>
       <c r="CJ50" s="1"/>
       <c r="CK50" s="1"/>
       <c r="CL50" s="46"/>
     </row>
     <row r="51" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="265" t="s">
+      <c r="B51" s="266" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="266"/>
-      <c r="D51" s="267"/>
+      <c r="C51" s="267"/>
+      <c r="D51" s="268"/>
       <c r="E51" s="26" t="s">
         <v>43</v>
       </c>
@@ -13172,14 +13179,14 @@
       <c r="AN51" s="114"/>
       <c r="AO51" s="201"/>
       <c r="AP51" s="202"/>
-      <c r="AQ51" s="303"/>
+      <c r="AQ51" s="306"/>
       <c r="AR51" s="201"/>
       <c r="AS51" s="203"/>
       <c r="AT51" s="116" t="s">
         <v>160</v>
       </c>
-      <c r="AU51" s="304"/>
-      <c r="AV51" s="297"/>
+      <c r="AU51" s="307"/>
+      <c r="AV51" s="308"/>
       <c r="AW51" s="65"/>
       <c r="AX51" s="65"/>
       <c r="AY51" s="115"/>
@@ -13191,14 +13198,14 @@
       <c r="BH51" s="114"/>
       <c r="BI51" s="201"/>
       <c r="BJ51" s="202"/>
-      <c r="BK51" s="303"/>
+      <c r="BK51" s="306"/>
       <c r="BL51" s="201"/>
       <c r="BM51" s="203"/>
       <c r="BN51" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="BO51" s="304"/>
-      <c r="BP51" s="297"/>
+      <c r="BO51" s="307"/>
+      <c r="BP51" s="308"/>
       <c r="BQ51" s="65"/>
       <c r="BR51" s="65"/>
       <c r="BS51" s="168"/>
@@ -13209,14 +13216,14 @@
       <c r="CA51" s="114"/>
       <c r="CB51" s="201"/>
       <c r="CC51" s="202"/>
-      <c r="CD51" s="303"/>
+      <c r="CD51" s="306"/>
       <c r="CE51" s="201"/>
       <c r="CF51" s="203" t="s">
         <v>180</v>
       </c>
       <c r="CG51" s="79"/>
-      <c r="CH51" s="304"/>
-      <c r="CI51" s="297"/>
+      <c r="CH51" s="307"/>
+      <c r="CI51" s="308"/>
       <c r="CJ51" s="65"/>
       <c r="CK51" s="65"/>
       <c r="CL51" s="168"/>
@@ -13237,11 +13244,11 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="46"/>
-      <c r="V52" s="265" t="s">
+      <c r="V52" s="266" t="s">
         <v>145</v>
       </c>
-      <c r="W52" s="266"/>
-      <c r="X52" s="267"/>
+      <c r="W52" s="267"/>
+      <c r="X52" s="268"/>
       <c r="Y52" s="26" t="s">
         <v>43</v>
       </c>
@@ -13343,11 +13350,11 @@
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
       <c r="AL53" s="46"/>
-      <c r="AO53" s="265" t="s">
+      <c r="AO53" s="266" t="s">
         <v>145</v>
       </c>
-      <c r="AP53" s="266"/>
-      <c r="AQ53" s="267"/>
+      <c r="AP53" s="267"/>
+      <c r="AQ53" s="268"/>
       <c r="AR53" s="26" t="s">
         <v>43</v>
       </c>
@@ -13394,11 +13401,11 @@
         <f ca="1">TODAY()</f>
         <v>45292</v>
       </c>
-      <c r="BJ53" s="265" t="s">
+      <c r="BJ53" s="266" t="s">
         <v>145</v>
       </c>
-      <c r="BK53" s="266"/>
-      <c r="BL53" s="267"/>
+      <c r="BK53" s="267"/>
+      <c r="BL53" s="268"/>
       <c r="BM53" s="26" t="s">
         <v>43</v>
       </c>
@@ -15447,10 +15454,10 @@
       </c>
     </row>
     <row r="66" spans="2:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="263" t="s">
+      <c r="B66" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="C66" s="264"/>
+      <c r="C66" s="265"/>
       <c r="D66" s="189"/>
       <c r="E66" s="9">
         <f>SUM(B53:D64)</f>
@@ -15463,8 +15470,8 @@
       <c r="J66" s="117"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="257"/>
-      <c r="O66" s="258"/>
+      <c r="N66" s="258"/>
+      <c r="O66" s="259"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
       <c r="R66" s="46"/>
@@ -15547,18 +15554,18 @@
       <c r="G67" s="119"/>
       <c r="H67" s="216"/>
       <c r="I67" s="119"/>
-      <c r="J67" s="256"/>
+      <c r="J67" s="257"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="257"/>
-      <c r="O67" s="258"/>
+      <c r="N67" s="258"/>
+      <c r="O67" s="259"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
       <c r="R67" s="46"/>
-      <c r="V67" s="263" t="s">
+      <c r="V67" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="W67" s="264"/>
+      <c r="W67" s="265"/>
       <c r="X67" s="189"/>
       <c r="Y67" s="9">
         <f>SUM(V54:X65)</f>
@@ -15570,8 +15577,8 @@
       <c r="AC67" s="119"/>
       <c r="AD67" s="117"/>
       <c r="AG67" s="2"/>
-      <c r="AH67" s="257"/>
-      <c r="AI67" s="258"/>
+      <c r="AH67" s="258"/>
+      <c r="AI67" s="259"/>
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
       <c r="AL67" s="46"/>
@@ -15613,7 +15620,7 @@
       <c r="G68" s="137"/>
       <c r="H68" s="203"/>
       <c r="I68" s="137"/>
-      <c r="J68" s="296"/>
+      <c r="J68" s="311"/>
       <c r="K68" s="50"/>
       <c r="L68" s="79"/>
       <c r="M68" s="79"/>
@@ -15629,17 +15636,17 @@
       <c r="AA68" s="119"/>
       <c r="AB68" s="216"/>
       <c r="AC68" s="119"/>
-      <c r="AD68" s="256"/>
+      <c r="AD68" s="257"/>
       <c r="AG68" s="2"/>
-      <c r="AH68" s="257"/>
-      <c r="AI68" s="258"/>
+      <c r="AH68" s="258"/>
+      <c r="AI68" s="259"/>
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
       <c r="AL68" s="46"/>
-      <c r="AO68" s="263" t="s">
+      <c r="AO68" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="AP68" s="264"/>
+      <c r="AP68" s="265"/>
       <c r="AQ68" s="189"/>
       <c r="AR68" s="9">
         <f>SUM(AO55:AQ66)</f>
@@ -15651,15 +15658,15 @@
       <c r="AV68" s="119"/>
       <c r="AW68" s="117"/>
       <c r="AZ68" s="2"/>
-      <c r="BA68" s="257"/>
-      <c r="BB68" s="258"/>
+      <c r="BA68" s="258"/>
+      <c r="BB68" s="259"/>
       <c r="BC68" s="1"/>
       <c r="BD68" s="1"/>
       <c r="BE68" s="46"/>
-      <c r="BJ68" s="263" t="s">
+      <c r="BJ68" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="BK68" s="264"/>
+      <c r="BK68" s="265"/>
       <c r="BL68" s="189"/>
       <c r="BM68" s="9">
         <f>SUM(BJ55:BL66)</f>
@@ -15671,8 +15678,8 @@
       <c r="BQ68" s="119"/>
       <c r="BR68" s="117"/>
       <c r="BU68" s="2"/>
-      <c r="BV68" s="257"/>
-      <c r="BW68" s="258"/>
+      <c r="BV68" s="258"/>
+      <c r="BW68" s="259"/>
       <c r="BX68" s="1"/>
       <c r="BY68" s="1"/>
       <c r="BZ68" s="46"/>
@@ -15688,7 +15695,7 @@
       <c r="AC69" s="137" t="s">
         <v>184</v>
       </c>
-      <c r="AD69" s="296"/>
+      <c r="AD69" s="311"/>
       <c r="AE69" s="50"/>
       <c r="AF69" s="50"/>
       <c r="AG69" s="79"/>
@@ -15704,10 +15711,10 @@
       <c r="AT69" s="119"/>
       <c r="AU69" s="192"/>
       <c r="AV69" s="119"/>
-      <c r="AW69" s="256"/>
+      <c r="AW69" s="257"/>
       <c r="AZ69" s="2"/>
-      <c r="BA69" s="257"/>
-      <c r="BB69" s="258"/>
+      <c r="BA69" s="258"/>
+      <c r="BB69" s="259"/>
       <c r="BC69" s="1"/>
       <c r="BD69" s="1"/>
       <c r="BE69" s="46"/>
@@ -15718,10 +15725,10 @@
       <c r="BO69" s="119"/>
       <c r="BP69" s="192"/>
       <c r="BQ69" s="119"/>
-      <c r="BR69" s="256"/>
+      <c r="BR69" s="257"/>
       <c r="BU69" s="2"/>
-      <c r="BV69" s="257"/>
-      <c r="BW69" s="258"/>
+      <c r="BV69" s="258"/>
+      <c r="BW69" s="259"/>
       <c r="BX69" s="1"/>
       <c r="BY69" s="1"/>
       <c r="BZ69" s="46"/>
@@ -15734,7 +15741,7 @@
       <c r="AT70" s="117"/>
       <c r="AU70" s="192"/>
       <c r="AV70" s="119"/>
-      <c r="AW70" s="256"/>
+      <c r="AW70" s="257"/>
       <c r="AZ70" s="2"/>
       <c r="BA70" s="152"/>
       <c r="BB70" s="1"/>
@@ -15748,7 +15755,7 @@
       <c r="BO70" s="117"/>
       <c r="BP70" s="192"/>
       <c r="BQ70" s="119"/>
-      <c r="BR70" s="256"/>
+      <c r="BR70" s="257"/>
       <c r="BU70" s="2"/>
       <c r="BV70" s="152"/>
       <c r="BW70" s="1"/>
@@ -15796,22 +15803,40 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="AO44:AO45"/>
-    <mergeCell ref="AQ49:AQ51"/>
-    <mergeCell ref="AU49:AU51"/>
-    <mergeCell ref="AV49:AV51"/>
-    <mergeCell ref="AJ50:AK50"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="S44:S45"/>
-    <mergeCell ref="T44:T45"/>
-    <mergeCell ref="W44:W45"/>
-    <mergeCell ref="AJ38:AL38"/>
-    <mergeCell ref="AJ44:AJ45"/>
-    <mergeCell ref="AK44:AK45"/>
+    <mergeCell ref="BJ53:BL53"/>
+    <mergeCell ref="BJ68:BK68"/>
+    <mergeCell ref="BV68:BV69"/>
+    <mergeCell ref="BW68:BW69"/>
+    <mergeCell ref="BR69:BR70"/>
+    <mergeCell ref="AO53:AQ53"/>
+    <mergeCell ref="AO68:AP68"/>
+    <mergeCell ref="BA68:BA69"/>
+    <mergeCell ref="BB68:BB69"/>
+    <mergeCell ref="AW69:AW70"/>
+    <mergeCell ref="V52:X52"/>
+    <mergeCell ref="V67:W67"/>
+    <mergeCell ref="AH67:AH68"/>
+    <mergeCell ref="AI67:AI68"/>
+    <mergeCell ref="AD68:AD69"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="N66:N67"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="J67:J68"/>
+    <mergeCell ref="CI49:CI51"/>
+    <mergeCell ref="BW50:BX50"/>
+    <mergeCell ref="BW38:BY38"/>
+    <mergeCell ref="BW44:BW45"/>
+    <mergeCell ref="CB44:CB45"/>
+    <mergeCell ref="CD49:CD51"/>
+    <mergeCell ref="CH49:CH51"/>
+    <mergeCell ref="BP49:BP51"/>
+    <mergeCell ref="BD50:BE50"/>
+    <mergeCell ref="BD38:BF38"/>
+    <mergeCell ref="BD44:BD45"/>
+    <mergeCell ref="BI44:BI45"/>
+    <mergeCell ref="BK49:BK51"/>
+    <mergeCell ref="BO49:BO51"/>
     <mergeCell ref="BR24:BS24"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B36:C36"/>
@@ -15827,40 +15852,22 @@
     <mergeCell ref="BM36:BN36"/>
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="BP49:BP51"/>
-    <mergeCell ref="BD50:BE50"/>
-    <mergeCell ref="BD38:BF38"/>
-    <mergeCell ref="BD44:BD45"/>
-    <mergeCell ref="BI44:BI45"/>
-    <mergeCell ref="BK49:BK51"/>
-    <mergeCell ref="BO49:BO51"/>
-    <mergeCell ref="CI49:CI51"/>
-    <mergeCell ref="BW50:BX50"/>
-    <mergeCell ref="BW38:BY38"/>
-    <mergeCell ref="BW44:BW45"/>
-    <mergeCell ref="CB44:CB45"/>
-    <mergeCell ref="CD49:CD51"/>
-    <mergeCell ref="CH49:CH51"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="N66:N67"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="V52:X52"/>
-    <mergeCell ref="V67:W67"/>
-    <mergeCell ref="AH67:AH68"/>
-    <mergeCell ref="AI67:AI68"/>
-    <mergeCell ref="AD68:AD69"/>
-    <mergeCell ref="AO53:AQ53"/>
-    <mergeCell ref="AO68:AP68"/>
-    <mergeCell ref="BA68:BA69"/>
-    <mergeCell ref="BB68:BB69"/>
-    <mergeCell ref="AW69:AW70"/>
-    <mergeCell ref="BJ53:BL53"/>
-    <mergeCell ref="BJ68:BK68"/>
-    <mergeCell ref="BV68:BV69"/>
-    <mergeCell ref="BW68:BW69"/>
-    <mergeCell ref="BR69:BR70"/>
+    <mergeCell ref="AQ49:AQ51"/>
+    <mergeCell ref="AU49:AU51"/>
+    <mergeCell ref="AV49:AV51"/>
+    <mergeCell ref="AJ50:AK50"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="S44:S45"/>
+    <mergeCell ref="T44:T45"/>
+    <mergeCell ref="W44:W45"/>
+    <mergeCell ref="AJ38:AL38"/>
+    <mergeCell ref="AJ44:AJ45"/>
+    <mergeCell ref="AK44:AK45"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="AO44:AO45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.1.3 _6:00PM
Boat Enabled -
InCapacity - [17,8,Cnt] , NodeW - [-3] , BirdW - [7] , FuelW_ANoon - [22] , OnHost - [8+1]
VillageW=[1] , [X-MarketShieldMatrix-X] = [5,24,10,9]
Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.9.xlsx
+++ b/Usage_S_1.0.9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54F4735-60C1-4C4C-9748-9497105C3CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F9390A-A59F-4C52-8EC4-966551D996CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2423" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2436" uniqueCount="285">
   <si>
     <t>UnSettled</t>
   </si>
@@ -818,9 +818,6 @@
     <t>X-Professional - (6)-X</t>
   </si>
   <si>
-    <t>X-FuelW(22)  - X</t>
-  </si>
-  <si>
     <t>X-Rathipur-X</t>
   </si>
   <si>
@@ -852,6 +849,48 @@
   </si>
   <si>
     <t>Validity Upto</t>
+  </si>
+  <si>
+    <t>X-MambaF(2)-X</t>
+  </si>
+  <si>
+    <t>X-VillageW(Rathipur)  - X</t>
+  </si>
+  <si>
+    <t>X-FuelW(22)_PM  - X</t>
+  </si>
+  <si>
+    <t>X-FishMP(1)-X</t>
+  </si>
+  <si>
+    <t>X-FuelW(22)_Day  - X</t>
+  </si>
+  <si>
+    <t>X-FuelW(22)_ANoon - X</t>
+  </si>
+  <si>
+    <t>025LB</t>
+  </si>
+  <si>
+    <t>2BR+1PF+1PF</t>
+  </si>
+  <si>
+    <t>Fish-2</t>
+  </si>
+  <si>
+    <t>1Bird+1Star+1dhauli</t>
+  </si>
+  <si>
+    <t>2MHall+Psooty2</t>
+  </si>
+  <si>
+    <t>NI CURD</t>
+  </si>
+  <si>
+    <t>X-Lx1-X</t>
+  </si>
+  <si>
+    <t>1IS+1BR+ToLet2+1ckl+2pp</t>
   </si>
 </sst>
 </file>
@@ -1795,7 +1834,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="321">
+  <cellXfs count="328">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2495,6 +2534,54 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2519,70 +2606,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2596,15 +2635,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2894,8 +2950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2912,7 +2968,7 @@
     <col min="11" max="11" width="22.28515625" style="192" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="117" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="117" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.7109375" style="152" customWidth="1"/>
@@ -2999,13 +3055,13 @@
         <v>92</v>
       </c>
       <c r="Q2" s="153" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R2" s="36" t="s">
         <v>131</v>
       </c>
       <c r="S2" s="156" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="T2" s="214" t="s">
         <v>224</v>
@@ -3031,7 +3087,7 @@
       </c>
       <c r="AC2" s="36">
         <f>SUM(AC3:AC25)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AD2" s="36">
         <f>SUM(AD3:AD25)</f>
@@ -3113,7 +3169,7 @@
         <v>30</v>
       </c>
       <c r="Q4" s="154">
-        <v>0.52083333333333337</v>
+        <v>0.73263888888888884</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>130</v>
@@ -3144,7 +3200,9 @@
       <c r="D5" s="156">
         <v>-2</v>
       </c>
-      <c r="E5" s="218"/>
+      <c r="E5" s="218">
+        <v>10</v>
+      </c>
       <c r="F5" s="206"/>
       <c r="G5" s="127"/>
       <c r="H5" s="9" t="s">
@@ -3156,7 +3214,9 @@
       <c r="J5" s="213" t="s">
         <v>165</v>
       </c>
-      <c r="K5" s="194"/>
+      <c r="K5" s="169" t="s">
+        <v>272</v>
+      </c>
       <c r="L5" s="167" t="s">
         <v>142</v>
       </c>
@@ -3173,7 +3233,7 @@
         <v>86</v>
       </c>
       <c r="Q5" s="154">
-        <v>0.88611111111111107</v>
+        <v>0.73263888888888884</v>
       </c>
       <c r="S5" s="154">
         <v>0.88611111111111107</v>
@@ -3265,7 +3325,9 @@
       <c r="B7" s="29">
         <v>0</v>
       </c>
-      <c r="E7" s="165"/>
+      <c r="E7" s="165">
+        <v>10</v>
+      </c>
       <c r="F7" s="242"/>
       <c r="G7" s="177"/>
       <c r="H7" s="9" t="s">
@@ -3277,7 +3339,9 @@
       <c r="J7" s="83" t="s">
         <v>105</v>
       </c>
-      <c r="K7" s="169"/>
+      <c r="K7" s="169" t="s">
+        <v>276</v>
+      </c>
       <c r="L7" s="83" t="s">
         <v>139</v>
       </c>
@@ -3294,13 +3358,13 @@
         <v>95</v>
       </c>
       <c r="Q7" s="154">
-        <v>0.64583333333333337</v>
+        <v>0.73263888888888884</v>
       </c>
       <c r="S7" s="154">
-        <v>0.88611111111111107</v>
+        <v>0.73263888888888884</v>
       </c>
       <c r="U7" s="245">
-        <v>45293</v>
+        <v>45294</v>
       </c>
       <c r="Y7" s="25" t="s">
         <v>244</v>
@@ -3350,7 +3414,7 @@
         <v>65</v>
       </c>
       <c r="Q8" s="154">
-        <v>0.52083333333333337</v>
+        <v>0.73263888888888884</v>
       </c>
       <c r="S8" s="154">
         <v>0.52083333333333337</v>
@@ -3393,7 +3457,9 @@
         <f>7000+B6+B5-C2</f>
         <v>10682</v>
       </c>
-      <c r="E9" s="163"/>
+      <c r="E9" s="163">
+        <v>14</v>
+      </c>
       <c r="F9" s="165"/>
       <c r="G9" s="177"/>
       <c r="H9" s="9" t="s">
@@ -3422,7 +3488,7 @@
         <v>30</v>
       </c>
       <c r="Q9" s="154">
-        <v>0.64583333333333337</v>
+        <v>0.73263888888888884</v>
       </c>
       <c r="S9" s="154">
         <v>0.64583333333333337</v>
@@ -3462,7 +3528,7 @@
       </c>
       <c r="J10" s="213"/>
       <c r="K10" s="169" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="L10" s="83" t="s">
         <v>143</v>
@@ -3480,7 +3546,7 @@
         <v>66</v>
       </c>
       <c r="Q10" s="154">
-        <v>0.52083333333333337</v>
+        <v>0.73263888888888884</v>
       </c>
       <c r="S10" s="154">
         <v>0.52083333333333337</v>
@@ -3550,7 +3616,7 @@
         <v>161</v>
       </c>
       <c r="Q11" s="154">
-        <v>0.52083333333333337</v>
+        <v>0.73263888888888884</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>126</v>
@@ -3649,7 +3715,9 @@
         <f>B18+Purchase!O2</f>
         <v>10682</v>
       </c>
-      <c r="E13" s="36"/>
+      <c r="E13" s="36">
+        <v>5</v>
+      </c>
       <c r="F13" s="206"/>
       <c r="G13" s="246"/>
       <c r="H13" s="9" t="s">
@@ -3661,7 +3729,9 @@
       <c r="J13" s="228" t="s">
         <v>186</v>
       </c>
-      <c r="K13" s="194"/>
+      <c r="K13" s="194" t="s">
+        <v>274</v>
+      </c>
       <c r="L13" s="183" t="s">
         <v>155</v>
       </c>
@@ -3678,11 +3748,14 @@
         <v>90</v>
       </c>
       <c r="Q13" s="154">
-        <v>0.64583333333333337</v>
+        <v>0.73263888888888884</v>
       </c>
       <c r="R13"/>
       <c r="S13" s="154">
         <v>0.88611111111111107</v>
+      </c>
+      <c r="T13" s="321">
+        <v>1</v>
       </c>
       <c r="U13" s="245">
         <v>45293</v>
@@ -3703,7 +3776,9 @@
     <row r="14" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="165"/>
+      <c r="E14" s="165">
+        <v>1</v>
+      </c>
       <c r="F14" s="205"/>
       <c r="G14" s="127"/>
       <c r="H14" s="9" t="s">
@@ -3713,7 +3788,9 @@
         <v>17</v>
       </c>
       <c r="J14" s="213"/>
-      <c r="K14" s="169"/>
+      <c r="K14" s="194" t="s">
+        <v>271</v>
+      </c>
       <c r="L14" s="83" t="s">
         <v>124</v>
       </c>
@@ -3730,7 +3807,7 @@
         <v>29</v>
       </c>
       <c r="Q14" s="154">
-        <v>0.94097222222222221</v>
+        <v>0.73263888888888884</v>
       </c>
       <c r="R14"/>
       <c r="S14" s="154">
@@ -3842,14 +3919,22 @@
       <c r="G17" s="189"/>
       <c r="H17" s="9">
         <f>SUM(E4:G15)</f>
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="I17" s="26"/>
       <c r="J17" s="119"/>
       <c r="K17" s="254"/>
       <c r="L17" s="255"/>
-      <c r="Q17" s="267"/>
+      <c r="N17" s="326" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q17" s="327" t="s">
+        <v>274</v>
+      </c>
       <c r="R17" s="268"/>
+      <c r="S17" s="24" t="s">
+        <v>279</v>
+      </c>
       <c r="V17" s="261"/>
       <c r="Y17" s="25" t="s">
         <v>244</v>
@@ -3889,7 +3974,10 @@
       </c>
       <c r="L18" s="169"/>
       <c r="M18" s="266"/>
-      <c r="Q18" s="267"/>
+      <c r="N18" s="25" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q18" s="327"/>
       <c r="R18" s="268"/>
       <c r="Y18" s="25" t="s">
         <v>244</v>
@@ -3907,11 +3995,20 @@
     </row>
     <row r="19" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I19" s="226"/>
-      <c r="K19" s="194" t="s">
-        <v>252</v>
-      </c>
+      <c r="K19" s="194"/>
       <c r="L19" s="119"/>
       <c r="M19" s="266"/>
+      <c r="N19" s="25" t="s">
+        <v>278</v>
+      </c>
+      <c r="O19" s="322" t="s">
+        <v>273</v>
+      </c>
+      <c r="P19" s="323"/>
+      <c r="Q19" s="325" t="s">
+        <v>281</v>
+      </c>
+      <c r="R19" s="324"/>
       <c r="Y19" s="25" t="s">
         <v>244</v>
       </c>
@@ -3931,13 +4028,22 @@
     </row>
     <row r="20" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I20" s="227"/>
-      <c r="K20" s="169"/>
+      <c r="K20" s="194"/>
       <c r="L20" s="119"/>
+      <c r="N20" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q20" s="327" t="s">
+        <v>283</v>
+      </c>
+      <c r="S20" s="24" t="s">
+        <v>282</v>
+      </c>
       <c r="Y20" s="25" t="s">
         <v>244</v>
       </c>
       <c r="Z20" s="169" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AA20" s="256"/>
       <c r="AB20" s="260">
@@ -3965,13 +4071,15 @@
         <v>244</v>
       </c>
       <c r="Z21" s="169" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AA21" s="42"/>
       <c r="AB21" s="15">
         <v>2</v>
       </c>
-      <c r="AC21" s="109"/>
+      <c r="AC21" s="109">
+        <v>1</v>
+      </c>
       <c r="AD21" s="44"/>
       <c r="AE21" s="281"/>
       <c r="AF21" s="25" t="s">
@@ -3989,7 +4097,7 @@
         <v>244</v>
       </c>
       <c r="Z22" s="169" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AA22" s="48"/>
       <c r="AB22" s="15">
@@ -4004,7 +4112,7 @@
         <v>30</v>
       </c>
       <c r="AG22" s="25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AH22" s="24" t="s">
         <v>246</v>
@@ -4015,7 +4123,7 @@
         <v>244</v>
       </c>
       <c r="Z23" s="169" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AA23" s="63"/>
       <c r="AB23" s="116">
@@ -4027,7 +4135,7 @@
       </c>
       <c r="AE23" s="281"/>
       <c r="AF23" s="25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AG23" s="25" t="s">
         <v>20</v>
@@ -4041,7 +4149,7 @@
         <v>244</v>
       </c>
       <c r="Z24" s="169" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AA24" s="256"/>
       <c r="AB24" s="260">
@@ -4064,10 +4172,10 @@
     </row>
     <row r="25" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Y25" s="25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Z25" s="169" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AA25" s="256"/>
       <c r="AB25" s="260">
@@ -4087,10 +4195,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="AF1:AI1"/>
     <mergeCell ref="M18:M19"/>
-    <mergeCell ref="Q17:Q18"/>
     <mergeCell ref="R17:R18"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="C2:C3"/>
@@ -4098,6 +4205,8 @@
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="AE3:AE25"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:R19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4133,18 +4242,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="283" t="s">
+      <c r="E1" s="299" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="285"/>
+      <c r="F1" s="301"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="283" t="s">
+      <c r="H1" s="299" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="284"/>
-      <c r="J1" s="285"/>
+      <c r="I1" s="300"/>
+      <c r="J1" s="301"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -4162,7 +4271,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="286">
+      <c r="B2" s="302">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -4189,15 +4298,15 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="289">
+      <c r="K2" s="305">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="307">
+      <c r="L2" s="296">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="297">
+      <c r="M2" s="286">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
@@ -4208,7 +4317,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="287"/>
+      <c r="B3" s="303"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -4223,13 +4332,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="290"/>
-      <c r="L3" s="308"/>
-      <c r="M3" s="298"/>
+      <c r="K3" s="306"/>
+      <c r="L3" s="297"/>
+      <c r="M3" s="287"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="288"/>
+      <c r="B4" s="304"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -4244,9 +4353,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="290"/>
-      <c r="L4" s="308"/>
-      <c r="M4" s="298"/>
+      <c r="K4" s="306"/>
+      <c r="L4" s="297"/>
+      <c r="M4" s="287"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -4328,7 +4437,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="299">
+      <c r="B7" s="288">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -4345,22 +4454,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="301">
+      <c r="K7" s="290">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="303">
+      <c r="L7" s="292">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="305">
+      <c r="M7" s="294">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="300"/>
+      <c r="B8" s="289"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -4381,9 +4490,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="302"/>
-      <c r="L8" s="304"/>
-      <c r="M8" s="306"/>
+      <c r="K8" s="291"/>
+      <c r="L8" s="293"/>
+      <c r="M8" s="295"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -4463,7 +4572,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="299">
+      <c r="B11" s="288">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -4490,7 +4599,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="300"/>
+      <c r="B12" s="289"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -4547,7 +4656,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="299">
+      <c r="B14" s="288">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -4570,7 +4679,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="300"/>
+      <c r="B15" s="289"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -4594,7 +4703,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="286">
+      <c r="B16" s="302">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -4625,7 +4734,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="287"/>
+      <c r="B17" s="303"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -4643,7 +4752,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="286">
+      <c r="B18" s="302">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -4672,7 +4781,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="288"/>
+      <c r="B19" s="304"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -4732,7 +4841,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="292">
+      <c r="B21" s="307">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -4760,7 +4869,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="293"/>
+      <c r="B22" s="308"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -4900,7 +5009,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="291"/>
+      <c r="B27" s="298"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -5231,7 +5340,7 @@
       <c r="A40" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="291"/>
+      <c r="B40" s="298"/>
       <c r="C40" s="96"/>
       <c r="D40" s="82">
         <v>210</v>
@@ -5286,7 +5395,7 @@
       <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="291"/>
+      <c r="B42" s="298"/>
       <c r="C42" s="142"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -5406,7 +5515,7 @@
       <c r="M46" s="18"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="291"/>
+      <c r="B47" s="298"/>
       <c r="C47" s="211"/>
       <c r="D47" s="132"/>
       <c r="E47" s="132"/>
@@ -5447,7 +5556,7 @@
       <c r="M48" s="18"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="291"/>
+      <c r="B49" s="298"/>
       <c r="C49" s="142"/>
       <c r="D49" s="18">
         <v>175</v>
@@ -5473,7 +5582,7 @@
       <c r="M49" s="18"/>
     </row>
     <row r="50" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="291"/>
+      <c r="B50" s="298"/>
       <c r="C50" s="96"/>
       <c r="D50" s="82"/>
       <c r="E50" s="82"/>
@@ -5585,7 +5694,7 @@
       <c r="T53" s="49"/>
     </row>
     <row r="54" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="291"/>
+      <c r="B54" s="298"/>
       <c r="C54" s="96"/>
       <c r="D54" s="82"/>
       <c r="E54" s="82"/>
@@ -5666,7 +5775,7 @@
       <c r="M56" s="82"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B57" s="294">
+      <c r="B57" s="283">
         <v>1</v>
       </c>
       <c r="C57" s="142"/>
@@ -5686,7 +5795,7 @@
       <c r="M57" s="18"/>
     </row>
     <row r="58" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="295"/>
+      <c r="B58" s="284"/>
       <c r="C58" s="142"/>
       <c r="D58" s="18"/>
       <c r="E58" s="18">
@@ -5715,7 +5824,7 @@
       <c r="A59" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="296"/>
+      <c r="B59" s="285"/>
       <c r="C59" s="142"/>
       <c r="D59" s="18"/>
       <c r="E59" s="18">
@@ -5764,6 +5873,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B35:B36"/>
     <mergeCell ref="B57:B59"/>
     <mergeCell ref="B55:B56"/>
     <mergeCell ref="B37:B38"/>
@@ -5780,21 +5904,6 @@
     <mergeCell ref="B46:B47"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="B53:B54"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B35:B36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10230,7 +10339,7 @@
       <c r="AW32" s="163">
         <v>25</v>
       </c>
-      <c r="AX32" s="318">
+      <c r="AX32" s="310">
         <v>70</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -10268,7 +10377,7 @@
       <c r="BM32" s="163">
         <v>50</v>
       </c>
-      <c r="BN32" s="318">
+      <c r="BN32" s="310">
         <v>20</v>
       </c>
       <c r="BO32" s="9" t="s">
@@ -10417,7 +10526,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="163"/>
-      <c r="AX33" s="319"/>
+      <c r="AX33" s="311"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -10453,7 +10562,7 @@
       <c r="BM33" s="140">
         <v>10</v>
       </c>
-      <c r="BN33" s="319"/>
+      <c r="BN33" s="311"/>
       <c r="BO33" s="9" t="s">
         <v>71</v>
       </c>
@@ -10604,7 +10713,7 @@
         <v>148</v>
       </c>
       <c r="AW34" s="140"/>
-      <c r="AX34" s="320"/>
+      <c r="AX34" s="312"/>
       <c r="AY34" s="9" t="s">
         <v>81</v>
       </c>
@@ -10642,7 +10751,7 @@
       <c r="BM34" s="165">
         <v>70</v>
       </c>
-      <c r="BN34" s="320"/>
+      <c r="BN34" s="312"/>
       <c r="BO34" s="9" t="s">
         <v>81</v>
       </c>
@@ -12115,7 +12224,7 @@
     </row>
     <row r="44" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="163"/>
-      <c r="C44" s="318">
+      <c r="C44" s="310">
         <v>55</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -12153,10 +12262,10 @@
       <c r="P44" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S44" s="311">
+      <c r="S44" s="319">
         <v>25</v>
       </c>
-      <c r="T44" s="318">
+      <c r="T44" s="310">
         <v>55</v>
       </c>
       <c r="U44" s="9" t="s">
@@ -12194,10 +12303,10 @@
       <c r="AG44" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="AJ44" s="311">
+      <c r="AJ44" s="319">
         <v>50</v>
       </c>
-      <c r="AK44" s="318">
+      <c r="AK44" s="310">
         <v>10</v>
       </c>
       <c r="AL44" s="190"/>
@@ -12237,7 +12346,7 @@
         <v>168</v>
       </c>
       <c r="AZ44" s="49"/>
-      <c r="BD44" s="311">
+      <c r="BD44" s="319">
         <v>50</v>
       </c>
       <c r="BE44" s="208"/>
@@ -12277,7 +12386,7 @@
       <c r="BS44" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW44" s="311">
+      <c r="BW44" s="319">
         <v>25</v>
       </c>
       <c r="BX44" s="208"/>
@@ -12320,7 +12429,7 @@
     </row>
     <row r="45" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="140"/>
-      <c r="C45" s="319"/>
+      <c r="C45" s="311"/>
       <c r="D45" s="9" t="s">
         <v>71</v>
       </c>
@@ -12354,8 +12463,8 @@
       <c r="P45" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S45" s="312"/>
-      <c r="T45" s="320"/>
+      <c r="S45" s="320"/>
+      <c r="T45" s="312"/>
       <c r="U45" s="9" t="s">
         <v>71</v>
       </c>
@@ -12389,8 +12498,8 @@
       <c r="AG45" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="AJ45" s="312"/>
-      <c r="AK45" s="320"/>
+      <c r="AJ45" s="320"/>
+      <c r="AK45" s="312"/>
       <c r="AL45" s="191"/>
       <c r="AM45" s="9" t="s">
         <v>71</v>
@@ -12426,7 +12535,7 @@
         <v>168</v>
       </c>
       <c r="AZ45" s="49"/>
-      <c r="BD45" s="312"/>
+      <c r="BD45" s="320"/>
       <c r="BE45" s="165">
         <v>20</v>
       </c>
@@ -12464,7 +12573,7 @@
       <c r="BS45" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW45" s="312"/>
+      <c r="BW45" s="320"/>
       <c r="BX45" s="165"/>
       <c r="BY45" s="191"/>
       <c r="BZ45" s="9" t="s">
@@ -12503,7 +12612,7 @@
     </row>
     <row r="46" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="165"/>
-      <c r="C46" s="320"/>
+      <c r="C46" s="312"/>
       <c r="D46" s="9" t="s">
         <v>81</v>
       </c>
@@ -13275,7 +13384,7 @@
         <v>160</v>
       </c>
       <c r="AU51" s="317"/>
-      <c r="AV51" s="310"/>
+      <c r="AV51" s="318"/>
       <c r="AW51" s="65"/>
       <c r="AX51" s="65"/>
       <c r="AY51" s="115"/>
@@ -13294,7 +13403,7 @@
         <v>168</v>
       </c>
       <c r="BO51" s="317"/>
-      <c r="BP51" s="310"/>
+      <c r="BP51" s="318"/>
       <c r="BQ51" s="65"/>
       <c r="BR51" s="65"/>
       <c r="BS51" s="168"/>
@@ -13312,7 +13421,7 @@
       </c>
       <c r="CG51" s="79"/>
       <c r="CH51" s="317"/>
-      <c r="CI51" s="310"/>
+      <c r="CI51" s="318"/>
       <c r="CJ51" s="65"/>
       <c r="CK51" s="65"/>
       <c r="CL51" s="168"/>
@@ -16551,27 +16660,40 @@
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="CC53:CE53"/>
-    <mergeCell ref="CC68:CD68"/>
-    <mergeCell ref="CO68:CO69"/>
-    <mergeCell ref="CP68:CP69"/>
-    <mergeCell ref="CK69:CK70"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="AO44:AO45"/>
-    <mergeCell ref="AQ49:AQ51"/>
-    <mergeCell ref="AU49:AU51"/>
-    <mergeCell ref="AV49:AV51"/>
-    <mergeCell ref="AJ50:AK50"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="S44:S45"/>
-    <mergeCell ref="T44:T45"/>
-    <mergeCell ref="W44:W45"/>
-    <mergeCell ref="AJ38:AL38"/>
-    <mergeCell ref="AJ44:AJ45"/>
-    <mergeCell ref="AK44:AK45"/>
+    <mergeCell ref="BJ53:BL53"/>
+    <mergeCell ref="BJ68:BK68"/>
+    <mergeCell ref="BV68:BV69"/>
+    <mergeCell ref="BW68:BW69"/>
+    <mergeCell ref="BR69:BR70"/>
+    <mergeCell ref="AO53:AQ53"/>
+    <mergeCell ref="AO68:AP68"/>
+    <mergeCell ref="BA68:BA69"/>
+    <mergeCell ref="BB68:BB69"/>
+    <mergeCell ref="AW69:AW70"/>
+    <mergeCell ref="V52:X52"/>
+    <mergeCell ref="V67:W67"/>
+    <mergeCell ref="AH67:AH68"/>
+    <mergeCell ref="AI67:AI68"/>
+    <mergeCell ref="AD68:AD69"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="N66:N67"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="J67:J68"/>
+    <mergeCell ref="CI49:CI51"/>
+    <mergeCell ref="BW50:BX50"/>
+    <mergeCell ref="BW38:BY38"/>
+    <mergeCell ref="BW44:BW45"/>
+    <mergeCell ref="CB44:CB45"/>
+    <mergeCell ref="CD49:CD51"/>
+    <mergeCell ref="CH49:CH51"/>
+    <mergeCell ref="BP49:BP51"/>
+    <mergeCell ref="BD50:BE50"/>
+    <mergeCell ref="BD38:BF38"/>
+    <mergeCell ref="BD44:BD45"/>
+    <mergeCell ref="BI44:BI45"/>
+    <mergeCell ref="BK49:BK51"/>
+    <mergeCell ref="BO49:BO51"/>
     <mergeCell ref="BR24:BS24"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B36:C36"/>
@@ -16587,40 +16709,27 @@
     <mergeCell ref="BM36:BN36"/>
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="BP49:BP51"/>
-    <mergeCell ref="BD50:BE50"/>
-    <mergeCell ref="BD38:BF38"/>
-    <mergeCell ref="BD44:BD45"/>
-    <mergeCell ref="BI44:BI45"/>
-    <mergeCell ref="BK49:BK51"/>
-    <mergeCell ref="BO49:BO51"/>
-    <mergeCell ref="CI49:CI51"/>
-    <mergeCell ref="BW50:BX50"/>
-    <mergeCell ref="BW38:BY38"/>
-    <mergeCell ref="BW44:BW45"/>
-    <mergeCell ref="CB44:CB45"/>
-    <mergeCell ref="CD49:CD51"/>
-    <mergeCell ref="CH49:CH51"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="N66:N67"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="V52:X52"/>
-    <mergeCell ref="V67:W67"/>
-    <mergeCell ref="AH67:AH68"/>
-    <mergeCell ref="AI67:AI68"/>
-    <mergeCell ref="AD68:AD69"/>
-    <mergeCell ref="AO53:AQ53"/>
-    <mergeCell ref="AO68:AP68"/>
-    <mergeCell ref="BA68:BA69"/>
-    <mergeCell ref="BB68:BB69"/>
-    <mergeCell ref="AW69:AW70"/>
-    <mergeCell ref="BJ53:BL53"/>
-    <mergeCell ref="BJ68:BK68"/>
-    <mergeCell ref="BV68:BV69"/>
-    <mergeCell ref="BW68:BW69"/>
-    <mergeCell ref="BR69:BR70"/>
+    <mergeCell ref="AQ49:AQ51"/>
+    <mergeCell ref="AU49:AU51"/>
+    <mergeCell ref="AV49:AV51"/>
+    <mergeCell ref="AJ50:AK50"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="S44:S45"/>
+    <mergeCell ref="T44:T45"/>
+    <mergeCell ref="W44:W45"/>
+    <mergeCell ref="AJ38:AL38"/>
+    <mergeCell ref="AJ44:AJ45"/>
+    <mergeCell ref="AK44:AK45"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="AO44:AO45"/>
+    <mergeCell ref="CC53:CE53"/>
+    <mergeCell ref="CC68:CD68"/>
+    <mergeCell ref="CO68:CO69"/>
+    <mergeCell ref="CP68:CP69"/>
+    <mergeCell ref="CK69:CK70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.1.4 _8:10PM
Boat Enabled -
InCapacity - [17,8,Cnt] , NodeW - [-3] , BirdW - [7] , FuelW_ANoon - [22] , OnHost - [8+1]
VillageW=[1] , [X-MarketShieldMatrix-X] = [5,24,10,9] = [Lx -2 , Bx - 4 ]
Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.9.xlsx
+++ b/Usage_S_1.0.9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F9390A-A59F-4C52-8EC4-966551D996CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B317D8D-21C6-40B7-9E4B-4CE68BEC6889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2436" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2444" uniqueCount="291">
   <si>
     <t>UnSettled</t>
   </si>
@@ -875,9 +875,6 @@
     <t>2BR+1PF+1PF</t>
   </si>
   <si>
-    <t>Fish-2</t>
-  </si>
-  <si>
     <t>1Bird+1Star+1dhauli</t>
   </si>
   <si>
@@ -891,6 +888,27 @@
   </si>
   <si>
     <t>1IS+1BR+ToLet2+1ckl+2pp</t>
+  </si>
+  <si>
+    <t>X-lx(2) - X</t>
+  </si>
+  <si>
+    <t>X-Local_BX(4)- X</t>
+  </si>
+  <si>
+    <t>X-dhauli-X</t>
+  </si>
+  <si>
+    <t>Fish-4</t>
+  </si>
+  <si>
+    <t>Cow-2</t>
+  </si>
+  <si>
+    <t>X-Cow2 -X</t>
+  </si>
+  <si>
+    <t>X-Cow2-X</t>
   </si>
 </sst>
 </file>
@@ -1834,7 +1852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="328">
+  <cellXfs count="326">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2474,6 +2492,9 @@
     <xf numFmtId="0" fontId="24" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2487,9 +2508,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2534,6 +2552,51 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2579,49 +2642,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2635,32 +2668,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2950,8 +2966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI16" sqref="AI16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2978,6 +2994,7 @@
     <col min="21" max="21" width="11.140625" style="24" customWidth="1"/>
     <col min="22" max="22" width="5.140625" customWidth="1"/>
     <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="3.85546875" customWidth="1"/>
@@ -3004,12 +3021,12 @@
       <c r="AD1" s="249" t="s">
         <v>224</v>
       </c>
-      <c r="AF1" s="263" t="s">
+      <c r="AF1" s="264" t="s">
         <v>241</v>
       </c>
-      <c r="AG1" s="264"/>
-      <c r="AH1" s="264"/>
-      <c r="AI1" s="265"/>
+      <c r="AG1" s="265"/>
+      <c r="AH1" s="265"/>
+      <c r="AI1" s="266"/>
     </row>
     <row r="2" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -3073,6 +3090,7 @@
         <f ca="1">TODAY()</f>
         <v>45293</v>
       </c>
+      <c r="X2" s="8"/>
       <c r="Y2" s="9" t="s">
         <v>243</v>
       </c>
@@ -3139,7 +3157,9 @@
       <c r="E4" s="244">
         <v>5</v>
       </c>
-      <c r="F4" s="205"/>
+      <c r="F4" s="205">
+        <v>10</v>
+      </c>
       <c r="G4" s="247"/>
       <c r="H4" s="9" t="s">
         <v>199</v>
@@ -3175,7 +3195,10 @@
         <v>130</v>
       </c>
       <c r="S4" s="154">
-        <v>0.52083333333333337</v>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="T4" s="105">
+        <v>2</v>
       </c>
       <c r="U4" s="245">
         <v>45294</v>
@@ -3203,7 +3226,9 @@
       <c r="E5" s="218">
         <v>10</v>
       </c>
-      <c r="F5" s="206"/>
+      <c r="F5" s="206">
+        <v>20</v>
+      </c>
       <c r="G5" s="127"/>
       <c r="H5" s="9" t="s">
         <v>1</v>
@@ -3233,13 +3258,16 @@
         <v>86</v>
       </c>
       <c r="Q5" s="154">
-        <v>0.73263888888888884</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="S5" s="154">
-        <v>0.88611111111111107</v>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="T5" s="238">
+        <v>1</v>
       </c>
       <c r="U5" s="245">
-        <v>45293</v>
+        <v>45294</v>
       </c>
       <c r="Y5" s="25" t="s">
         <v>244</v>
@@ -3258,10 +3286,10 @@
     </row>
     <row r="6" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
-        <v>3682</v>
+        <v>3782</v>
       </c>
       <c r="C6">
-        <v>5393</v>
+        <v>5251</v>
       </c>
       <c r="E6" s="218"/>
       <c r="F6" s="207"/>
@@ -3302,6 +3330,9 @@
       </c>
       <c r="U6" s="245">
         <v>45293</v>
+      </c>
+      <c r="X6" s="25" t="s">
+        <v>282</v>
       </c>
       <c r="Y6" s="25" t="s">
         <v>244</v>
@@ -3455,7 +3486,7 @@
       </c>
       <c r="B9" s="8">
         <f>7000+B6+B5-C2</f>
-        <v>10682</v>
+        <v>10782</v>
       </c>
       <c r="E9" s="163">
         <v>14</v>
@@ -3554,6 +3585,7 @@
       <c r="U10" s="245">
         <v>45294</v>
       </c>
+      <c r="X10" s="216"/>
       <c r="Y10" s="25" t="s">
         <v>256</v>
       </c>
@@ -3586,7 +3618,9 @@
       <c r="E11" s="221">
         <v>10</v>
       </c>
-      <c r="F11" s="242"/>
+      <c r="F11" s="242">
+        <v>10</v>
+      </c>
       <c r="G11" s="37"/>
       <c r="H11" s="9" t="s">
         <v>102</v>
@@ -3598,7 +3632,7 @@
         <v>116</v>
       </c>
       <c r="K11" s="169" t="s">
-        <v>258</v>
+        <v>285</v>
       </c>
       <c r="L11" s="83" t="s">
         <v>124</v>
@@ -3616,13 +3650,13 @@
         <v>161</v>
       </c>
       <c r="Q11" s="154">
-        <v>0.73263888888888884</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>126</v>
       </c>
       <c r="S11" s="154">
-        <v>0.52083333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="T11" s="262">
         <v>3</v>
@@ -3651,7 +3685,9 @@
     </row>
     <row r="12" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E12" s="165"/>
-      <c r="F12" s="205"/>
+      <c r="F12" s="205">
+        <v>60</v>
+      </c>
       <c r="G12" s="164"/>
       <c r="H12" s="28" t="s">
         <v>128</v>
@@ -3660,7 +3696,9 @@
         <v>17</v>
       </c>
       <c r="J12" s="213"/>
-      <c r="K12" s="169"/>
+      <c r="K12" s="169" t="s">
+        <v>284</v>
+      </c>
       <c r="L12" s="224" t="s">
         <v>123</v>
       </c>
@@ -3677,14 +3715,14 @@
         <v>181</v>
       </c>
       <c r="Q12" s="154">
-        <v>0.94097222222222221</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="R12" s="24"/>
       <c r="S12" s="154">
-        <v>0.94097222222222221</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="U12" s="245">
-        <v>45293</v>
+        <v>45294</v>
       </c>
       <c r="Y12" s="25" t="s">
         <v>244</v>
@@ -3713,7 +3751,7 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>10682</v>
+        <v>10782</v>
       </c>
       <c r="E13" s="36">
         <v>5</v>
@@ -3754,7 +3792,7 @@
       <c r="S13" s="154">
         <v>0.88611111111111107</v>
       </c>
-      <c r="T13" s="321">
+      <c r="T13" s="263">
         <v>1</v>
       </c>
       <c r="U13" s="245">
@@ -3816,6 +3854,9 @@
       <c r="U14" s="245">
         <v>45293</v>
       </c>
+      <c r="X14" s="25" t="s">
+        <v>286</v>
+      </c>
       <c r="Y14" s="25" t="s">
         <v>256</v>
       </c>
@@ -3898,6 +3939,9 @@
       <c r="J16" s="119"/>
       <c r="K16" s="216"/>
       <c r="L16" s="119"/>
+      <c r="X16" s="216" t="s">
+        <v>290</v>
+      </c>
       <c r="Y16" s="25" t="s">
         <v>244</v>
       </c>
@@ -3919,21 +3963,21 @@
       <c r="G17" s="189"/>
       <c r="H17" s="9">
         <f>SUM(E4:G15)</f>
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="I17" s="26"/>
       <c r="J17" s="119"/>
       <c r="K17" s="254"/>
       <c r="L17" s="255"/>
-      <c r="N17" s="326" t="s">
-        <v>280</v>
-      </c>
-      <c r="Q17" s="327" t="s">
+      <c r="N17" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q17" s="25" t="s">
         <v>274</v>
       </c>
       <c r="R17" s="268"/>
       <c r="S17" s="24" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="V17" s="261"/>
       <c r="Y17" s="25" t="s">
@@ -3969,16 +4013,17 @@
       <c r="G18" s="20"/>
       <c r="I18" s="226"/>
       <c r="J18" s="119"/>
-      <c r="K18" s="169" t="s">
-        <v>253</v>
-      </c>
+      <c r="K18" s="169"/>
       <c r="L18" s="169"/>
-      <c r="M18" s="266"/>
+      <c r="M18" s="267"/>
       <c r="N18" s="25" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q18" s="327"/>
+        <v>283</v>
+      </c>
+      <c r="Q18" s="25"/>
       <c r="R18" s="268"/>
+      <c r="X18" s="25" t="s">
+        <v>289</v>
+      </c>
       <c r="Y18" s="25" t="s">
         <v>244</v>
       </c>
@@ -3997,18 +4042,18 @@
       <c r="I19" s="226"/>
       <c r="K19" s="194"/>
       <c r="L19" s="119"/>
-      <c r="M19" s="266"/>
+      <c r="M19" s="267"/>
       <c r="N19" s="25" t="s">
         <v>278</v>
       </c>
-      <c r="O19" s="322" t="s">
+      <c r="O19" s="283" t="s">
         <v>273</v>
       </c>
-      <c r="P19" s="323"/>
-      <c r="Q19" s="325" t="s">
-        <v>281</v>
-      </c>
-      <c r="R19" s="324"/>
+      <c r="P19" s="284"/>
+      <c r="Q19" s="285" t="s">
+        <v>280</v>
+      </c>
+      <c r="R19" s="286"/>
       <c r="Y19" s="25" t="s">
         <v>244</v>
       </c>
@@ -4033,11 +4078,11 @@
       <c r="N20" s="25" t="s">
         <v>277</v>
       </c>
-      <c r="Q20" s="327" t="s">
-        <v>283</v>
+      <c r="Q20" s="25" t="s">
+        <v>282</v>
       </c>
       <c r="S20" s="24" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="Y20" s="25" t="s">
         <v>244</v>
@@ -4067,6 +4112,12 @@
       </c>
     </row>
     <row r="21" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S21" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="X21" s="25" t="s">
+        <v>282</v>
+      </c>
       <c r="Y21" s="25" t="s">
         <v>244</v>
       </c>
@@ -4093,6 +4144,9 @@
       </c>
     </row>
     <row r="22" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S22" s="24" t="s">
+        <v>281</v>
+      </c>
       <c r="Y22" s="25" t="s">
         <v>244</v>
       </c>
@@ -4171,6 +4225,9 @@
       </c>
     </row>
     <row r="25" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X25" s="25" t="s">
+        <v>274</v>
+      </c>
       <c r="Y25" s="25" t="s">
         <v>268</v>
       </c>
@@ -4217,8 +4274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K64" sqref="K64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4242,18 +4299,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="299" t="s">
+      <c r="E1" s="287" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="301"/>
+      <c r="F1" s="289"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="299" t="s">
+      <c r="H1" s="287" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="300"/>
-      <c r="J1" s="301"/>
+      <c r="I1" s="288"/>
+      <c r="J1" s="289"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -4271,7 +4328,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="302">
+      <c r="B2" s="290">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -4298,26 +4355,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="305">
+      <c r="K2" s="293">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="296">
+      <c r="L2" s="311">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="286">
+      <c r="M2" s="301">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
         <f>SUM(E2:J60)</f>
-        <v>10642</v>
+        <v>10742</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="303"/>
+      <c r="B3" s="291"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -4332,13 +4389,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="306"/>
-      <c r="L3" s="297"/>
-      <c r="M3" s="287"/>
+      <c r="K3" s="294"/>
+      <c r="L3" s="312"/>
+      <c r="M3" s="302"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="304"/>
+      <c r="B4" s="292"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -4353,9 +4410,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="306"/>
-      <c r="L4" s="297"/>
-      <c r="M4" s="287"/>
+      <c r="K4" s="294"/>
+      <c r="L4" s="312"/>
+      <c r="M4" s="302"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -4437,7 +4494,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="288">
+      <c r="B7" s="303">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -4454,22 +4511,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="290">
+      <c r="K7" s="305">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="292">
+      <c r="L7" s="307">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="294">
+      <c r="M7" s="309">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="289"/>
+      <c r="B8" s="304"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -4490,9 +4547,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="291"/>
-      <c r="L8" s="293"/>
-      <c r="M8" s="295"/>
+      <c r="K8" s="306"/>
+      <c r="L8" s="308"/>
+      <c r="M8" s="310"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -4572,7 +4629,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="288">
+      <c r="B11" s="303">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -4599,7 +4656,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="289"/>
+      <c r="B12" s="304"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -4656,7 +4713,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="288">
+      <c r="B14" s="303">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -4679,7 +4736,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="289"/>
+      <c r="B15" s="304"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -4703,7 +4760,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="302">
+      <c r="B16" s="290">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -4734,7 +4791,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="303"/>
+      <c r="B17" s="291"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -4752,7 +4809,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="302">
+      <c r="B18" s="290">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -4781,7 +4838,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="304"/>
+      <c r="B19" s="292"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -4841,7 +4898,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="307">
+      <c r="B21" s="296">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -4869,7 +4926,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="308"/>
+      <c r="B22" s="297"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -5009,7 +5066,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="298"/>
+      <c r="B27" s="295"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -5340,7 +5397,7 @@
       <c r="A40" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="298"/>
+      <c r="B40" s="295"/>
       <c r="C40" s="96"/>
       <c r="D40" s="82">
         <v>210</v>
@@ -5395,7 +5452,7 @@
       <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="298"/>
+      <c r="B42" s="295"/>
       <c r="C42" s="142"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -5515,7 +5572,7 @@
       <c r="M46" s="18"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="298"/>
+      <c r="B47" s="295"/>
       <c r="C47" s="211"/>
       <c r="D47" s="132"/>
       <c r="E47" s="132"/>
@@ -5556,7 +5613,7 @@
       <c r="M48" s="18"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="298"/>
+      <c r="B49" s="295"/>
       <c r="C49" s="142"/>
       <c r="D49" s="18">
         <v>175</v>
@@ -5582,7 +5639,7 @@
       <c r="M49" s="18"/>
     </row>
     <row r="50" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="298"/>
+      <c r="B50" s="295"/>
       <c r="C50" s="96"/>
       <c r="D50" s="82"/>
       <c r="E50" s="82"/>
@@ -5694,7 +5751,7 @@
       <c r="T53" s="49"/>
     </row>
     <row r="54" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="298"/>
+      <c r="B54" s="295"/>
       <c r="C54" s="96"/>
       <c r="D54" s="82"/>
       <c r="E54" s="82"/>
@@ -5775,7 +5832,7 @@
       <c r="M56" s="82"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B57" s="283">
+      <c r="B57" s="298">
         <v>1</v>
       </c>
       <c r="C57" s="142"/>
@@ -5795,7 +5852,7 @@
       <c r="M57" s="18"/>
     </row>
     <row r="58" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="284"/>
+      <c r="B58" s="299"/>
       <c r="C58" s="142"/>
       <c r="D58" s="18"/>
       <c r="E58" s="18">
@@ -5824,7 +5881,7 @@
       <c r="A59" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="285"/>
+      <c r="B59" s="300"/>
       <c r="C59" s="142"/>
       <c r="D59" s="18"/>
       <c r="E59" s="18">
@@ -5855,12 +5912,18 @@
       </c>
       <c r="C60" s="18"/>
       <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
+      <c r="E60" s="18">
+        <v>20</v>
+      </c>
+      <c r="F60" s="18">
+        <v>60</v>
+      </c>
       <c r="G60" s="18">
         <v>70</v>
       </c>
-      <c r="H60" s="18"/>
+      <c r="H60" s="18">
+        <v>20</v>
+      </c>
       <c r="I60" s="18">
         <v>15</v>
       </c>
@@ -5873,21 +5936,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B35:B36"/>
     <mergeCell ref="B57:B59"/>
     <mergeCell ref="B55:B56"/>
     <mergeCell ref="B37:B38"/>
@@ -5904,6 +5952,21 @@
     <mergeCell ref="B46:B47"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="B53:B54"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B35:B36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10339,7 +10402,7 @@
       <c r="AW32" s="163">
         <v>25</v>
       </c>
-      <c r="AX32" s="310">
+      <c r="AX32" s="323">
         <v>70</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -10377,7 +10440,7 @@
       <c r="BM32" s="163">
         <v>50</v>
       </c>
-      <c r="BN32" s="310">
+      <c r="BN32" s="323">
         <v>20</v>
       </c>
       <c r="BO32" s="9" t="s">
@@ -10526,7 +10589,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="163"/>
-      <c r="AX33" s="311"/>
+      <c r="AX33" s="324"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -10562,7 +10625,7 @@
       <c r="BM33" s="140">
         <v>10</v>
       </c>
-      <c r="BN33" s="311"/>
+      <c r="BN33" s="324"/>
       <c r="BO33" s="9" t="s">
         <v>71</v>
       </c>
@@ -10713,7 +10776,7 @@
         <v>148</v>
       </c>
       <c r="AW34" s="140"/>
-      <c r="AX34" s="312"/>
+      <c r="AX34" s="325"/>
       <c r="AY34" s="9" t="s">
         <v>81</v>
       </c>
@@ -10751,7 +10814,7 @@
       <c r="BM34" s="165">
         <v>70</v>
       </c>
-      <c r="BN34" s="312"/>
+      <c r="BN34" s="325"/>
       <c r="BO34" s="9" t="s">
         <v>81</v>
       </c>
@@ -12224,7 +12287,7 @@
     </row>
     <row r="44" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="163"/>
-      <c r="C44" s="310">
+      <c r="C44" s="323">
         <v>55</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -12262,10 +12325,10 @@
       <c r="P44" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S44" s="319">
+      <c r="S44" s="316">
         <v>25</v>
       </c>
-      <c r="T44" s="310">
+      <c r="T44" s="323">
         <v>55</v>
       </c>
       <c r="U44" s="9" t="s">
@@ -12274,7 +12337,7 @@
       <c r="V44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="W44" s="313" t="s">
+      <c r="W44" s="318" t="s">
         <v>105</v>
       </c>
       <c r="X44" s="83" t="s">
@@ -12303,10 +12366,10 @@
       <c r="AG44" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="AJ44" s="319">
+      <c r="AJ44" s="316">
         <v>50</v>
       </c>
-      <c r="AK44" s="310">
+      <c r="AK44" s="323">
         <v>10</v>
       </c>
       <c r="AL44" s="190"/>
@@ -12316,7 +12379,7 @@
       <c r="AN44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO44" s="313" t="s">
+      <c r="AO44" s="318" t="s">
         <v>105</v>
       </c>
       <c r="AP44" s="83" t="s">
@@ -12346,7 +12409,7 @@
         <v>168</v>
       </c>
       <c r="AZ44" s="49"/>
-      <c r="BD44" s="319">
+      <c r="BD44" s="316">
         <v>50</v>
       </c>
       <c r="BE44" s="208"/>
@@ -12357,7 +12420,7 @@
       <c r="BH44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI44" s="313" t="s">
+      <c r="BI44" s="318" t="s">
         <v>105</v>
       </c>
       <c r="BJ44" s="83" t="s">
@@ -12386,7 +12449,7 @@
       <c r="BS44" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW44" s="319">
+      <c r="BW44" s="316">
         <v>25</v>
       </c>
       <c r="BX44" s="208"/>
@@ -12397,7 +12460,7 @@
       <c r="CA44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB44" s="313" t="s">
+      <c r="CB44" s="318" t="s">
         <v>105</v>
       </c>
       <c r="CC44" s="83" t="s">
@@ -12429,7 +12492,7 @@
     </row>
     <row r="45" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="140"/>
-      <c r="C45" s="311"/>
+      <c r="C45" s="324"/>
       <c r="D45" s="9" t="s">
         <v>71</v>
       </c>
@@ -12463,15 +12526,15 @@
       <c r="P45" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S45" s="320"/>
-      <c r="T45" s="312"/>
+      <c r="S45" s="317"/>
+      <c r="T45" s="325"/>
       <c r="U45" s="9" t="s">
         <v>71</v>
       </c>
       <c r="V45" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="W45" s="314"/>
+      <c r="W45" s="319"/>
       <c r="X45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12498,8 +12561,8 @@
       <c r="AG45" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="AJ45" s="320"/>
-      <c r="AK45" s="312"/>
+      <c r="AJ45" s="317"/>
+      <c r="AK45" s="325"/>
       <c r="AL45" s="191"/>
       <c r="AM45" s="9" t="s">
         <v>71</v>
@@ -12507,7 +12570,7 @@
       <c r="AN45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO45" s="314"/>
+      <c r="AO45" s="319"/>
       <c r="AP45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12535,7 +12598,7 @@
         <v>168</v>
       </c>
       <c r="AZ45" s="49"/>
-      <c r="BD45" s="320"/>
+      <c r="BD45" s="317"/>
       <c r="BE45" s="165">
         <v>20</v>
       </c>
@@ -12546,7 +12609,7 @@
       <c r="BH45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI45" s="314"/>
+      <c r="BI45" s="319"/>
       <c r="BJ45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12573,7 +12636,7 @@
       <c r="BS45" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW45" s="320"/>
+      <c r="BW45" s="317"/>
       <c r="BX45" s="165"/>
       <c r="BY45" s="191"/>
       <c r="BZ45" s="9" t="s">
@@ -12582,7 +12645,7 @@
       <c r="CA45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB45" s="314"/>
+      <c r="CB45" s="319"/>
       <c r="CC45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12612,7 +12675,7 @@
     </row>
     <row r="46" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="165"/>
-      <c r="C46" s="312"/>
+      <c r="C46" s="325"/>
       <c r="D46" s="9" t="s">
         <v>81</v>
       </c>
@@ -13217,10 +13280,10 @@
       <c r="AN49" s="25"/>
       <c r="AO49" s="119"/>
       <c r="AP49" s="119"/>
-      <c r="AQ49" s="315"/>
+      <c r="AQ49" s="320"/>
       <c r="AS49" s="192"/>
       <c r="AT49" s="2"/>
-      <c r="AU49" s="267"/>
+      <c r="AU49" s="313"/>
       <c r="AV49" s="268"/>
       <c r="AW49" s="1"/>
       <c r="AX49" s="1"/>
@@ -13233,10 +13296,10 @@
       <c r="BH49" s="25"/>
       <c r="BI49" s="119"/>
       <c r="BJ49" s="119"/>
-      <c r="BK49" s="315"/>
+      <c r="BK49" s="320"/>
       <c r="BM49" s="192"/>
       <c r="BN49" s="2"/>
-      <c r="BO49" s="267"/>
+      <c r="BO49" s="313"/>
       <c r="BP49" s="268"/>
       <c r="BQ49" s="1"/>
       <c r="BR49" s="1"/>
@@ -13248,10 +13311,10 @@
       <c r="CA49" s="25"/>
       <c r="CB49" s="119"/>
       <c r="CC49" s="119"/>
-      <c r="CD49" s="315"/>
+      <c r="CD49" s="320"/>
       <c r="CF49" s="192"/>
       <c r="CG49" s="2"/>
-      <c r="CH49" s="267"/>
+      <c r="CH49" s="313"/>
       <c r="CI49" s="268"/>
       <c r="CJ49" s="1"/>
       <c r="CK49" s="1"/>
@@ -13272,10 +13335,10 @@
       <c r="AN50" s="25"/>
       <c r="AO50" s="119"/>
       <c r="AP50" s="119"/>
-      <c r="AQ50" s="315"/>
+      <c r="AQ50" s="320"/>
       <c r="AS50" s="192"/>
       <c r="AT50" s="2"/>
-      <c r="AU50" s="267"/>
+      <c r="AU50" s="313"/>
       <c r="AV50" s="268"/>
       <c r="AW50" s="1"/>
       <c r="AX50" s="1"/>
@@ -13293,10 +13356,10 @@
       <c r="BH50" s="25"/>
       <c r="BI50" s="119"/>
       <c r="BJ50" s="119"/>
-      <c r="BK50" s="315"/>
+      <c r="BK50" s="320"/>
       <c r="BM50" s="192"/>
       <c r="BN50" s="2"/>
-      <c r="BO50" s="267"/>
+      <c r="BO50" s="313"/>
       <c r="BP50" s="268"/>
       <c r="BQ50" s="1"/>
       <c r="BR50" s="1"/>
@@ -13313,10 +13376,10 @@
       <c r="CA50" s="25"/>
       <c r="CB50" s="119"/>
       <c r="CC50" s="119"/>
-      <c r="CD50" s="315"/>
+      <c r="CD50" s="320"/>
       <c r="CF50" s="192"/>
       <c r="CG50" s="2"/>
-      <c r="CH50" s="267"/>
+      <c r="CH50" s="313"/>
       <c r="CI50" s="268"/>
       <c r="CJ50" s="1"/>
       <c r="CK50" s="1"/>
@@ -13377,14 +13440,14 @@
       <c r="AN51" s="114"/>
       <c r="AO51" s="201"/>
       <c r="AP51" s="202"/>
-      <c r="AQ51" s="316"/>
+      <c r="AQ51" s="321"/>
       <c r="AR51" s="201"/>
       <c r="AS51" s="203"/>
       <c r="AT51" s="116" t="s">
         <v>160</v>
       </c>
-      <c r="AU51" s="317"/>
-      <c r="AV51" s="318"/>
+      <c r="AU51" s="322"/>
+      <c r="AV51" s="315"/>
       <c r="AW51" s="65"/>
       <c r="AX51" s="65"/>
       <c r="AY51" s="115"/>
@@ -13396,14 +13459,14 @@
       <c r="BH51" s="114"/>
       <c r="BI51" s="201"/>
       <c r="BJ51" s="202"/>
-      <c r="BK51" s="316"/>
+      <c r="BK51" s="321"/>
       <c r="BL51" s="201"/>
       <c r="BM51" s="203"/>
       <c r="BN51" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="BO51" s="317"/>
-      <c r="BP51" s="318"/>
+      <c r="BO51" s="322"/>
+      <c r="BP51" s="315"/>
       <c r="BQ51" s="65"/>
       <c r="BR51" s="65"/>
       <c r="BS51" s="168"/>
@@ -13414,14 +13477,14 @@
       <c r="CA51" s="114"/>
       <c r="CB51" s="201"/>
       <c r="CC51" s="202"/>
-      <c r="CD51" s="316"/>
+      <c r="CD51" s="321"/>
       <c r="CE51" s="201"/>
       <c r="CF51" s="203" t="s">
         <v>180</v>
       </c>
       <c r="CG51" s="79"/>
-      <c r="CH51" s="317"/>
-      <c r="CI51" s="318"/>
+      <c r="CH51" s="322"/>
+      <c r="CI51" s="315"/>
       <c r="CJ51" s="65"/>
       <c r="CK51" s="65"/>
       <c r="CL51" s="168"/>
@@ -16234,7 +16297,7 @@
       <c r="J66" s="117"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="267"/>
+      <c r="N66" s="313"/>
       <c r="O66" s="268"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
@@ -16346,10 +16409,10 @@
       <c r="G67" s="119"/>
       <c r="H67" s="216"/>
       <c r="I67" s="119"/>
-      <c r="J67" s="266"/>
+      <c r="J67" s="267"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="267"/>
+      <c r="N67" s="313"/>
       <c r="O67" s="268"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
@@ -16369,7 +16432,7 @@
       <c r="AC67" s="119"/>
       <c r="AD67" s="117"/>
       <c r="AG67" s="2"/>
-      <c r="AH67" s="267"/>
+      <c r="AH67" s="313"/>
       <c r="AI67" s="268"/>
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
@@ -16426,7 +16489,7 @@
       <c r="G68" s="137"/>
       <c r="H68" s="203"/>
       <c r="I68" s="137"/>
-      <c r="J68" s="309"/>
+      <c r="J68" s="314"/>
       <c r="K68" s="50"/>
       <c r="L68" s="79"/>
       <c r="M68" s="79"/>
@@ -16442,9 +16505,9 @@
       <c r="AA68" s="119"/>
       <c r="AB68" s="216"/>
       <c r="AC68" s="119"/>
-      <c r="AD68" s="266"/>
+      <c r="AD68" s="267"/>
       <c r="AG68" s="2"/>
-      <c r="AH68" s="267"/>
+      <c r="AH68" s="313"/>
       <c r="AI68" s="268"/>
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
@@ -16464,7 +16527,7 @@
       <c r="AV68" s="119"/>
       <c r="AW68" s="117"/>
       <c r="AZ68" s="2"/>
-      <c r="BA68" s="267"/>
+      <c r="BA68" s="313"/>
       <c r="BB68" s="268"/>
       <c r="BC68" s="1"/>
       <c r="BD68" s="1"/>
@@ -16484,7 +16547,7 @@
       <c r="BQ68" s="119"/>
       <c r="BR68" s="117"/>
       <c r="BU68" s="2"/>
-      <c r="BV68" s="267"/>
+      <c r="BV68" s="313"/>
       <c r="BW68" s="268"/>
       <c r="BX68" s="1"/>
       <c r="BY68" s="1"/>
@@ -16504,7 +16567,7 @@
       <c r="CJ68" s="119"/>
       <c r="CK68" s="117"/>
       <c r="CN68" s="2"/>
-      <c r="CO68" s="267"/>
+      <c r="CO68" s="313"/>
       <c r="CP68" s="268"/>
       <c r="CQ68" s="1"/>
       <c r="CR68" s="1"/>
@@ -16521,7 +16584,7 @@
       <c r="AC69" s="137" t="s">
         <v>184</v>
       </c>
-      <c r="AD69" s="309"/>
+      <c r="AD69" s="314"/>
       <c r="AE69" s="50"/>
       <c r="AF69" s="50"/>
       <c r="AG69" s="79"/>
@@ -16537,9 +16600,9 @@
       <c r="AT69" s="119"/>
       <c r="AU69" s="192"/>
       <c r="AV69" s="119"/>
-      <c r="AW69" s="266"/>
+      <c r="AW69" s="267"/>
       <c r="AZ69" s="2"/>
-      <c r="BA69" s="267"/>
+      <c r="BA69" s="313"/>
       <c r="BB69" s="268"/>
       <c r="BC69" s="1"/>
       <c r="BD69" s="1"/>
@@ -16551,9 +16614,9 @@
       <c r="BO69" s="119"/>
       <c r="BP69" s="192"/>
       <c r="BQ69" s="119"/>
-      <c r="BR69" s="266"/>
+      <c r="BR69" s="267"/>
       <c r="BU69" s="2"/>
-      <c r="BV69" s="267"/>
+      <c r="BV69" s="313"/>
       <c r="BW69" s="268"/>
       <c r="BX69" s="1"/>
       <c r="BY69" s="1"/>
@@ -16565,9 +16628,9 @@
       <c r="CH69" s="119"/>
       <c r="CI69" s="192"/>
       <c r="CJ69" s="119"/>
-      <c r="CK69" s="266"/>
+      <c r="CK69" s="267"/>
       <c r="CN69" s="2"/>
-      <c r="CO69" s="267"/>
+      <c r="CO69" s="313"/>
       <c r="CP69" s="268"/>
       <c r="CQ69" s="1"/>
       <c r="CR69" s="1"/>
@@ -16581,7 +16644,7 @@
       <c r="AT70" s="117"/>
       <c r="AU70" s="192"/>
       <c r="AV70" s="119"/>
-      <c r="AW70" s="266"/>
+      <c r="AW70" s="267"/>
       <c r="AZ70" s="2"/>
       <c r="BA70" s="152"/>
       <c r="BB70" s="1"/>
@@ -16595,7 +16658,7 @@
       <c r="BO70" s="117"/>
       <c r="BP70" s="192"/>
       <c r="BQ70" s="119"/>
-      <c r="BR70" s="266"/>
+      <c r="BR70" s="267"/>
       <c r="BU70" s="2"/>
       <c r="BV70" s="152"/>
       <c r="BW70" s="1"/>
@@ -16610,7 +16673,7 @@
       <c r="CH70" s="137"/>
       <c r="CI70" s="203"/>
       <c r="CJ70" s="201"/>
-      <c r="CK70" s="309"/>
+      <c r="CK70" s="314"/>
       <c r="CL70" s="50"/>
       <c r="CM70" s="50"/>
       <c r="CN70" s="79"/>
@@ -16660,40 +16723,27 @@
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="BJ53:BL53"/>
-    <mergeCell ref="BJ68:BK68"/>
-    <mergeCell ref="BV68:BV69"/>
-    <mergeCell ref="BW68:BW69"/>
-    <mergeCell ref="BR69:BR70"/>
-    <mergeCell ref="AO53:AQ53"/>
-    <mergeCell ref="AO68:AP68"/>
-    <mergeCell ref="BA68:BA69"/>
-    <mergeCell ref="BB68:BB69"/>
-    <mergeCell ref="AW69:AW70"/>
-    <mergeCell ref="V52:X52"/>
-    <mergeCell ref="V67:W67"/>
-    <mergeCell ref="AH67:AH68"/>
-    <mergeCell ref="AI67:AI68"/>
-    <mergeCell ref="AD68:AD69"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="N66:N67"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="CI49:CI51"/>
-    <mergeCell ref="BW50:BX50"/>
-    <mergeCell ref="BW38:BY38"/>
-    <mergeCell ref="BW44:BW45"/>
-    <mergeCell ref="CB44:CB45"/>
-    <mergeCell ref="CD49:CD51"/>
-    <mergeCell ref="CH49:CH51"/>
-    <mergeCell ref="BP49:BP51"/>
-    <mergeCell ref="BD50:BE50"/>
-    <mergeCell ref="BD38:BF38"/>
-    <mergeCell ref="BD44:BD45"/>
-    <mergeCell ref="BI44:BI45"/>
-    <mergeCell ref="BK49:BK51"/>
-    <mergeCell ref="BO49:BO51"/>
+    <mergeCell ref="CC53:CE53"/>
+    <mergeCell ref="CC68:CD68"/>
+    <mergeCell ref="CO68:CO69"/>
+    <mergeCell ref="CP68:CP69"/>
+    <mergeCell ref="CK69:CK70"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="AO44:AO45"/>
+    <mergeCell ref="AQ49:AQ51"/>
+    <mergeCell ref="AU49:AU51"/>
+    <mergeCell ref="AV49:AV51"/>
+    <mergeCell ref="AJ50:AK50"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="S44:S45"/>
+    <mergeCell ref="T44:T45"/>
+    <mergeCell ref="W44:W45"/>
+    <mergeCell ref="AJ38:AL38"/>
+    <mergeCell ref="AJ44:AJ45"/>
+    <mergeCell ref="AK44:AK45"/>
     <mergeCell ref="BR24:BS24"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B36:C36"/>
@@ -16709,27 +16759,40 @@
     <mergeCell ref="BM36:BN36"/>
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="AQ49:AQ51"/>
-    <mergeCell ref="AU49:AU51"/>
-    <mergeCell ref="AV49:AV51"/>
-    <mergeCell ref="AJ50:AK50"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="S44:S45"/>
-    <mergeCell ref="T44:T45"/>
-    <mergeCell ref="W44:W45"/>
-    <mergeCell ref="AJ38:AL38"/>
-    <mergeCell ref="AJ44:AJ45"/>
-    <mergeCell ref="AK44:AK45"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="AO44:AO45"/>
-    <mergeCell ref="CC53:CE53"/>
-    <mergeCell ref="CC68:CD68"/>
-    <mergeCell ref="CO68:CO69"/>
-    <mergeCell ref="CP68:CP69"/>
-    <mergeCell ref="CK69:CK70"/>
+    <mergeCell ref="BP49:BP51"/>
+    <mergeCell ref="BD50:BE50"/>
+    <mergeCell ref="BD38:BF38"/>
+    <mergeCell ref="BD44:BD45"/>
+    <mergeCell ref="BI44:BI45"/>
+    <mergeCell ref="BK49:BK51"/>
+    <mergeCell ref="BO49:BO51"/>
+    <mergeCell ref="CI49:CI51"/>
+    <mergeCell ref="BW50:BX50"/>
+    <mergeCell ref="BW38:BY38"/>
+    <mergeCell ref="BW44:BW45"/>
+    <mergeCell ref="CB44:CB45"/>
+    <mergeCell ref="CD49:CD51"/>
+    <mergeCell ref="CH49:CH51"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="N66:N67"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="J67:J68"/>
+    <mergeCell ref="V52:X52"/>
+    <mergeCell ref="V67:W67"/>
+    <mergeCell ref="AH67:AH68"/>
+    <mergeCell ref="AI67:AI68"/>
+    <mergeCell ref="AD68:AD69"/>
+    <mergeCell ref="AO53:AQ53"/>
+    <mergeCell ref="AO68:AP68"/>
+    <mergeCell ref="BA68:BA69"/>
+    <mergeCell ref="BB68:BB69"/>
+    <mergeCell ref="AW69:AW70"/>
+    <mergeCell ref="BJ53:BL53"/>
+    <mergeCell ref="BJ68:BK68"/>
+    <mergeCell ref="BV68:BV69"/>
+    <mergeCell ref="BW68:BW69"/>
+    <mergeCell ref="BR69:BR70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.1.5 _11:30PM
Boat Enabled -
InCapacity - [17,8,Cnt] , NodeW - [-3] , BirdW - [7] , FuelW_Night - [22] , OnHost - [8+1]
VillageW=[1],CityW=[1] , [X-MarketShieldMatrix-X] = [5,24,10,9] = [Lx -2 , Bx - 4 ]

Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.9.xlsx
+++ b/Usage_S_1.0.9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B317D8D-21C6-40B7-9E4B-4CE68BEC6889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097FBB39-27AA-419F-97A7-CE426D54F46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2444" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2447" uniqueCount="294">
   <si>
     <t>UnSettled</t>
   </si>
@@ -857,9 +857,6 @@
     <t>X-VillageW(Rathipur)  - X</t>
   </si>
   <si>
-    <t>X-FuelW(22)_PM  - X</t>
-  </si>
-  <si>
     <t>X-FishMP(1)-X</t>
   </si>
   <si>
@@ -909,6 +906,18 @@
   </si>
   <si>
     <t>X-Cow2-X</t>
+  </si>
+  <si>
+    <t>X-FuelW(22)_Night - X</t>
+  </si>
+  <si>
+    <t>X-CityW(Mundia Sahi)  - X</t>
+  </si>
+  <si>
+    <t>X-FuelW(22)_ANoon  - X</t>
+  </si>
+  <si>
+    <t>X-FuelW(22)_Night  - X</t>
   </si>
 </sst>
 </file>
@@ -1852,7 +1861,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="326">
+  <cellXfs count="333">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2552,16 +2561,52 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2588,73 +2633,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2668,14 +2665,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2966,8 +2990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI16" sqref="AI16"/>
+    <sheetView tabSelected="1" topLeftCell="N2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG6" sqref="AG6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3229,7 +3253,9 @@
       <c r="F5" s="206">
         <v>20</v>
       </c>
-      <c r="G5" s="127"/>
+      <c r="G5" s="127">
+        <v>30</v>
+      </c>
       <c r="H5" s="9" t="s">
         <v>1</v>
       </c>
@@ -3258,7 +3284,7 @@
         <v>86</v>
       </c>
       <c r="Q5" s="154">
-        <v>0.83333333333333337</v>
+        <v>0.98263888888888884</v>
       </c>
       <c r="S5" s="154">
         <v>0.83333333333333337</v>
@@ -3286,14 +3312,16 @@
     </row>
     <row r="6" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
-        <v>3782</v>
+        <v>4057</v>
       </c>
       <c r="C6">
-        <v>5251</v>
+        <v>4511</v>
       </c>
       <c r="E6" s="218"/>
       <c r="F6" s="207"/>
-      <c r="G6" s="127"/>
+      <c r="G6" s="127">
+        <v>30</v>
+      </c>
       <c r="H6" s="9" t="s">
         <v>203</v>
       </c>
@@ -3303,7 +3331,9 @@
       <c r="J6" s="213" t="s">
         <v>165</v>
       </c>
-      <c r="K6" s="169"/>
+      <c r="K6" s="169" t="s">
+        <v>291</v>
+      </c>
       <c r="L6" s="83" t="s">
         <v>123</v>
       </c>
@@ -3320,7 +3350,7 @@
         <v>69</v>
       </c>
       <c r="Q6" s="154">
-        <v>0.88611111111111107</v>
+        <v>0.98263888888888884</v>
       </c>
       <c r="S6" s="154">
         <v>0.88611111111111107</v>
@@ -3329,10 +3359,10 @@
         <v>1</v>
       </c>
       <c r="U6" s="245">
-        <v>45293</v>
+        <v>45294</v>
       </c>
       <c r="X6" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Y6" s="25" t="s">
         <v>244</v>
@@ -3356,11 +3386,16 @@
       <c r="B7" s="29">
         <v>0</v>
       </c>
+      <c r="C7">
+        <v>365</v>
+      </c>
       <c r="E7" s="165">
         <v>10</v>
       </c>
       <c r="F7" s="242"/>
-      <c r="G7" s="177"/>
+      <c r="G7" s="177">
+        <v>30</v>
+      </c>
       <c r="H7" s="9" t="s">
         <v>188</v>
       </c>
@@ -3371,7 +3406,7 @@
         <v>105</v>
       </c>
       <c r="K7" s="169" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L7" s="83" t="s">
         <v>139</v>
@@ -3389,7 +3424,7 @@
         <v>95</v>
       </c>
       <c r="Q7" s="154">
-        <v>0.73263888888888884</v>
+        <v>0.98263888888888884</v>
       </c>
       <c r="S7" s="154">
         <v>0.73263888888888884</v>
@@ -3418,7 +3453,9 @@
         <v>25</v>
       </c>
       <c r="F8" s="242"/>
-      <c r="G8" s="190"/>
+      <c r="G8" s="190">
+        <v>50</v>
+      </c>
       <c r="H8" s="9" t="s">
         <v>72</v>
       </c>
@@ -3445,13 +3482,13 @@
         <v>65</v>
       </c>
       <c r="Q8" s="154">
-        <v>0.73263888888888884</v>
+        <v>0.98263888888888884</v>
       </c>
       <c r="S8" s="154">
-        <v>0.52083333333333337</v>
+        <v>0.98263888888888884</v>
       </c>
       <c r="U8" s="245">
-        <v>45294</v>
+        <v>45295</v>
       </c>
       <c r="Y8" s="25" t="s">
         <v>244</v>
@@ -3486,7 +3523,7 @@
       </c>
       <c r="B9" s="8">
         <f>7000+B6+B5-C2</f>
-        <v>10782</v>
+        <v>11057</v>
       </c>
       <c r="E9" s="163">
         <v>14</v>
@@ -3502,7 +3539,9 @@
       <c r="J9" s="213" t="s">
         <v>165</v>
       </c>
-      <c r="K9" s="169"/>
+      <c r="K9" s="169" t="s">
+        <v>290</v>
+      </c>
       <c r="L9" s="223" t="s">
         <v>163</v>
       </c>
@@ -3525,7 +3564,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="U9" s="245">
-        <v>45293</v>
+        <v>45294</v>
       </c>
       <c r="Y9" s="25" t="s">
         <v>257</v>
@@ -3550,7 +3589,9 @@
         <v>70</v>
       </c>
       <c r="F10" s="206"/>
-      <c r="G10" s="177"/>
+      <c r="G10" s="177">
+        <v>100</v>
+      </c>
       <c r="H10" s="9" t="s">
         <v>81</v>
       </c>
@@ -3559,7 +3600,7 @@
       </c>
       <c r="J10" s="213"/>
       <c r="K10" s="169" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L10" s="83" t="s">
         <v>143</v>
@@ -3577,13 +3618,13 @@
         <v>66</v>
       </c>
       <c r="Q10" s="154">
-        <v>0.73263888888888884</v>
+        <v>0.98263888888888884</v>
       </c>
       <c r="S10" s="154">
         <v>0.52083333333333337</v>
       </c>
       <c r="U10" s="245">
-        <v>45294</v>
+        <v>45295</v>
       </c>
       <c r="X10" s="216"/>
       <c r="Y10" s="25" t="s">
@@ -3632,7 +3673,7 @@
         <v>116</v>
       </c>
       <c r="K11" s="169" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L11" s="83" t="s">
         <v>124</v>
@@ -3697,7 +3738,7 @@
       </c>
       <c r="J12" s="213"/>
       <c r="K12" s="169" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L12" s="224" t="s">
         <v>123</v>
@@ -3751,13 +3792,15 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>10782</v>
+        <v>11057</v>
       </c>
       <c r="E13" s="36">
         <v>5</v>
       </c>
       <c r="F13" s="206"/>
-      <c r="G13" s="246"/>
+      <c r="G13" s="246">
+        <v>35</v>
+      </c>
       <c r="H13" s="9" t="s">
         <v>189</v>
       </c>
@@ -3768,7 +3811,7 @@
         <v>186</v>
       </c>
       <c r="K13" s="194" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L13" s="183" t="s">
         <v>155</v>
@@ -3786,7 +3829,7 @@
         <v>90</v>
       </c>
       <c r="Q13" s="154">
-        <v>0.73263888888888884</v>
+        <v>0.98263888888888884</v>
       </c>
       <c r="R13"/>
       <c r="S13" s="154">
@@ -3796,7 +3839,7 @@
         <v>1</v>
       </c>
       <c r="U13" s="245">
-        <v>45293</v>
+        <v>45294</v>
       </c>
       <c r="Y13" s="25" t="s">
         <v>244</v>
@@ -3852,10 +3895,10 @@
         <v>0.94097222222222221</v>
       </c>
       <c r="U14" s="245">
-        <v>45293</v>
+        <v>45294</v>
       </c>
       <c r="X14" s="25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Y14" s="25" t="s">
         <v>256</v>
@@ -3940,7 +3983,7 @@
       <c r="K16" s="216"/>
       <c r="L16" s="119"/>
       <c r="X16" s="216" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Y16" s="25" t="s">
         <v>244</v>
@@ -3963,21 +4006,23 @@
       <c r="G17" s="189"/>
       <c r="H17" s="9">
         <f>SUM(E4:G15)</f>
-        <v>250</v>
+        <v>525</v>
       </c>
       <c r="I17" s="26"/>
-      <c r="J17" s="119"/>
+      <c r="J17" s="322"/>
       <c r="K17" s="254"/>
       <c r="L17" s="255"/>
-      <c r="N17" s="28" t="s">
-        <v>279</v>
-      </c>
-      <c r="Q17" s="25" t="s">
-        <v>274</v>
-      </c>
-      <c r="R17" s="268"/>
-      <c r="S17" s="24" t="s">
-        <v>287</v>
+      <c r="N17" s="327" t="s">
+        <v>278</v>
+      </c>
+      <c r="O17" s="18"/>
+      <c r="P17" s="328"/>
+      <c r="Q17" s="159" t="s">
+        <v>273</v>
+      </c>
+      <c r="R17" s="297"/>
+      <c r="S17" s="329" t="s">
+        <v>286</v>
       </c>
       <c r="V17" s="261"/>
       <c r="Y17" s="25" t="s">
@@ -4012,17 +4057,20 @@
       <c r="F18" s="24"/>
       <c r="G18" s="20"/>
       <c r="I18" s="226"/>
-      <c r="J18" s="119"/>
+      <c r="J18" s="322"/>
       <c r="K18" s="169"/>
       <c r="L18" s="169"/>
       <c r="M18" s="267"/>
-      <c r="N18" s="25" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="268"/>
+      <c r="N18" s="159" t="s">
+        <v>282</v>
+      </c>
+      <c r="O18" s="18"/>
+      <c r="P18" s="328"/>
+      <c r="Q18" s="159"/>
+      <c r="R18" s="297"/>
+      <c r="S18" s="17"/>
       <c r="X18" s="25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Y18" s="25" t="s">
         <v>244</v>
@@ -4043,17 +4091,18 @@
       <c r="K19" s="194"/>
       <c r="L19" s="119"/>
       <c r="M19" s="267"/>
-      <c r="N19" s="25" t="s">
-        <v>278</v>
-      </c>
-      <c r="O19" s="283" t="s">
-        <v>273</v>
-      </c>
-      <c r="P19" s="284"/>
-      <c r="Q19" s="285" t="s">
-        <v>280</v>
-      </c>
-      <c r="R19" s="286"/>
+      <c r="N19" s="159" t="s">
+        <v>277</v>
+      </c>
+      <c r="O19" s="330" t="s">
+        <v>292</v>
+      </c>
+      <c r="P19" s="330"/>
+      <c r="Q19" s="331" t="s">
+        <v>279</v>
+      </c>
+      <c r="R19" s="331"/>
+      <c r="S19" s="17"/>
       <c r="Y19" s="25" t="s">
         <v>244</v>
       </c>
@@ -4072,17 +4121,22 @@
       </c>
     </row>
     <row r="20" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="326"/>
+      <c r="B20" s="326"/>
       <c r="I20" s="227"/>
       <c r="K20" s="194"/>
       <c r="L20" s="119"/>
-      <c r="N20" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q20" s="25" t="s">
-        <v>282</v>
-      </c>
-      <c r="S20" s="24" t="s">
-        <v>288</v>
+      <c r="N20" s="159" t="s">
+        <v>276</v>
+      </c>
+      <c r="O20" s="18"/>
+      <c r="P20" s="328"/>
+      <c r="Q20" s="159" t="s">
+        <v>281</v>
+      </c>
+      <c r="R20" s="17"/>
+      <c r="S20" s="329" t="s">
+        <v>287</v>
       </c>
       <c r="Y20" s="25" t="s">
         <v>244</v>
@@ -4112,11 +4166,18 @@
       </c>
     </row>
     <row r="21" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S21" s="24" t="s">
-        <v>288</v>
+      <c r="N21" s="18"/>
+      <c r="O21" s="330" t="s">
+        <v>293</v>
+      </c>
+      <c r="P21" s="330"/>
+      <c r="Q21" s="332"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="329" t="s">
+        <v>287</v>
       </c>
       <c r="X21" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Y21" s="25" t="s">
         <v>244</v>
@@ -4145,7 +4206,7 @@
     </row>
     <row r="22" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="S22" s="24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Y22" s="25" t="s">
         <v>244</v>
@@ -4226,7 +4287,7 @@
     </row>
     <row r="25" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="X25" s="25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Y25" s="25" t="s">
         <v>268</v>
@@ -4252,7 +4313,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="AF1:AI1"/>
     <mergeCell ref="M18:M19"/>
     <mergeCell ref="R17:R18"/>
@@ -4264,6 +4325,7 @@
     <mergeCell ref="AE3:AE25"/>
     <mergeCell ref="O19:P19"/>
     <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="O21:P21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4272,10 +4334,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:T60"/>
+  <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K64" sqref="K64"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4299,18 +4361,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="287" t="s">
+      <c r="E1" s="299" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="289"/>
+      <c r="F1" s="301"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="287" t="s">
+      <c r="H1" s="299" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="288"/>
-      <c r="J1" s="289"/>
+      <c r="I1" s="300"/>
+      <c r="J1" s="301"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -4328,7 +4390,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="290">
+      <c r="B2" s="302">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -4355,26 +4417,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="293">
+      <c r="K2" s="305">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="311">
+      <c r="L2" s="296">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="301">
+      <c r="M2" s="286">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J60)</f>
-        <v>10742</v>
+        <f>SUM(E2:J62)</f>
+        <v>11017</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="291"/>
+      <c r="B3" s="303"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -4389,13 +4451,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="294"/>
-      <c r="L3" s="312"/>
-      <c r="M3" s="302"/>
+      <c r="K3" s="306"/>
+      <c r="L3" s="297"/>
+      <c r="M3" s="287"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="292"/>
+      <c r="B4" s="304"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -4410,9 +4472,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="294"/>
-      <c r="L4" s="312"/>
-      <c r="M4" s="302"/>
+      <c r="K4" s="306"/>
+      <c r="L4" s="297"/>
+      <c r="M4" s="287"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -4494,7 +4556,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="303">
+      <c r="B7" s="288">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -4511,22 +4573,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="305">
+      <c r="K7" s="290">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="307">
+      <c r="L7" s="292">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="309">
+      <c r="M7" s="294">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="304"/>
+      <c r="B8" s="289"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -4547,9 +4609,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="306"/>
-      <c r="L8" s="308"/>
-      <c r="M8" s="310"/>
+      <c r="K8" s="291"/>
+      <c r="L8" s="293"/>
+      <c r="M8" s="295"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -4629,7 +4691,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="303">
+      <c r="B11" s="288">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -4656,7 +4718,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="304"/>
+      <c r="B12" s="289"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -4713,7 +4775,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="303">
+      <c r="B14" s="288">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -4736,7 +4798,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="304"/>
+      <c r="B15" s="289"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -4760,7 +4822,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="290">
+      <c r="B16" s="302">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -4791,7 +4853,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="291"/>
+      <c r="B17" s="303"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -4809,7 +4871,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="290">
+      <c r="B18" s="302">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -4838,7 +4900,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="292"/>
+      <c r="B19" s="304"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -4898,7 +4960,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="296">
+      <c r="B21" s="307">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -4926,7 +4988,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="297"/>
+      <c r="B22" s="308"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -5066,7 +5128,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="295"/>
+      <c r="B27" s="298"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -5397,7 +5459,7 @@
       <c r="A40" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="295"/>
+      <c r="B40" s="298"/>
       <c r="C40" s="96"/>
       <c r="D40" s="82">
         <v>210</v>
@@ -5452,7 +5514,7 @@
       <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="295"/>
+      <c r="B42" s="298"/>
       <c r="C42" s="142"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -5572,7 +5634,7 @@
       <c r="M46" s="18"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="295"/>
+      <c r="B47" s="298"/>
       <c r="C47" s="211"/>
       <c r="D47" s="132"/>
       <c r="E47" s="132"/>
@@ -5613,7 +5675,7 @@
       <c r="M48" s="18"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="295"/>
+      <c r="B49" s="298"/>
       <c r="C49" s="142"/>
       <c r="D49" s="18">
         <v>175</v>
@@ -5639,7 +5701,7 @@
       <c r="M49" s="18"/>
     </row>
     <row r="50" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="295"/>
+      <c r="B50" s="298"/>
       <c r="C50" s="96"/>
       <c r="D50" s="82"/>
       <c r="E50" s="82"/>
@@ -5751,7 +5813,7 @@
       <c r="T53" s="49"/>
     </row>
     <row r="54" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="295"/>
+      <c r="B54" s="298"/>
       <c r="C54" s="96"/>
       <c r="D54" s="82"/>
       <c r="E54" s="82"/>
@@ -5832,7 +5894,7 @@
       <c r="M56" s="82"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B57" s="298">
+      <c r="B57" s="283">
         <v>1</v>
       </c>
       <c r="C57" s="142"/>
@@ -5852,7 +5914,7 @@
       <c r="M57" s="18"/>
     </row>
     <row r="58" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="299"/>
+      <c r="B58" s="284"/>
       <c r="C58" s="142"/>
       <c r="D58" s="18"/>
       <c r="E58" s="18">
@@ -5881,7 +5943,7 @@
       <c r="A59" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="300"/>
+      <c r="B59" s="285"/>
       <c r="C59" s="142"/>
       <c r="D59" s="18"/>
       <c r="E59" s="18">
@@ -5906,15 +5968,13 @@
       <c r="L59" s="18"/>
       <c r="M59" s="18"/>
     </row>
-    <row r="60" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="130">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B60" s="271">
         <v>2</v>
       </c>
-      <c r="C60" s="18"/>
+      <c r="C60" s="142"/>
       <c r="D60" s="18"/>
-      <c r="E60" s="18">
-        <v>20</v>
-      </c>
+      <c r="E60" s="18"/>
       <c r="F60" s="18">
         <v>60</v>
       </c>
@@ -5934,8 +5994,68 @@
       <c r="L60" s="18"/>
       <c r="M60" s="18"/>
     </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B61" s="323"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18">
+        <v>240</v>
+      </c>
+      <c r="E61" s="18"/>
+      <c r="F61" s="325">
+        <v>50</v>
+      </c>
+      <c r="G61" s="325">
+        <v>100</v>
+      </c>
+      <c r="H61" s="325">
+        <v>30</v>
+      </c>
+      <c r="I61" s="325">
+        <v>30</v>
+      </c>
+      <c r="J61" s="325">
+        <v>30</v>
+      </c>
+      <c r="K61" s="18"/>
+      <c r="L61" s="18"/>
+      <c r="M61" s="18"/>
+    </row>
+    <row r="62" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="324"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+      <c r="I62" s="325">
+        <v>35</v>
+      </c>
+      <c r="J62" s="325">
+        <v>20</v>
+      </c>
+      <c r="K62" s="18"/>
+      <c r="L62" s="18"/>
+      <c r="M62" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="32">
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B35:B36"/>
     <mergeCell ref="B57:B59"/>
     <mergeCell ref="B55:B56"/>
     <mergeCell ref="B37:B38"/>
@@ -5952,21 +6072,6 @@
     <mergeCell ref="B46:B47"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="B53:B54"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B35:B36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10402,7 +10507,7 @@
       <c r="AW32" s="163">
         <v>25</v>
       </c>
-      <c r="AX32" s="323">
+      <c r="AX32" s="311">
         <v>70</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -10440,7 +10545,7 @@
       <c r="BM32" s="163">
         <v>50</v>
       </c>
-      <c r="BN32" s="323">
+      <c r="BN32" s="311">
         <v>20</v>
       </c>
       <c r="BO32" s="9" t="s">
@@ -10589,7 +10694,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="163"/>
-      <c r="AX33" s="324"/>
+      <c r="AX33" s="312"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -10625,7 +10730,7 @@
       <c r="BM33" s="140">
         <v>10</v>
       </c>
-      <c r="BN33" s="324"/>
+      <c r="BN33" s="312"/>
       <c r="BO33" s="9" t="s">
         <v>71</v>
       </c>
@@ -10776,7 +10881,7 @@
         <v>148</v>
       </c>
       <c r="AW34" s="140"/>
-      <c r="AX34" s="325"/>
+      <c r="AX34" s="313"/>
       <c r="AY34" s="9" t="s">
         <v>81</v>
       </c>
@@ -10814,7 +10919,7 @@
       <c r="BM34" s="165">
         <v>70</v>
       </c>
-      <c r="BN34" s="325"/>
+      <c r="BN34" s="313"/>
       <c r="BO34" s="9" t="s">
         <v>81</v>
       </c>
@@ -12287,7 +12392,7 @@
     </row>
     <row r="44" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="163"/>
-      <c r="C44" s="323">
+      <c r="C44" s="311">
         <v>55</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -12325,10 +12430,10 @@
       <c r="P44" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S44" s="316">
+      <c r="S44" s="320">
         <v>25</v>
       </c>
-      <c r="T44" s="323">
+      <c r="T44" s="311">
         <v>55</v>
       </c>
       <c r="U44" s="9" t="s">
@@ -12337,7 +12442,7 @@
       <c r="V44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="W44" s="318" t="s">
+      <c r="W44" s="314" t="s">
         <v>105</v>
       </c>
       <c r="X44" s="83" t="s">
@@ -12366,10 +12471,10 @@
       <c r="AG44" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="AJ44" s="316">
+      <c r="AJ44" s="320">
         <v>50</v>
       </c>
-      <c r="AK44" s="323">
+      <c r="AK44" s="311">
         <v>10</v>
       </c>
       <c r="AL44" s="190"/>
@@ -12379,7 +12484,7 @@
       <c r="AN44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO44" s="318" t="s">
+      <c r="AO44" s="314" t="s">
         <v>105</v>
       </c>
       <c r="AP44" s="83" t="s">
@@ -12409,7 +12514,7 @@
         <v>168</v>
       </c>
       <c r="AZ44" s="49"/>
-      <c r="BD44" s="316">
+      <c r="BD44" s="320">
         <v>50</v>
       </c>
       <c r="BE44" s="208"/>
@@ -12420,7 +12525,7 @@
       <c r="BH44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI44" s="318" t="s">
+      <c r="BI44" s="314" t="s">
         <v>105</v>
       </c>
       <c r="BJ44" s="83" t="s">
@@ -12449,7 +12554,7 @@
       <c r="BS44" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW44" s="316">
+      <c r="BW44" s="320">
         <v>25</v>
       </c>
       <c r="BX44" s="208"/>
@@ -12460,7 +12565,7 @@
       <c r="CA44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB44" s="318" t="s">
+      <c r="CB44" s="314" t="s">
         <v>105</v>
       </c>
       <c r="CC44" s="83" t="s">
@@ -12492,7 +12597,7 @@
     </row>
     <row r="45" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="140"/>
-      <c r="C45" s="324"/>
+      <c r="C45" s="312"/>
       <c r="D45" s="9" t="s">
         <v>71</v>
       </c>
@@ -12526,15 +12631,15 @@
       <c r="P45" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S45" s="317"/>
-      <c r="T45" s="325"/>
+      <c r="S45" s="321"/>
+      <c r="T45" s="313"/>
       <c r="U45" s="9" t="s">
         <v>71</v>
       </c>
       <c r="V45" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="W45" s="319"/>
+      <c r="W45" s="315"/>
       <c r="X45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12561,8 +12666,8 @@
       <c r="AG45" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="AJ45" s="317"/>
-      <c r="AK45" s="325"/>
+      <c r="AJ45" s="321"/>
+      <c r="AK45" s="313"/>
       <c r="AL45" s="191"/>
       <c r="AM45" s="9" t="s">
         <v>71</v>
@@ -12570,7 +12675,7 @@
       <c r="AN45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO45" s="319"/>
+      <c r="AO45" s="315"/>
       <c r="AP45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12598,7 +12703,7 @@
         <v>168</v>
       </c>
       <c r="AZ45" s="49"/>
-      <c r="BD45" s="317"/>
+      <c r="BD45" s="321"/>
       <c r="BE45" s="165">
         <v>20</v>
       </c>
@@ -12609,7 +12714,7 @@
       <c r="BH45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI45" s="319"/>
+      <c r="BI45" s="315"/>
       <c r="BJ45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12636,7 +12741,7 @@
       <c r="BS45" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW45" s="317"/>
+      <c r="BW45" s="321"/>
       <c r="BX45" s="165"/>
       <c r="BY45" s="191"/>
       <c r="BZ45" s="9" t="s">
@@ -12645,7 +12750,7 @@
       <c r="CA45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB45" s="319"/>
+      <c r="CB45" s="315"/>
       <c r="CC45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12675,7 +12780,7 @@
     </row>
     <row r="46" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="165"/>
-      <c r="C46" s="325"/>
+      <c r="C46" s="313"/>
       <c r="D46" s="9" t="s">
         <v>81</v>
       </c>
@@ -13280,10 +13385,10 @@
       <c r="AN49" s="25"/>
       <c r="AO49" s="119"/>
       <c r="AP49" s="119"/>
-      <c r="AQ49" s="320"/>
+      <c r="AQ49" s="316"/>
       <c r="AS49" s="192"/>
       <c r="AT49" s="2"/>
-      <c r="AU49" s="313"/>
+      <c r="AU49" s="309"/>
       <c r="AV49" s="268"/>
       <c r="AW49" s="1"/>
       <c r="AX49" s="1"/>
@@ -13296,10 +13401,10 @@
       <c r="BH49" s="25"/>
       <c r="BI49" s="119"/>
       <c r="BJ49" s="119"/>
-      <c r="BK49" s="320"/>
+      <c r="BK49" s="316"/>
       <c r="BM49" s="192"/>
       <c r="BN49" s="2"/>
-      <c r="BO49" s="313"/>
+      <c r="BO49" s="309"/>
       <c r="BP49" s="268"/>
       <c r="BQ49" s="1"/>
       <c r="BR49" s="1"/>
@@ -13311,10 +13416,10 @@
       <c r="CA49" s="25"/>
       <c r="CB49" s="119"/>
       <c r="CC49" s="119"/>
-      <c r="CD49" s="320"/>
+      <c r="CD49" s="316"/>
       <c r="CF49" s="192"/>
       <c r="CG49" s="2"/>
-      <c r="CH49" s="313"/>
+      <c r="CH49" s="309"/>
       <c r="CI49" s="268"/>
       <c r="CJ49" s="1"/>
       <c r="CK49" s="1"/>
@@ -13335,10 +13440,10 @@
       <c r="AN50" s="25"/>
       <c r="AO50" s="119"/>
       <c r="AP50" s="119"/>
-      <c r="AQ50" s="320"/>
+      <c r="AQ50" s="316"/>
       <c r="AS50" s="192"/>
       <c r="AT50" s="2"/>
-      <c r="AU50" s="313"/>
+      <c r="AU50" s="309"/>
       <c r="AV50" s="268"/>
       <c r="AW50" s="1"/>
       <c r="AX50" s="1"/>
@@ -13356,10 +13461,10 @@
       <c r="BH50" s="25"/>
       <c r="BI50" s="119"/>
       <c r="BJ50" s="119"/>
-      <c r="BK50" s="320"/>
+      <c r="BK50" s="316"/>
       <c r="BM50" s="192"/>
       <c r="BN50" s="2"/>
-      <c r="BO50" s="313"/>
+      <c r="BO50" s="309"/>
       <c r="BP50" s="268"/>
       <c r="BQ50" s="1"/>
       <c r="BR50" s="1"/>
@@ -13376,10 +13481,10 @@
       <c r="CA50" s="25"/>
       <c r="CB50" s="119"/>
       <c r="CC50" s="119"/>
-      <c r="CD50" s="320"/>
+      <c r="CD50" s="316"/>
       <c r="CF50" s="192"/>
       <c r="CG50" s="2"/>
-      <c r="CH50" s="313"/>
+      <c r="CH50" s="309"/>
       <c r="CI50" s="268"/>
       <c r="CJ50" s="1"/>
       <c r="CK50" s="1"/>
@@ -13440,14 +13545,14 @@
       <c r="AN51" s="114"/>
       <c r="AO51" s="201"/>
       <c r="AP51" s="202"/>
-      <c r="AQ51" s="321"/>
+      <c r="AQ51" s="317"/>
       <c r="AR51" s="201"/>
       <c r="AS51" s="203"/>
       <c r="AT51" s="116" t="s">
         <v>160</v>
       </c>
-      <c r="AU51" s="322"/>
-      <c r="AV51" s="315"/>
+      <c r="AU51" s="318"/>
+      <c r="AV51" s="319"/>
       <c r="AW51" s="65"/>
       <c r="AX51" s="65"/>
       <c r="AY51" s="115"/>
@@ -13459,14 +13564,14 @@
       <c r="BH51" s="114"/>
       <c r="BI51" s="201"/>
       <c r="BJ51" s="202"/>
-      <c r="BK51" s="321"/>
+      <c r="BK51" s="317"/>
       <c r="BL51" s="201"/>
       <c r="BM51" s="203"/>
       <c r="BN51" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="BO51" s="322"/>
-      <c r="BP51" s="315"/>
+      <c r="BO51" s="318"/>
+      <c r="BP51" s="319"/>
       <c r="BQ51" s="65"/>
       <c r="BR51" s="65"/>
       <c r="BS51" s="168"/>
@@ -13477,14 +13582,14 @@
       <c r="CA51" s="114"/>
       <c r="CB51" s="201"/>
       <c r="CC51" s="202"/>
-      <c r="CD51" s="321"/>
+      <c r="CD51" s="317"/>
       <c r="CE51" s="201"/>
       <c r="CF51" s="203" t="s">
         <v>180</v>
       </c>
       <c r="CG51" s="79"/>
-      <c r="CH51" s="322"/>
-      <c r="CI51" s="315"/>
+      <c r="CH51" s="318"/>
+      <c r="CI51" s="319"/>
       <c r="CJ51" s="65"/>
       <c r="CK51" s="65"/>
       <c r="CL51" s="168"/>
@@ -16297,7 +16402,7 @@
       <c r="J66" s="117"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="313"/>
+      <c r="N66" s="309"/>
       <c r="O66" s="268"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
@@ -16412,7 +16517,7 @@
       <c r="J67" s="267"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="313"/>
+      <c r="N67" s="309"/>
       <c r="O67" s="268"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
@@ -16432,7 +16537,7 @@
       <c r="AC67" s="119"/>
       <c r="AD67" s="117"/>
       <c r="AG67" s="2"/>
-      <c r="AH67" s="313"/>
+      <c r="AH67" s="309"/>
       <c r="AI67" s="268"/>
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
@@ -16489,7 +16594,7 @@
       <c r="G68" s="137"/>
       <c r="H68" s="203"/>
       <c r="I68" s="137"/>
-      <c r="J68" s="314"/>
+      <c r="J68" s="310"/>
       <c r="K68" s="50"/>
       <c r="L68" s="79"/>
       <c r="M68" s="79"/>
@@ -16507,7 +16612,7 @@
       <c r="AC68" s="119"/>
       <c r="AD68" s="267"/>
       <c r="AG68" s="2"/>
-      <c r="AH68" s="313"/>
+      <c r="AH68" s="309"/>
       <c r="AI68" s="268"/>
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
@@ -16527,7 +16632,7 @@
       <c r="AV68" s="119"/>
       <c r="AW68" s="117"/>
       <c r="AZ68" s="2"/>
-      <c r="BA68" s="313"/>
+      <c r="BA68" s="309"/>
       <c r="BB68" s="268"/>
       <c r="BC68" s="1"/>
       <c r="BD68" s="1"/>
@@ -16547,7 +16652,7 @@
       <c r="BQ68" s="119"/>
       <c r="BR68" s="117"/>
       <c r="BU68" s="2"/>
-      <c r="BV68" s="313"/>
+      <c r="BV68" s="309"/>
       <c r="BW68" s="268"/>
       <c r="BX68" s="1"/>
       <c r="BY68" s="1"/>
@@ -16567,7 +16672,7 @@
       <c r="CJ68" s="119"/>
       <c r="CK68" s="117"/>
       <c r="CN68" s="2"/>
-      <c r="CO68" s="313"/>
+      <c r="CO68" s="309"/>
       <c r="CP68" s="268"/>
       <c r="CQ68" s="1"/>
       <c r="CR68" s="1"/>
@@ -16584,7 +16689,7 @@
       <c r="AC69" s="137" t="s">
         <v>184</v>
       </c>
-      <c r="AD69" s="314"/>
+      <c r="AD69" s="310"/>
       <c r="AE69" s="50"/>
       <c r="AF69" s="50"/>
       <c r="AG69" s="79"/>
@@ -16602,7 +16707,7 @@
       <c r="AV69" s="119"/>
       <c r="AW69" s="267"/>
       <c r="AZ69" s="2"/>
-      <c r="BA69" s="313"/>
+      <c r="BA69" s="309"/>
       <c r="BB69" s="268"/>
       <c r="BC69" s="1"/>
       <c r="BD69" s="1"/>
@@ -16616,7 +16721,7 @@
       <c r="BQ69" s="119"/>
       <c r="BR69" s="267"/>
       <c r="BU69" s="2"/>
-      <c r="BV69" s="313"/>
+      <c r="BV69" s="309"/>
       <c r="BW69" s="268"/>
       <c r="BX69" s="1"/>
       <c r="BY69" s="1"/>
@@ -16630,7 +16735,7 @@
       <c r="CJ69" s="119"/>
       <c r="CK69" s="267"/>
       <c r="CN69" s="2"/>
-      <c r="CO69" s="313"/>
+      <c r="CO69" s="309"/>
       <c r="CP69" s="268"/>
       <c r="CQ69" s="1"/>
       <c r="CR69" s="1"/>
@@ -16673,7 +16778,7 @@
       <c r="CH70" s="137"/>
       <c r="CI70" s="203"/>
       <c r="CJ70" s="201"/>
-      <c r="CK70" s="314"/>
+      <c r="CK70" s="310"/>
       <c r="CL70" s="50"/>
       <c r="CM70" s="50"/>
       <c r="CN70" s="79"/>
@@ -16723,27 +16828,40 @@
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="CC53:CE53"/>
-    <mergeCell ref="CC68:CD68"/>
-    <mergeCell ref="CO68:CO69"/>
-    <mergeCell ref="CP68:CP69"/>
-    <mergeCell ref="CK69:CK70"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="AO44:AO45"/>
-    <mergeCell ref="AQ49:AQ51"/>
-    <mergeCell ref="AU49:AU51"/>
-    <mergeCell ref="AV49:AV51"/>
-    <mergeCell ref="AJ50:AK50"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="S44:S45"/>
-    <mergeCell ref="T44:T45"/>
-    <mergeCell ref="W44:W45"/>
-    <mergeCell ref="AJ38:AL38"/>
-    <mergeCell ref="AJ44:AJ45"/>
-    <mergeCell ref="AK44:AK45"/>
+    <mergeCell ref="BJ53:BL53"/>
+    <mergeCell ref="BJ68:BK68"/>
+    <mergeCell ref="BV68:BV69"/>
+    <mergeCell ref="BW68:BW69"/>
+    <mergeCell ref="BR69:BR70"/>
+    <mergeCell ref="AO53:AQ53"/>
+    <mergeCell ref="AO68:AP68"/>
+    <mergeCell ref="BA68:BA69"/>
+    <mergeCell ref="BB68:BB69"/>
+    <mergeCell ref="AW69:AW70"/>
+    <mergeCell ref="V52:X52"/>
+    <mergeCell ref="V67:W67"/>
+    <mergeCell ref="AH67:AH68"/>
+    <mergeCell ref="AI67:AI68"/>
+    <mergeCell ref="AD68:AD69"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="N66:N67"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="J67:J68"/>
+    <mergeCell ref="CI49:CI51"/>
+    <mergeCell ref="BW50:BX50"/>
+    <mergeCell ref="BW38:BY38"/>
+    <mergeCell ref="BW44:BW45"/>
+    <mergeCell ref="CB44:CB45"/>
+    <mergeCell ref="CD49:CD51"/>
+    <mergeCell ref="CH49:CH51"/>
+    <mergeCell ref="BP49:BP51"/>
+    <mergeCell ref="BD50:BE50"/>
+    <mergeCell ref="BD38:BF38"/>
+    <mergeCell ref="BD44:BD45"/>
+    <mergeCell ref="BI44:BI45"/>
+    <mergeCell ref="BK49:BK51"/>
+    <mergeCell ref="BO49:BO51"/>
     <mergeCell ref="BR24:BS24"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B36:C36"/>
@@ -16759,40 +16877,27 @@
     <mergeCell ref="BM36:BN36"/>
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="BP49:BP51"/>
-    <mergeCell ref="BD50:BE50"/>
-    <mergeCell ref="BD38:BF38"/>
-    <mergeCell ref="BD44:BD45"/>
-    <mergeCell ref="BI44:BI45"/>
-    <mergeCell ref="BK49:BK51"/>
-    <mergeCell ref="BO49:BO51"/>
-    <mergeCell ref="CI49:CI51"/>
-    <mergeCell ref="BW50:BX50"/>
-    <mergeCell ref="BW38:BY38"/>
-    <mergeCell ref="BW44:BW45"/>
-    <mergeCell ref="CB44:CB45"/>
-    <mergeCell ref="CD49:CD51"/>
-    <mergeCell ref="CH49:CH51"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="N66:N67"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="V52:X52"/>
-    <mergeCell ref="V67:W67"/>
-    <mergeCell ref="AH67:AH68"/>
-    <mergeCell ref="AI67:AI68"/>
-    <mergeCell ref="AD68:AD69"/>
-    <mergeCell ref="AO53:AQ53"/>
-    <mergeCell ref="AO68:AP68"/>
-    <mergeCell ref="BA68:BA69"/>
-    <mergeCell ref="BB68:BB69"/>
-    <mergeCell ref="AW69:AW70"/>
-    <mergeCell ref="BJ53:BL53"/>
-    <mergeCell ref="BJ68:BK68"/>
-    <mergeCell ref="BV68:BV69"/>
-    <mergeCell ref="BW68:BW69"/>
-    <mergeCell ref="BR69:BR70"/>
+    <mergeCell ref="AQ49:AQ51"/>
+    <mergeCell ref="AU49:AU51"/>
+    <mergeCell ref="AV49:AV51"/>
+    <mergeCell ref="AJ50:AK50"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="S44:S45"/>
+    <mergeCell ref="T44:T45"/>
+    <mergeCell ref="W44:W45"/>
+    <mergeCell ref="AJ38:AL38"/>
+    <mergeCell ref="AJ44:AJ45"/>
+    <mergeCell ref="AK44:AK45"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="AO44:AO45"/>
+    <mergeCell ref="CC53:CE53"/>
+    <mergeCell ref="CC68:CD68"/>
+    <mergeCell ref="CO68:CO69"/>
+    <mergeCell ref="CP68:CP69"/>
+    <mergeCell ref="CK69:CK70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>